<commit_message>
edit to progression sheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179016" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="111">
   <si>
     <t>Act or Con</t>
   </si>
@@ -176,7 +177,7 @@
     <t>The hot plate</t>
   </si>
   <si>
-    <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
+    <t>[$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer]</t>
   </si>
   <si>
     <t>Chain Rule</t>
@@ -348,6 +349,15 @@
   </si>
   <si>
     <t>Chain Rules</t>
+  </si>
+  <si>
+    <t>$\frac{\partial f}{\partial x}$</t>
+  </si>
+  <si>
+    <t>Contour Maps</t>
+  </si>
+  <si>
+    <t>Inclinometer</t>
   </si>
 </sst>
 </file>
@@ -933,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G61" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="K69" sqref="K69:K84"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1796,7 +1806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="48">
+    <row r="32" spans="1:11" ht="15.75">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1825,7 +1835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="96">
+    <row r="33" spans="1:11" ht="63">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3188,4 +3198,37 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EFD8F-45BF-44EB-A2B4-FA9451BFAEEC}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="47.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="31.5">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="31.5">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create function to clean up views of representations
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>

</xml_diff>

<commit_message>
various improvments to the visualization
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="111">
   <si>
     <t>Act or Con</t>
   </si>
@@ -315,7 +315,7 @@
     <t>Total differentials are linear</t>
   </si>
   <si>
-    <t>Differntials are small chunks</t>
+    <t>Differentials are small chunks</t>
   </si>
   <si>
     <t>There might be experimental limits to how 'small' you can get</t>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="96">
+    <row r="47" spans="1:11" ht="31.5">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2181,6 +2181,9 @@
         <v>59</v>
       </c>
       <c r="I47" s="1"/>
+      <c r="K47" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="48" spans="1:11" ht="32.1">
       <c r="A48" t="s">
@@ -2882,7 +2885,7 @@
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Differntials are small chunks. It is quite a long descrption!</v>
+        <v>This is the long description for Differentials are small chunks. It is quite a long descrption!</v>
       </c>
       <c r="K73" t="s">
         <v>15</v>
@@ -3119,7 +3122,7 @@
       </c>
       <c r="E82" t="str">
         <f>"["&amp;B73&amp;"]"</f>
-        <v>[Differntials are small chunks]</v>
+        <v>[Differentials are small chunks]</v>
       </c>
       <c r="F82" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
color arrows to emphasize left-going arrows, which are less obvious
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="112">
   <si>
     <t>Act or Con</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>You can flip a derivative</t>
+  </si>
+  <si>
+    <t>In other words, $\frac{dy}{dx} = \frac{1}{\frac{dx}{dy}}$</t>
   </si>
   <si>
     <t>"With respect to what" matters</t>
@@ -943,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1374,7 +1377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1393,9 +1396,8 @@
       <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for You can flip a derivative. It is quite a long descrption!</v>
+      <c r="I16" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="K16" t="s">
         <v>15</v>
@@ -1406,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1433,7 +1435,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" t="str">
         <f>"["&amp;B13&amp;"]"</f>
@@ -1446,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1461,19 +1463,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
         <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" t="s">
-        <v>32</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1488,7 +1490,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -1500,7 +1502,7 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1515,7 +1517,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
@@ -1527,7 +1529,7 @@
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1542,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -1554,7 +1556,7 @@
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1569,7 +1571,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1581,7 +1583,7 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1596,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1608,7 +1610,7 @@
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1620,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25" t="str">
         <f>"["&amp;B6&amp;"]"</f>
@@ -1633,7 +1635,7 @@
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1648,7 +1650,7 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1660,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1675,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" t="str">
         <f>"["&amp;B6&amp;"]"</f>
@@ -1688,7 +1690,7 @@
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1703,7 +1705,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -1715,7 +1717,7 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1730,7 +1732,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -1742,7 +1744,7 @@
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1757,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1769,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1784,7 +1786,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1796,7 +1798,7 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1808,10 +1810,10 @@
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D32" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
@@ -1822,10 +1824,10 @@
         <v>[Derivatives can be found while holding some variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1837,10 +1839,10 @@
     </row>
     <row r="33" spans="1:11" ht="63">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" t="str">
         <f>"["&amp;B6&amp;", "&amp;B8&amp;", "&amp;B12&amp;", "&amp;B17&amp;"]"</f>
@@ -1851,10 +1853,10 @@
         <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, Partial derivatives depend on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1866,10 +1868,10 @@
     </row>
     <row r="34" spans="1:11" ht="63.95">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D34" t="str">
         <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;"]"</f>
@@ -1880,10 +1882,10 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1895,10 +1897,10 @@
     </row>
     <row r="35" spans="1:11" ht="48">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D35" t="str">
         <f>"["&amp;B6&amp;", "&amp;B23&amp;"]"</f>
@@ -1908,10 +1910,10 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1923,10 +1925,10 @@
     </row>
     <row r="36" spans="1:11" ht="96">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D36" t="str">
         <f>"["&amp;B6&amp;", "&amp;B18&amp;", "&amp;B19&amp;", "&amp;B20&amp;"]"</f>
@@ -1937,10 +1939,10 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1952,10 +1954,10 @@
     </row>
     <row r="37" spans="1:11" ht="80.099999999999994">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D37" t="str">
         <f>"["&amp;B10&amp;", "&amp;B19&amp;", "&amp;B23&amp;"]"</f>
@@ -1966,10 +1968,10 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane]</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1984,7 +1986,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -1996,11 +1998,14 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for The components of d \vec r is an arbitrary small change between two arbitrary position vectors. . It is quite a long descrption!</v>
+      </c>
+      <c r="K38" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="33.950000000000003" customHeight="1">
@@ -2008,7 +2013,7 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -2022,6 +2027,9 @@
       <c r="I39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for The magnitude of dr is the length of a small step along a path. It is quite a long descrption!</v>
+      </c>
+      <c r="K39" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="33.950000000000003" customHeight="1">
@@ -2029,7 +2037,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -2044,13 +2052,16 @@
         <f t="shared" si="0"/>
         <v>This is the long description for The direction of dr is ? . It is quite a long descrption!</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="48">
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="47.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -2062,16 +2073,19 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for The gradient can tell you a small change in a function in any direction (differentials edition). It is quite a long descrption!</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="32.1">
+      <c r="K41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75">
       <c r="B42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -2085,6 +2099,9 @@
       <c r="I42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for The divergence is a scalar field. It is quite a long descrption!</v>
+      </c>
+      <c r="K42" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="51" customHeight="1">
@@ -2101,9 +2118,12 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I43" s="1"/>
+      <c r="K43" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="30.95" customHeight="1">
       <c r="A44" t="s">
@@ -2119,13 +2139,16 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I44" s="1"/>
+      <c r="K44" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45" spans="1:11" ht="45" customHeight="1">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -2137,9 +2160,12 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I45" s="1"/>
+      <c r="K45" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="46" spans="1:11" ht="45.95" customHeight="1">
       <c r="A46" t="s">
@@ -2155,16 +2181,19 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I46" s="1"/>
+      <c r="K46" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:11" ht="31.5">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D47" t="str">
         <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
@@ -2175,22 +2204,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I47" s="1"/>
-      <c r="K47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="32.1">
+    </row>
+    <row r="48" spans="1:11" ht="15.75">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D48" t="str">
         <f>"["&amp;B28&amp;"]"</f>
@@ -2201,19 +2227,22 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I48" s="1"/>
+      <c r="K48" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="32.1">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D49" t="str">
         <f>"["&amp;B64&amp;"]"</f>
@@ -2226,7 +2255,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2241,19 +2270,19 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" t="s">
         <v>70</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" t="s">
-        <v>69</v>
       </c>
       <c r="I50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2268,7 +2297,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D51" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2281,7 +2310,7 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2296,7 +2325,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -2308,7 +2337,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2323,7 +2352,7 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -2335,7 +2364,7 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2350,7 +2379,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -2362,7 +2391,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2377,7 +2406,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D55" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2390,7 +2419,7 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2405,7 +2434,7 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -2417,7 +2446,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2432,7 +2461,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -2444,7 +2473,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2459,7 +2488,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -2471,7 +2500,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2486,7 +2515,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -2498,7 +2527,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2513,7 +2542,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D60" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2526,7 +2555,7 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2541,7 +2570,7 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -2553,7 +2582,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2568,7 +2597,7 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -2580,7 +2609,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2595,7 +2624,7 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -2607,7 +2636,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2619,10 +2648,10 @@
     </row>
     <row r="64" spans="1:11" ht="48">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D64" t="str">
         <f>"["&amp;B2&amp;", "&amp;B38&amp;"]"</f>
@@ -2633,10 +2662,10 @@
         <v>[Differential form of r in spherical and cylindrical coordinates]</v>
       </c>
       <c r="F64" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G64" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2648,10 +2677,10 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -2663,7 +2692,7 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2675,10 +2704,10 @@
     </row>
     <row r="66" spans="1:11" ht="48">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D66" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
@@ -2689,10 +2718,10 @@
         <v>[The gradient's dimension is the same as real spice. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G66" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2704,10 +2733,10 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -2719,7 +2748,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2731,10 +2760,10 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -2746,7 +2775,7 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2761,7 +2790,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -2773,7 +2802,7 @@
         <v>13</v>
       </c>
       <c r="G69" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2788,19 +2817,19 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" t="s">
         <v>93</v>
-      </c>
-      <c r="D70" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" t="s">
-        <v>92</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2815,7 +2844,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -2827,7 +2856,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2842,7 +2871,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -2854,7 +2883,7 @@
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2869,7 +2898,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -2881,7 +2910,7 @@
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2896,7 +2925,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -2908,7 +2937,7 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2923,7 +2952,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -2935,7 +2964,7 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2950,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -2962,7 +2991,7 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2977,7 +3006,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -2989,7 +3018,7 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3004,7 +3033,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -3016,7 +3045,7 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I78" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3031,7 +3060,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -3043,7 +3072,7 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3058,7 +3087,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D80" t="s">
         <v>13</v>
@@ -3070,7 +3099,7 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3082,10 +3111,10 @@
     </row>
     <row r="81" spans="1:11" ht="15.75">
       <c r="A81" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B81" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D81" t="str">
         <f>"["&amp;B2&amp;", "&amp;B4&amp;", "&amp;B5&amp;", "&amp;B7&amp;", "&amp;B8&amp;", "&amp;B13&amp;"]"</f>
@@ -3099,7 +3128,7 @@
         <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3111,10 +3140,10 @@
     </row>
     <row r="82" spans="1:11" ht="15.75">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B82" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D82" t="str">
         <f>"["&amp;B69&amp;", "&amp;B71&amp;"]"</f>
@@ -3128,7 +3157,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3140,10 +3169,10 @@
     </row>
     <row r="83" spans="1:11" ht="31.5">
       <c r="A83" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D83" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;"]"</f>
@@ -3157,7 +3186,7 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I83" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3169,10 +3198,10 @@
     </row>
     <row r="84" spans="1:11" ht="15.75">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D84" t="str">
         <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
@@ -3186,7 +3215,7 @@
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I84" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3218,17 +3247,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new representation and put course prereqs always vertically above activity/concept prereqs
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="114">
   <si>
     <t>Act or Con</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Chain Rules</t>
+  </si>
+  <si>
+    <t>[partial f/partial x fixing y]</t>
   </si>
   <si>
     <t>$\frac{\partial f}{\partial x}$</t>
@@ -949,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -3038,8 +3041,9 @@
       <c r="B78" t="s">
         <v>102</v>
       </c>
-      <c r="D78" t="s">
-        <v>13</v>
+      <c r="D78" t="str">
+        <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
+        <v>[You can flip a derivative, Derivatives can be found while holding some variables constant]</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -3169,7 +3173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="31.5">
+    <row r="83" spans="1:11" ht="93" customHeight="1">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -3198,7 +3202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.75">
+    <row r="84" spans="1:11" ht="31.5">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differntials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="G84" t="s">
         <v>93</v>
@@ -3249,17 +3253,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove redundant copies of concepts
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -180,7 +180,7 @@
     <t>The hot plate</t>
   </si>
   <si>
-    <t>[$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer]</t>
+    <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
   </si>
   <si>
     <t>Chain Rule</t>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1843,7 +1843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="63">
+    <row r="33" spans="1:11" ht="47.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
add "hints" to be removed later for concepts related to a given concept
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="115">
   <si>
     <t>Act or Con</t>
   </si>
@@ -138,6 +138,9 @@
     <t>The derivative is related to the density of contour lines</t>
   </si>
   <si>
+    <t>[Contour Maps]</t>
+  </si>
+  <si>
     <t>Partial derivatives depend on the value(s) of what is held constant</t>
   </si>
   <si>
@@ -174,9 +177,6 @@
     <t>The heater II</t>
   </si>
   <si>
-    <t>[Contour Maps]</t>
-  </si>
-  <si>
     <t>The hot plate</t>
   </si>
   <si>
@@ -306,10 +306,13 @@
     <t>Differentials are small changes / differences</t>
   </si>
   <si>
+    <t>[df]</t>
+  </si>
+  <si>
     <t>PH 423</t>
   </si>
   <si>
-    <t>Equations can be 'zapped with d' to relate differnetials</t>
+    <t>Equations can be 'zapped with d' to relate differentials</t>
   </si>
   <si>
     <t>Individual differentials can be manipulated algebraically</t>
@@ -342,7 +345,7 @@
     <t>There might be experimental limits on what quantities you can measure</t>
   </si>
   <si>
-    <t>Differntials allow the finding of partial derivatives when a variable cannot be solved for</t>
+    <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
   </si>
   <si>
     <t>Zapping with d</t>
@@ -952,8 +955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="B56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1059,7 +1063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="32.1">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1518,7 +1522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="32.1">
+    <row r="21" spans="1:11" ht="31.5">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1532,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
         <v>33</v>
@@ -1550,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -1577,7 +1581,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1604,7 +1608,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1628,7 +1632,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" t="str">
         <f>"["&amp;B6&amp;"]"</f>
@@ -1651,12 +1655,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="32.1">
+    <row r="26" spans="1:11" ht="31.5">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1665,7 +1669,7 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G26" t="s">
         <v>33</v>
@@ -1683,7 +1687,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" t="str">
         <f>"["&amp;B6&amp;"]"</f>
@@ -1711,7 +1715,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -1738,7 +1742,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -1765,7 +1769,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1792,7 +1796,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1816,10 +1820,10 @@
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D32" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
@@ -1830,7 +1834,7 @@
         <v>[Derivatives can be found while holding some variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
@@ -1845,7 +1849,7 @@
     </row>
     <row r="33" spans="1:11" ht="47.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
         <v>50</v>
@@ -1874,7 +1878,7 @@
     </row>
     <row r="34" spans="1:11" ht="63.95">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>52</v>
@@ -1903,7 +1907,7 @@
     </row>
     <row r="35" spans="1:11" ht="48">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
@@ -1931,7 +1935,7 @@
     </row>
     <row r="36" spans="1:11" ht="96">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>56</v>
@@ -1960,7 +1964,7 @@
     </row>
     <row r="37" spans="1:11" ht="80.099999999999994">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
         <v>57</v>
@@ -2196,7 +2200,7 @@
     </row>
     <row r="47" spans="1:11" ht="31.5">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
         <v>66</v>
@@ -2219,7 +2223,7 @@
     </row>
     <row r="48" spans="1:11" ht="15.75">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>68</v>
@@ -2233,7 +2237,7 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G48" t="s">
         <v>60</v>
@@ -2462,7 +2466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="32.1">
+    <row r="57" spans="1:11" ht="31.5">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2654,7 +2658,7 @@
     </row>
     <row r="64" spans="1:11" ht="48">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
         <v>85</v>
@@ -2683,7 +2687,7 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
         <v>87</v>
@@ -2710,7 +2714,7 @@
     </row>
     <row r="66" spans="1:11" ht="48">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
         <v>88</v>
@@ -2739,7 +2743,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
         <v>90</v>
@@ -2766,7 +2770,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
         <v>91</v>
@@ -2798,17 +2802,18 @@
       <c r="B69" t="s">
         <v>92</v>
       </c>
-      <c r="D69" t="s">
-        <v>13</v>
+      <c r="D69" t="str">
+        <f>"["&amp;B$2&amp;"]"</f>
+        <v>[Difference / Change]</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G69" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2823,23 +2828,23 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" t="s">
         <v>94</v>
       </c>
-      <c r="D70" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" t="s">
-        <v>93</v>
-      </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Equations can be 'zapped with d' to relate differnetials. It is quite a long descrption!</v>
+        <v>This is the long description for Equations can be 'zapped with d' to relate differentials. It is quite a long descrption!</v>
       </c>
       <c r="K70" t="s">
         <v>15</v>
@@ -2850,7 +2855,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -2862,7 +2867,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2877,7 +2882,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -2886,10 +2891,10 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2904,7 +2909,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -2913,10 +2918,10 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G73" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2931,10 +2936,11 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>98</v>
-      </c>
-      <c r="D74" t="s">
-        <v>13</v>
+        <v>99</v>
+      </c>
+      <c r="D74" t="str">
+        <f>"["&amp;B$4&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes]</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -2943,7 +2949,7 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2958,7 +2964,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -2970,7 +2976,7 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2985,7 +2991,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -2997,7 +3003,7 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3007,15 +3013,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="31.5">
+    <row r="77" spans="1:11" ht="50.25" customHeight="1">
       <c r="A77" t="s">
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>101</v>
-      </c>
-      <c r="D77" t="s">
-        <v>13</v>
+        <v>102</v>
+      </c>
+      <c r="D77" t="str">
+        <f>"["&amp;B$4&amp;","&amp;B$69&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes,Differentials are small changes / differences]</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -3024,7 +3031,7 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3039,7 +3046,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D78" t="str">
         <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
@@ -3052,10 +3059,10 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -3066,7 +3073,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -3078,7 +3085,7 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3093,7 +3100,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D80" t="s">
         <v>13</v>
@@ -3105,11 +3112,11 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Differntials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long descrption!</v>
+        <v>This is the long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long descrption!</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
@@ -3117,10 +3124,10 @@
     </row>
     <row r="81" spans="1:11" ht="15.75">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D81" t="str">
         <f>"["&amp;B2&amp;", "&amp;B4&amp;", "&amp;B5&amp;", "&amp;B7&amp;", "&amp;B8&amp;", "&amp;B13&amp;"]"</f>
@@ -3128,13 +3135,13 @@
       </c>
       <c r="E81" t="str">
         <f>"["&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B72&amp;"]"</f>
-        <v>[Differentials are small changes / differences, Equations can be 'zapped with d' to relate differnetials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
+        <v>[Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3146,10 +3153,10 @@
     </row>
     <row r="82" spans="1:11" ht="15.75">
       <c r="A82" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D82" t="str">
         <f>"["&amp;B69&amp;", "&amp;B71&amp;"]"</f>
@@ -3163,7 +3170,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3175,10 +3182,10 @@
     </row>
     <row r="83" spans="1:11" ht="93" customHeight="1">
       <c r="A83" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D83" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;"]"</f>
@@ -3192,7 +3199,7 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I83" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3204,24 +3211,24 @@
     </row>
     <row r="84" spans="1:11" ht="31.5">
       <c r="A84" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D84" t="str">
         <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding some variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes / differences, Equations can be 'zapped with d' to relate differnetials, Individual differentials can be manipulated algebraically, Partial derivatives depend on what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
+        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding some variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives depend on what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="E84" t="str">
         <f>"["&amp;B78&amp;", "&amp;B79&amp;", "&amp;B80&amp;"]"</f>
-        <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differntials allow the finding of partial derivatives when a variable cannot be solved for]</v>
+        <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I84" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3253,17 +3260,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add row numbers for concepts, to make it easier to edit spreadsheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -33,7 +33,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>URL name</t>
+    <t>Row</t>
   </si>
   <si>
     <t>[Prereq Concepts]</t>
@@ -956,8 +956,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="B56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <pane ySplit="1" topLeftCell="B16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1016,6 +1016,10 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
+      <c r="C2">
+        <f>ROW()</f>
+        <v>2</v>
+      </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
@@ -1036,12 +1040,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="32.1">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
+      </c>
+      <c r="C3">
+        <f>ROW()</f>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1070,6 +1078,10 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
+      <c r="C4">
+        <f>ROW()</f>
+        <v>4</v>
+      </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
@@ -1090,13 +1102,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="32.1">
+    <row r="5" spans="1:11" ht="31.5">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
+      <c r="C5">
+        <f>ROW()</f>
+        <v>5</v>
+      </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
@@ -1117,13 +1133,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.1">
+    <row r="6" spans="1:11" ht="31.5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
+      <c r="C6">
+        <f>ROW()</f>
+        <v>6</v>
+      </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
@@ -1144,13 +1164,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
+      <c r="C7">
+        <f>ROW()</f>
+        <v>7</v>
+      </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -1171,13 +1195,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="32.1">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
+      <c r="C8">
+        <f>ROW()</f>
+        <v>8</v>
+      </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
@@ -1198,13 +1226,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="32.1">
+    <row r="9" spans="1:11" ht="15.75">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
+      <c r="C9">
+        <f>ROW()</f>
+        <v>9</v>
+      </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -1225,13 +1257,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.1">
+    <row r="10" spans="1:11" ht="15.75">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
+      <c r="C10">
+        <f>ROW()</f>
+        <v>10</v>
+      </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
@@ -1252,13 +1288,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
+      <c r="C11">
+        <f>ROW()</f>
+        <v>11</v>
+      </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
@@ -1279,13 +1319,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="32.1">
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
+      <c r="C12">
+        <f>ROW()</f>
+        <v>12</v>
+      </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
@@ -1306,13 +1350,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="32.1">
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
+      <c r="C13">
+        <f>ROW()</f>
+        <v>13</v>
+      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
@@ -1333,13 +1381,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
+      <c r="C14">
+        <f>ROW()</f>
+        <v>14</v>
+      </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
@@ -1360,13 +1412,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
+      <c r="C15">
+        <f>ROW()</f>
+        <v>15</v>
+      </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -1394,6 +1450,10 @@
       <c r="B16" t="s">
         <v>29</v>
       </c>
+      <c r="C16">
+        <f>ROW()</f>
+        <v>16</v>
+      </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
@@ -1413,13 +1473,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1">
+    <row r="17" spans="1:11" ht="15.75">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
+      <c r="C17">
+        <f>ROW()</f>
+        <v>17</v>
+      </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
@@ -1440,12 +1504,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="32.1">
+    <row r="18" spans="1:11" ht="31.5">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
+      </c>
+      <c r="C18">
+        <f>ROW()</f>
+        <v>18</v>
       </c>
       <c r="D18" t="str">
         <f>"["&amp;B13&amp;"]"</f>
@@ -1468,13 +1536,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="32.1">
+    <row r="19" spans="1:11" ht="31.5">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
+      <c r="C19">
+        <f>ROW()</f>
+        <v>19</v>
+      </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
@@ -1495,13 +1567,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="32.1">
+    <row r="20" spans="1:11" ht="31.5">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
+      <c r="C20">
+        <f>ROW()</f>
+        <v>20</v>
+      </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
@@ -1529,6 +1605,10 @@
       <c r="B21" t="s">
         <v>36</v>
       </c>
+      <c r="C21">
+        <f>ROW()</f>
+        <v>21</v>
+      </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
@@ -1549,13 +1629,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="32.1">
+    <row r="22" spans="1:11" ht="31.5">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
+      <c r="C22">
+        <f>ROW()</f>
+        <v>22</v>
+      </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
@@ -1576,13 +1660,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="32.1">
+    <row r="23" spans="1:11" ht="31.5">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>39</v>
       </c>
+      <c r="C23">
+        <f>ROW()</f>
+        <v>23</v>
+      </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
@@ -1603,13 +1691,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="15.75">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
+      <c r="C24">
+        <f>ROW()</f>
+        <v>24</v>
+      </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
@@ -1627,12 +1719,16 @@
         <v>This is the long description for The gradient is a vector. It is quite a long descrption!</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="48">
+    <row r="25" spans="1:11" ht="47.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
+      </c>
+      <c r="C25">
+        <f>ROW()</f>
+        <v>25</v>
       </c>
       <c r="D25" t="str">
         <f>"["&amp;B6&amp;"]"</f>
@@ -1662,6 +1758,10 @@
       <c r="B26" t="s">
         <v>42</v>
       </c>
+      <c r="C26">
+        <f>ROW()</f>
+        <v>26</v>
+      </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
@@ -1682,16 +1782,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="32.1">
+    <row r="27" spans="1:11" ht="31.5">
       <c r="A27" t="s">
         <v>11</v>
       </c>
       <c r="B27" t="s">
         <v>43</v>
       </c>
+      <c r="C27">
+        <f>ROW()</f>
+        <v>27</v>
+      </c>
       <c r="D27" t="str">
-        <f>"["&amp;B6&amp;"]"</f>
-        <v>[The derivative is the slope of a tangent line]</v>
+        <f>"["&amp;B6&amp;","&amp;B$19&amp;"]"</f>
+        <v>[The derivative is the slope of a tangent line,There is a  partial derivative in every direction at any point]</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1710,13 +1814,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="32.1">
+    <row r="28" spans="1:11" ht="31.5">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
+      <c r="C28">
+        <f>ROW()</f>
+        <v>28</v>
+      </c>
       <c r="D28" t="s">
         <v>13</v>
       </c>
@@ -1737,13 +1845,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="32.1">
+    <row r="29" spans="1:11" ht="15.75">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
       </c>
+      <c r="C29">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
@@ -1764,13 +1876,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="32.1">
+    <row r="30" spans="1:11" ht="15.75">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
         <v>46</v>
       </c>
+      <c r="C30">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
       <c r="D30" t="s">
         <v>13</v>
       </c>
@@ -1791,12 +1907,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="32.1">
+    <row r="31" spans="1:11" ht="15.75">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
+      </c>
+      <c r="C31">
+        <f>ROW()</f>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1825,6 +1945,10 @@
       <c r="B32" t="s">
         <v>49</v>
       </c>
+      <c r="C32">
+        <f>ROW()</f>
+        <v>32</v>
+      </c>
       <c r="D32" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
         <v>[The derivative is a ratio of small changes, Variables can be held constant, "With respect to what" matters]</v>
@@ -1854,6 +1978,10 @@
       <c r="B33" t="s">
         <v>50</v>
       </c>
+      <c r="C33">
+        <f>ROW()</f>
+        <v>33</v>
+      </c>
       <c r="D33" t="str">
         <f>"["&amp;B6&amp;", "&amp;B8&amp;", "&amp;B12&amp;", "&amp;B17&amp;"]"</f>
         <v>[The derivative is the slope of a tangent line, The derivative can be a function, The derivative at a cusp is undefined, "With respect to what" matters]</v>
@@ -1876,12 +2004,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="63.95">
+    <row r="34" spans="1:11" ht="15.75">
       <c r="A34" t="s">
         <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>52</v>
+      </c>
+      <c r="C34">
+        <f>ROW()</f>
+        <v>34</v>
       </c>
       <c r="D34" t="str">
         <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;"]"</f>
@@ -1905,12 +2037,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="48">
+    <row r="35" spans="1:11" ht="31.5">
       <c r="A35" t="s">
         <v>48</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
+      </c>
+      <c r="C35">
+        <f>ROW()</f>
+        <v>35</v>
       </c>
       <c r="D35" t="str">
         <f>"["&amp;B6&amp;", "&amp;B23&amp;"]"</f>
@@ -1933,12 +2069,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="96">
+    <row r="36" spans="1:11" ht="31.5">
       <c r="A36" t="s">
         <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>56</v>
+      </c>
+      <c r="C36">
+        <f>ROW()</f>
+        <v>36</v>
       </c>
       <c r="D36" t="str">
         <f>"["&amp;B6&amp;", "&amp;B18&amp;", "&amp;B19&amp;", "&amp;B20&amp;"]"</f>
@@ -1962,12 +2102,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="80.099999999999994">
+    <row r="37" spans="1:11" ht="47.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
       <c r="B37" t="s">
         <v>57</v>
+      </c>
+      <c r="C37">
+        <f>ROW()</f>
+        <v>37</v>
       </c>
       <c r="D37" t="str">
         <f>"["&amp;B10&amp;", "&amp;B19&amp;", "&amp;B23&amp;"]"</f>
@@ -1998,6 +2142,10 @@
       <c r="B38" t="s">
         <v>59</v>
       </c>
+      <c r="C38">
+        <f>ROW()</f>
+        <v>38</v>
+      </c>
       <c r="D38" t="s">
         <v>13</v>
       </c>
@@ -2025,6 +2173,10 @@
       <c r="B39" t="s">
         <v>61</v>
       </c>
+      <c r="C39">
+        <f>ROW()</f>
+        <v>39</v>
+      </c>
       <c r="D39" t="s">
         <v>13</v>
       </c>
@@ -2049,6 +2201,10 @@
       <c r="B40" t="s">
         <v>62</v>
       </c>
+      <c r="C40">
+        <f>ROW()</f>
+        <v>40</v>
+      </c>
       <c r="D40" t="s">
         <v>13</v>
       </c>
@@ -2072,6 +2228,10 @@
       </c>
       <c r="B41" t="s">
         <v>63</v>
+      </c>
+      <c r="C41">
+        <f>ROW()</f>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -2097,6 +2257,10 @@
       <c r="B42" t="s">
         <v>64</v>
       </c>
+      <c r="C42">
+        <f>ROW()</f>
+        <v>42</v>
+      </c>
       <c r="D42" t="s">
         <v>13</v>
       </c>
@@ -2118,6 +2282,10 @@
       <c r="A43" t="s">
         <v>11</v>
       </c>
+      <c r="C43">
+        <f>ROW()</f>
+        <v>43</v>
+      </c>
       <c r="D43" t="s">
         <v>13</v>
       </c>
@@ -2138,6 +2306,10 @@
     <row r="44" spans="1:11" ht="30.95" customHeight="1">
       <c r="A44" t="s">
         <v>11</v>
+      </c>
+      <c r="C44">
+        <f>ROW()</f>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -2160,6 +2332,10 @@
       <c r="A45" t="s">
         <v>65</v>
       </c>
+      <c r="C45">
+        <f>ROW()</f>
+        <v>45</v>
+      </c>
       <c r="D45" t="s">
         <v>13</v>
       </c>
@@ -2180,6 +2356,10 @@
     <row r="46" spans="1:11" ht="45.95" customHeight="1">
       <c r="A46" t="s">
         <v>11</v>
+      </c>
+      <c r="C46">
+        <f>ROW()</f>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -2205,6 +2385,10 @@
       <c r="B47" t="s">
         <v>66</v>
       </c>
+      <c r="C47">
+        <f>ROW()</f>
+        <v>47</v>
+      </c>
       <c r="D47" t="str">
         <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
         <v>[Derivatives can be found while holding some variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, Partial derivatives depend on the value(s) of what is held constant]</v>
@@ -2228,6 +2412,10 @@
       <c r="B48" t="s">
         <v>68</v>
       </c>
+      <c r="C48">
+        <f>ROW()</f>
+        <v>48</v>
+      </c>
       <c r="D48" t="str">
         <f>"["&amp;B28&amp;"]"</f>
         <v>[The components of the gradient are partial derivatives]</v>
@@ -2247,12 +2435,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="32.1">
+    <row r="49" spans="1:11" ht="31.5">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
         <v>69</v>
+      </c>
+      <c r="C49">
+        <f>ROW()</f>
+        <v>49</v>
       </c>
       <c r="D49" t="str">
         <f>"["&amp;B64&amp;"]"</f>
@@ -2282,6 +2474,10 @@
       <c r="B50" t="s">
         <v>71</v>
       </c>
+      <c r="C50">
+        <f>ROW()</f>
+        <v>50</v>
+      </c>
       <c r="D50" t="s">
         <v>13</v>
       </c>
@@ -2302,12 +2498,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="32.1">
+    <row r="51" spans="1:11" ht="15.75">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51" t="s">
         <v>72</v>
+      </c>
+      <c r="C51">
+        <f>ROW()</f>
+        <v>51</v>
       </c>
       <c r="D51" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2330,13 +2530,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="32.1">
+    <row r="52" spans="1:11" ht="31.5">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>73</v>
       </c>
+      <c r="C52">
+        <f>ROW()</f>
+        <v>52</v>
+      </c>
       <c r="D52" t="s">
         <v>13</v>
       </c>
@@ -2357,13 +2561,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="32.1">
+    <row r="53" spans="1:11" ht="31.5">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
         <v>74</v>
       </c>
+      <c r="C53">
+        <f>ROW()</f>
+        <v>53</v>
+      </c>
       <c r="D53" t="s">
         <v>13</v>
       </c>
@@ -2384,13 +2592,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="32.1">
+    <row r="54" spans="1:11" ht="15.75">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
         <v>75</v>
       </c>
+      <c r="C54">
+        <f>ROW()</f>
+        <v>54</v>
+      </c>
       <c r="D54" t="s">
         <v>13</v>
       </c>
@@ -2411,12 +2623,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="32.1">
+    <row r="55" spans="1:11" ht="15.75">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
         <v>76</v>
+      </c>
+      <c r="C55">
+        <f>ROW()</f>
+        <v>55</v>
       </c>
       <c r="D55" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2439,13 +2655,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="32.1">
+    <row r="56" spans="1:11" ht="31.5">
       <c r="A56" t="s">
         <v>11</v>
       </c>
       <c r="B56" t="s">
         <v>77</v>
       </c>
+      <c r="C56">
+        <f>ROW()</f>
+        <v>56</v>
+      </c>
       <c r="D56" t="s">
         <v>13</v>
       </c>
@@ -2473,6 +2693,10 @@
       <c r="B57" t="s">
         <v>78</v>
       </c>
+      <c r="C57">
+        <f>ROW()</f>
+        <v>57</v>
+      </c>
       <c r="D57" t="s">
         <v>13</v>
       </c>
@@ -2493,13 +2717,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="48">
+    <row r="58" spans="1:11" ht="31.5">
       <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
         <v>79</v>
       </c>
+      <c r="C58">
+        <f>ROW()</f>
+        <v>58</v>
+      </c>
       <c r="D58" t="s">
         <v>13</v>
       </c>
@@ -2520,13 +2748,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="32.1">
+    <row r="59" spans="1:11" ht="15.75">
       <c r="A59" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
         <v>80</v>
       </c>
+      <c r="C59">
+        <f>ROW()</f>
+        <v>59</v>
+      </c>
       <c r="D59" t="s">
         <v>13</v>
       </c>
@@ -2547,12 +2779,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="32.1">
+    <row r="60" spans="1:11" ht="15.75">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
+      </c>
+      <c r="C60">
+        <f>ROW()</f>
+        <v>60</v>
       </c>
       <c r="D60" t="str">
         <f>"["&amp;B29&amp;"]"</f>
@@ -2575,13 +2811,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="32.1">
+    <row r="61" spans="1:11" ht="31.5">
       <c r="A61" t="s">
         <v>11</v>
       </c>
       <c r="B61" t="s">
         <v>82</v>
       </c>
+      <c r="C61">
+        <f>ROW()</f>
+        <v>61</v>
+      </c>
       <c r="D61" t="s">
         <v>13</v>
       </c>
@@ -2602,13 +2842,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="32.1">
+    <row r="62" spans="1:11" ht="31.5">
       <c r="A62" t="s">
         <v>11</v>
       </c>
       <c r="B62" t="s">
         <v>83</v>
       </c>
+      <c r="C62">
+        <f>ROW()</f>
+        <v>62</v>
+      </c>
       <c r="D62" t="s">
         <v>13</v>
       </c>
@@ -2629,13 +2873,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="48">
+    <row r="63" spans="1:11" ht="47.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">
         <v>84</v>
       </c>
+      <c r="C63">
+        <f>ROW()</f>
+        <v>63</v>
+      </c>
       <c r="D63" t="s">
         <v>13</v>
       </c>
@@ -2656,12 +2904,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="48">
+    <row r="64" spans="1:11" ht="15.75">
       <c r="A64" t="s">
         <v>48</v>
       </c>
       <c r="B64" t="s">
         <v>85</v>
+      </c>
+      <c r="C64">
+        <f>ROW()</f>
+        <v>64</v>
       </c>
       <c r="D64" t="str">
         <f>"["&amp;B2&amp;", "&amp;B38&amp;"]"</f>
@@ -2685,13 +2937,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" ht="15.75">
       <c r="A65" t="s">
         <v>48</v>
       </c>
       <c r="B65" t="s">
         <v>87</v>
       </c>
+      <c r="C65">
+        <f>ROW()</f>
+        <v>65</v>
+      </c>
       <c r="D65" t="s">
         <v>13</v>
       </c>
@@ -2712,12 +2968,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="48">
+    <row r="66" spans="1:11" ht="47.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
       <c r="B66" t="s">
         <v>88</v>
+      </c>
+      <c r="C66">
+        <f>ROW()</f>
+        <v>66</v>
       </c>
       <c r="D66" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
@@ -2741,13 +3001,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" ht="15.75">
       <c r="A67" t="s">
         <v>48</v>
       </c>
       <c r="B67" t="s">
         <v>90</v>
       </c>
+      <c r="C67">
+        <f>ROW()</f>
+        <v>67</v>
+      </c>
       <c r="D67" t="s">
         <v>13</v>
       </c>
@@ -2768,13 +3032,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" ht="15.75">
       <c r="A68" t="s">
         <v>48</v>
       </c>
       <c r="B68" t="s">
         <v>91</v>
       </c>
+      <c r="C68">
+        <f>ROW()</f>
+        <v>68</v>
+      </c>
       <c r="D68" t="s">
         <v>13</v>
       </c>
@@ -2801,6 +3069,10 @@
       </c>
       <c r="B69" t="s">
         <v>92</v>
+      </c>
+      <c r="C69">
+        <f>ROW()</f>
+        <v>69</v>
       </c>
       <c r="D69" t="str">
         <f>"["&amp;B$2&amp;"]"</f>
@@ -2830,6 +3102,10 @@
       <c r="B70" t="s">
         <v>95</v>
       </c>
+      <c r="C70">
+        <f>ROW()</f>
+        <v>70</v>
+      </c>
       <c r="D70" t="s">
         <v>13</v>
       </c>
@@ -2857,6 +3133,10 @@
       <c r="B71" t="s">
         <v>96</v>
       </c>
+      <c r="C71">
+        <f>ROW()</f>
+        <v>71</v>
+      </c>
       <c r="D71" t="s">
         <v>13</v>
       </c>
@@ -2884,6 +3164,10 @@
       <c r="B72" t="s">
         <v>97</v>
       </c>
+      <c r="C72">
+        <f>ROW()</f>
+        <v>72</v>
+      </c>
       <c r="D72" t="s">
         <v>13</v>
       </c>
@@ -2911,6 +3195,10 @@
       <c r="B73" t="s">
         <v>98</v>
       </c>
+      <c r="C73">
+        <f>ROW()</f>
+        <v>73</v>
+      </c>
       <c r="D73" t="s">
         <v>13</v>
       </c>
@@ -2937,6 +3225,10 @@
       </c>
       <c r="B74" t="s">
         <v>99</v>
+      </c>
+      <c r="C74">
+        <f>ROW()</f>
+        <v>74</v>
       </c>
       <c r="D74" t="str">
         <f>"["&amp;B$4&amp;"]"</f>
@@ -2966,6 +3258,10 @@
       <c r="B75" t="s">
         <v>100</v>
       </c>
+      <c r="C75">
+        <f>ROW()</f>
+        <v>75</v>
+      </c>
       <c r="D75" t="s">
         <v>13</v>
       </c>
@@ -2993,6 +3289,10 @@
       <c r="B76" t="s">
         <v>101</v>
       </c>
+      <c r="C76">
+        <f>ROW()</f>
+        <v>76</v>
+      </c>
       <c r="D76" t="s">
         <v>13</v>
       </c>
@@ -3019,6 +3319,10 @@
       </c>
       <c r="B77" t="s">
         <v>102</v>
+      </c>
+      <c r="C77">
+        <f>ROW()</f>
+        <v>77</v>
       </c>
       <c r="D77" t="str">
         <f>"["&amp;B$4&amp;","&amp;B$69&amp;"]"</f>
@@ -3048,6 +3352,10 @@
       <c r="B78" t="s">
         <v>103</v>
       </c>
+      <c r="C78">
+        <f>ROW()</f>
+        <v>78</v>
+      </c>
       <c r="D78" t="str">
         <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
         <v>[You can flip a derivative, Derivatives can be found while holding some variables constant]</v>
@@ -3075,6 +3383,10 @@
       <c r="B79" t="s">
         <v>105</v>
       </c>
+      <c r="C79">
+        <f>ROW()</f>
+        <v>79</v>
+      </c>
       <c r="D79" t="s">
         <v>13</v>
       </c>
@@ -3101,6 +3413,10 @@
       </c>
       <c r="B80" t="s">
         <v>106</v>
+      </c>
+      <c r="C80">
+        <f>ROW()</f>
+        <v>80</v>
       </c>
       <c r="D80" t="s">
         <v>13</v>
@@ -3129,6 +3445,10 @@
       <c r="B81" t="s">
         <v>107</v>
       </c>
+      <c r="C81">
+        <f>ROW()</f>
+        <v>81</v>
+      </c>
       <c r="D81" t="str">
         <f>"["&amp;B2&amp;", "&amp;B4&amp;", "&amp;B5&amp;", "&amp;B7&amp;", "&amp;B8&amp;", "&amp;B13&amp;"]"</f>
         <v>[Difference / Change, The derivative is a ratio of small changes, The derivative can be approximated by the slope of a secant line, The derivative is a limit, The derivative can be a function, Variables can be held constant]</v>
@@ -3158,6 +3478,10 @@
       <c r="B82" t="s">
         <v>108</v>
       </c>
+      <c r="C82">
+        <f>ROW()</f>
+        <v>82</v>
+      </c>
       <c r="D82" t="str">
         <f>"["&amp;B69&amp;", "&amp;B71&amp;"]"</f>
         <v>[Differentials are small changes / differences, Individual differentials can be manipulated algebraically]</v>
@@ -3187,6 +3511,10 @@
       <c r="B83" t="s">
         <v>109</v>
       </c>
+      <c r="C83">
+        <f>ROW()</f>
+        <v>83</v>
+      </c>
       <c r="D83" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;"]"</f>
         <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding some variables constant, Partial derivatives depend on the value(s) of what is held constant]</v>
@@ -3215,6 +3543,10 @@
       </c>
       <c r="B84" t="s">
         <v>110</v>
+      </c>
+      <c r="C84">
+        <f>ROW()</f>
+        <v>84</v>
       </c>
       <c r="D84" t="str">
         <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>

</xml_diff>

<commit_message>
use rsync rather than cp, and update progression sheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -956,8 +956,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="B16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -2004,7 +2004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75">
+    <row r="34" spans="1:11" ht="71.25" customHeight="1">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2016,8 +2016,8 @@
         <v>34</v>
       </c>
       <c r="D34" t="str">
-        <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;"]"</f>
-        <v>[The derivative can be a function, The derivative is a linear function, Variables can be held constant, Product rule, "With respect to what" matters]</v>
+        <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;", "&amp;B15&amp;"]"</f>
+        <v>[The derivative can be a function, The derivative is a linear function, Variables can be held constant, Product rule, "With respect to what" matters, Single variable chain rule]</v>
       </c>
       <c r="E34" t="str">
         <f>"["&amp;B23&amp;"]"</f>

</xml_diff>

<commit_message>
handle external URL links
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="116">
   <si>
     <t>Act or Con</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>The Valley</t>
+  </si>
+  <si>
+    <t>vcvalley</t>
   </si>
   <si>
     <t>Differential form of r in spherical and cylindrical coordinates</t>
@@ -956,8 +959,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="E43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1671,8 +1674,9 @@
         <f>ROW()</f>
         <v>23</v>
       </c>
-      <c r="D23" t="s">
-        <v>13</v>
+      <c r="D23" t="str">
+        <f>"["&amp;B15&amp;"]"</f>
+        <v>[Single variable chain rule]</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -2431,6 +2435,9 @@
         <v>60</v>
       </c>
       <c r="I48" s="1"/>
+      <c r="J48" t="s">
+        <v>69</v>
+      </c>
       <c r="K48" t="s">
         <v>15</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2457,7 +2464,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2472,23 +2479,23 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50">
+        <f>ROW()</f>
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" t="s">
         <v>71</v>
-      </c>
-      <c r="C50">
-        <f>ROW()</f>
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" t="s">
-        <v>70</v>
       </c>
       <c r="I50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2503,7 +2510,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2520,7 +2527,7 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2535,7 +2542,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -2551,7 +2558,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2566,7 +2573,7 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -2582,7 +2589,7 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2597,7 +2604,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -2613,7 +2620,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2628,7 +2635,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -2645,7 +2652,7 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2660,7 +2667,7 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -2676,7 +2683,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2691,7 +2698,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -2707,7 +2714,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2722,7 +2729,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -2738,7 +2745,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2753,7 +2760,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -2769,7 +2776,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2784,7 +2791,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -2801,7 +2808,7 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2816,7 +2823,7 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -2832,7 +2839,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2847,7 +2854,7 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -2863,7 +2870,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2878,7 +2885,7 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -2894,7 +2901,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2909,7 +2916,7 @@
         <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -2924,10 +2931,10 @@
         <v>[Differential form of r in spherical and cylindrical coordinates]</v>
       </c>
       <c r="F64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2942,7 +2949,7 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -2958,7 +2965,7 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2973,7 +2980,7 @@
         <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -2988,10 +2995,10 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G66" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3006,7 +3013,7 @@
         <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3022,7 +3029,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3037,7 +3044,7 @@
         <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3053,7 +3060,7 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3068,7 +3075,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3082,10 +3089,10 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G69" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3100,23 +3107,23 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70">
+        <f>ROW()</f>
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" t="s">
         <v>95</v>
-      </c>
-      <c r="C70">
-        <f>ROW()</f>
-        <v>70</v>
-      </c>
-      <c r="D70" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" t="s">
-        <v>94</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3131,7 +3138,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3147,7 +3154,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3162,7 +3169,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3175,10 +3182,10 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G72" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3193,7 +3200,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3206,10 +3213,10 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G73" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3224,7 +3231,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3241,7 +3248,7 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3256,7 +3263,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3272,7 +3279,7 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3287,14 +3294,15 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
         <v>76</v>
       </c>
-      <c r="D76" t="s">
-        <v>13</v>
+      <c r="D76" t="str">
+        <f>"["&amp;B$18&amp;","&amp;B$22&amp;"]"</f>
+        <v>[Derivatives can be found while holding some variables constant,Partial derivatives depend on the value(s) of what is held constant]</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -3303,7 +3311,7 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3318,7 +3326,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3335,7 +3343,7 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3350,7 +3358,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3367,10 +3375,10 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -3381,7 +3389,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3397,7 +3405,7 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3412,7 +3420,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3428,7 +3436,7 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3443,7 +3451,7 @@
         <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3458,10 +3466,10 @@
         <v>[Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G81" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3476,7 +3484,7 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3494,7 +3502,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3509,7 +3517,7 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -3527,7 +3535,7 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I83" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3542,7 +3550,7 @@
         <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3557,10 +3565,10 @@
         <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G84" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I84" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3592,17 +3600,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update progression to have two activities teach same concept
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19222"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="116">
   <si>
     <t>Act or Con</t>
   </si>
@@ -959,8 +959,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="E43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+      <pane ySplit="1" topLeftCell="F39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -2408,6 +2408,9 @@
         <v>60</v>
       </c>
       <c r="I47" s="1"/>
+      <c r="K47" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="48" spans="1:11" ht="15.75">
       <c r="A48" t="s">

</xml_diff>

<commit_message>
updated version of database
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="116">
   <si>
     <t>Act or Con</t>
   </si>
@@ -75,7 +75,7 @@
     <t>Active</t>
   </si>
   <si>
-    <t>How much f changes as x changes</t>
+    <t>How much $f$ changes as $x$ changes</t>
   </si>
   <si>
     <t>The derivative is a ratio of small changes</t>
@@ -204,16 +204,19 @@
     <t>[partial f/partial x, Inclinometer, Del f]</t>
   </si>
   <si>
-    <t xml:space="preserve">The components of d \vec r is an arbitrary small change between two arbitrary position vectors. </t>
+    <t>The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. </t>
   </si>
   <si>
     <t>MTH 255</t>
   </si>
   <si>
-    <t>The magnitude of dr is the length of a small step along a path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The direction of dr is ? </t>
+    <t>The magnitude of $d\vec r$ is the length of a small step along a path</t>
+  </si>
+  <si>
+    <t>PH 422</t>
+  </si>
+  <si>
+    <t>The direction of $d\vec r$ is ? </t>
   </si>
   <si>
     <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
@@ -237,10 +240,7 @@
     <t>vcvalley</t>
   </si>
   <si>
-    <t>Differential form of r in spherical and cylindrical coordinates</t>
-  </si>
-  <si>
-    <t>PH 422</t>
+    <t>Differential form of $\vec r$ in spherical and cylindrical coordinates</t>
   </si>
   <si>
     <t>The gradient's dimension is the same as real space. The gradient lives in the domain</t>
@@ -959,8 +959,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="F39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1043,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
+    <row r="3" spans="1:11" ht="31.5">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="I3" s="1" t="str">
         <f t="shared" ref="I3:I84" si="0">"This is the long description for " &amp;B3 &amp;". It is quite a long descrption!"</f>
-        <v>This is the long description for How much f changes as x changes. It is quite a long descrption!</v>
+        <v>This is the long description for How much $f$ changes as $x$ changes. It is quite a long descrption!</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for The components of d \vec r is an arbitrary small change between two arbitrary position vectors. . It is quite a long descrption!</v>
+        <v>This is the long description for The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. . It is quite a long descrption!</v>
       </c>
       <c r="K38" t="s">
         <v>15</v>
@@ -2190,9 +2190,12 @@
       <c r="F39" t="s">
         <v>13</v>
       </c>
+      <c r="G39" t="s">
+        <v>62</v>
+      </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for The magnitude of dr is the length of a small step along a path. It is quite a long descrption!</v>
+        <v>This is the long description for The magnitude of $d\vec r$ is the length of a small step along a path. It is quite a long descrption!</v>
       </c>
       <c r="K39" t="s">
         <v>15</v>
@@ -2203,24 +2206,27 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40">
+        <f>ROW()</f>
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
         <v>62</v>
       </c>
-      <c r="C40">
-        <f>ROW()</f>
-        <v>40</v>
-      </c>
-      <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" t="s">
-        <v>13</v>
-      </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for The direction of dr is ? . It is quite a long descrption!</v>
+        <v>This is the long description for The direction of $d\vec r$ is ? . It is quite a long descrption!</v>
       </c>
       <c r="K40" t="s">
         <v>15</v>
@@ -2231,7 +2237,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2259,7 +2265,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.75">
       <c r="B42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
@@ -2334,7 +2340,7 @@
     </row>
     <row r="45" spans="1:11" ht="45" customHeight="1">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C45">
         <f>ROW()</f>
@@ -2387,7 +2393,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2402,7 +2408,7 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G47" t="s">
         <v>60</v>
@@ -2417,7 +2423,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2439,7 +2445,7 @@
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K48" t="s">
         <v>15</v>
@@ -2450,7 +2456,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2467,11 +2473,11 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Differential form of r in spherical and cylindrical coordinates. It is quite a long descrption!</v>
+        <v>This is the long description for Differential form of $\vec r$ in spherical and cylindrical coordinates. It is quite a long descrption!</v>
       </c>
       <c r="K49" t="s">
         <v>15</v>
@@ -2498,7 +2504,7 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2530,7 +2536,7 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2561,7 +2567,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2592,7 +2598,7 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2623,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2655,7 +2661,7 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2686,7 +2692,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2717,7 +2723,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2748,7 +2754,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2779,7 +2785,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2811,7 +2817,7 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2842,7 +2848,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2873,7 +2879,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2904,7 +2910,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2927,17 +2933,17 @@
       </c>
       <c r="D64" t="str">
         <f>"["&amp;B2&amp;", "&amp;B38&amp;"]"</f>
-        <v>[Difference / Change, The components of d \vec r is an arbitrary small change between two arbitrary position vectors. ]</v>
+        <v>[Difference / Change, The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. ]</v>
       </c>
       <c r="E64" t="str">
         <f>"["&amp;B49&amp;"]"</f>
-        <v>[Differential form of r in spherical and cylindrical coordinates]</v>
+        <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates]</v>
       </c>
       <c r="F64" t="s">
         <v>87</v>
       </c>
       <c r="G64" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2968,7 +2974,7 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3001,7 +3007,7 @@
         <v>90</v>
       </c>
       <c r="G66" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3032,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3063,7 +3069,7 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
new version of database
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="122">
   <si>
     <t>Act or Con</t>
   </si>
@@ -177,24 +177,36 @@
     <t>The heater II</t>
   </si>
   <si>
+    <t>mvheater2</t>
+  </si>
+  <si>
     <t>The hot plate</t>
   </si>
   <si>
     <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
   </si>
   <si>
+    <t>mvhotplate</t>
+  </si>
+  <si>
     <t>Chain Rule</t>
   </si>
   <si>
     <t>[partial f/partial x]</t>
   </si>
   <si>
+    <t>mvchain</t>
+  </si>
+  <si>
     <t>Chain Rule Measurements</t>
   </si>
   <si>
     <t>[partial f/partial x, Inclinometer]</t>
   </si>
   <si>
+    <t>mvpchain</t>
+  </si>
+  <si>
     <t>The Hillside</t>
   </si>
   <si>
@@ -204,6 +216,9 @@
     <t>[partial f/partial x, Inclinometer, Del f]</t>
   </si>
   <si>
+    <t>mvdderiv</t>
+  </si>
+  <si>
     <t>The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. </t>
   </si>
   <si>
@@ -232,6 +247,9 @@
   </si>
   <si>
     <t>[Contour Maps, Del dot f]</t>
+  </si>
+  <si>
+    <t>vchill</t>
   </si>
   <si>
     <t>The Valley</t>
@@ -959,8 +977,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="I40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1971,6 +1989,9 @@
         <f t="shared" si="0"/>
         <v>This is the long description for The heater II. It is quite a long descrption!</v>
       </c>
+      <c r="J32" t="s">
+        <v>50</v>
+      </c>
       <c r="K32" t="s">
         <v>15</v>
       </c>
@@ -1980,7 +2001,7 @@
         <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -1995,7 +2016,7 @@
         <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, Partial derivatives depend on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
@@ -2003,6 +2024,9 @@
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for The hot plate. It is quite a long descrption!</v>
+      </c>
+      <c r="J33" t="s">
+        <v>53</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
@@ -2013,7 +2037,7 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2028,7 +2052,7 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
         <v>33</v>
@@ -2036,6 +2060,9 @@
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for Chain Rule. It is quite a long descrption!</v>
+      </c>
+      <c r="J34" t="s">
+        <v>56</v>
       </c>
       <c r="K34" t="s">
         <v>15</v>
@@ -2046,7 +2073,7 @@
         <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2060,7 +2087,7 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G35" t="s">
         <v>33</v>
@@ -2068,6 +2095,9 @@
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>This is the long description for Chain Rule Measurements. It is quite a long descrption!</v>
+      </c>
+      <c r="J35" t="s">
+        <v>59</v>
       </c>
       <c r="K35" t="s">
         <v>15</v>
@@ -2078,7 +2108,7 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2093,7 +2123,7 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G36" t="s">
         <v>33</v>
@@ -2111,7 +2141,7 @@
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2126,7 +2156,7 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane]</v>
       </c>
       <c r="F37" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G37" t="s">
         <v>33</v>
@@ -2135,6 +2165,9 @@
         <f t="shared" si="0"/>
         <v>This is the long description for Directional Derivatives. It is quite a long descrption!</v>
       </c>
+      <c r="J37" t="s">
+        <v>63</v>
+      </c>
       <c r="K37" t="s">
         <v>15</v>
       </c>
@@ -2144,7 +2177,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2160,7 +2193,7 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2175,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2191,7 +2224,7 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2206,7 +2239,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
@@ -2222,7 +2255,7 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2237,7 +2270,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2253,7 +2286,7 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2265,7 +2298,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.75">
       <c r="B42" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
@@ -2306,7 +2339,7 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I43" s="1"/>
       <c r="K43" t="s">
@@ -2331,7 +2364,7 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I44" s="1"/>
       <c r="K44" t="s">
@@ -2340,7 +2373,7 @@
     </row>
     <row r="45" spans="1:11" ht="45" customHeight="1">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C45">
         <f>ROW()</f>
@@ -2356,7 +2389,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I45" s="1"/>
       <c r="K45" t="s">
@@ -2381,7 +2414,7 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I46" s="1"/>
       <c r="K46" t="s">
@@ -2393,7 +2426,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2408,12 +2441,15 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G47" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I47" s="1"/>
+      <c r="J47" t="s">
+        <v>74</v>
+      </c>
       <c r="K47" t="s">
         <v>15</v>
       </c>
@@ -2423,7 +2459,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2441,11 +2477,11 @@
         <v>37</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K48" t="s">
         <v>15</v>
@@ -2456,7 +2492,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2473,7 +2509,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2488,7 +2524,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -2504,7 +2540,7 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2519,7 +2555,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2536,7 +2572,7 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2551,7 +2587,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -2567,7 +2603,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2582,7 +2618,7 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -2598,7 +2634,7 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2613,7 +2649,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -2629,7 +2665,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2644,7 +2680,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -2661,7 +2697,7 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2676,7 +2712,7 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -2692,7 +2728,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2707,7 +2743,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -2723,7 +2759,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2738,7 +2774,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -2754,7 +2790,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2769,7 +2805,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -2785,7 +2821,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2800,7 +2836,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -2817,7 +2853,7 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2832,7 +2868,7 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -2848,7 +2884,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2863,7 +2899,7 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -2879,7 +2915,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I62" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2894,7 +2930,7 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -2910,7 +2946,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2925,7 +2961,7 @@
         <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -2940,10 +2976,10 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates]</v>
       </c>
       <c r="F64" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G64" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2958,7 +2994,7 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -2974,7 +3010,7 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2989,7 +3025,7 @@
         <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3004,10 +3040,10 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="G66" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3022,7 +3058,7 @@
         <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3038,7 +3074,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I67" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3053,7 +3089,7 @@
         <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3069,7 +3105,7 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3084,7 +3120,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3098,10 +3134,10 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G69" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3116,7 +3152,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3132,7 +3168,7 @@
         <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3147,7 +3183,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3163,7 +3199,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3178,7 +3214,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3191,10 +3227,10 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G72" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3209,7 +3245,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3222,10 +3258,10 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3240,7 +3276,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3257,7 +3293,7 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3272,23 +3308,23 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75">
+        <f>ROW()</f>
+        <v>75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" t="s">
         <v>101</v>
-      </c>
-      <c r="C75">
-        <f>ROW()</f>
-        <v>75</v>
-      </c>
-      <c r="D75" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" t="s">
-        <v>13</v>
-      </c>
-      <c r="G75" t="s">
-        <v>95</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3303,7 +3339,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3320,7 +3356,7 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3335,7 +3371,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3352,7 +3388,7 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3367,7 +3403,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3384,10 +3420,10 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -3398,7 +3434,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3414,7 +3450,7 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3429,7 +3465,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3445,7 +3481,7 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3460,7 +3496,7 @@
         <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3475,10 +3511,10 @@
         <v>[Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G81" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3493,7 +3529,7 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3511,7 +3547,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I82" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3526,7 +3562,7 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -3544,7 +3580,7 @@
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I83" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3559,7 +3595,7 @@
         <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3574,10 +3610,10 @@
         <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G84" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I84" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3609,17 +3645,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
newer version of spreadsheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19304"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="124">
   <si>
     <t>Act or Con</t>
   </si>
@@ -141,7 +141,7 @@
     <t>[Contour Maps]</t>
   </si>
   <si>
-    <t>Partial derivatives depend on the value(s) of what is held constant</t>
+    <t>The value of a partial derivative depend on the value(s) of what is held constant</t>
   </si>
   <si>
     <t>A partial derivative can be expressed in terms of other partial derivatives</t>
@@ -315,7 +315,7 @@
     <t>Visualizing Gradient</t>
   </si>
   <si>
-    <t>[Kinesthetic, Vector Field Map, Contour Map]</t>
+    <t>[Kinesthetic, Vector Field Map, Contour Maps]</t>
   </si>
   <si>
     <t>Visualizing Divergence</t>
@@ -351,7 +351,7 @@
     <t>The derivative can have a physical interpretation</t>
   </si>
   <si>
-    <t>Partial derivatives depend on what you hold constant</t>
+    <t>Partial derivatives depend on (are defined by?) what you hold constant</t>
   </si>
   <si>
     <t>Partial derivatives are coefficients in a differentials equation</t>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Partial Derivative Machine Derivatives</t>
+  </si>
+  <si>
+    <t>[partial f/partial x rightarrow partial f/partial x fixing y, picture of PDM, data table (pic)]</t>
+  </si>
+  <si>
+    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
   </si>
   <si>
     <t>Chain Rules</t>
@@ -977,8 +983,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="I40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1650,7 +1656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="31.5">
+    <row r="22" spans="1:11" ht="47.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1675,7 +1681,7 @@
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Partial derivatives depend on the value(s) of what is held constant. It is quite a long descrption!</v>
+        <v>This is the long description for The value of a partial derivative depend on the value(s) of what is held constant. It is quite a long descrption!</v>
       </c>
       <c r="K22" t="s">
         <v>15</v>
@@ -2013,7 +2019,7 @@
       </c>
       <c r="E33" t="str">
         <f>"["&amp;B19&amp;", "&amp;B20&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, Partial derivatives depend on the value(s) of what is held constant]</v>
+        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depend on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
         <v>52</v>
@@ -2434,7 +2440,7 @@
       </c>
       <c r="D47" t="str">
         <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[Derivatives can be found while holding some variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, Partial derivatives depend on the value(s) of what is held constant]</v>
+        <v>[Derivatives can be found while holding some variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, The value of a partial derivative depend on the value(s) of what is held constant]</v>
       </c>
       <c r="E47" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
@@ -3347,7 +3353,7 @@
       </c>
       <c r="D76" t="str">
         <f>"["&amp;B$18&amp;","&amp;B$22&amp;"]"</f>
-        <v>[Derivatives can be found while holding some variables constant,Partial derivatives depend on the value(s) of what is held constant]</v>
+        <v>[Derivatives can be found while holding some variables constant,The value of a partial derivative depend on the value(s) of what is held constant]</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -3360,7 +3366,7 @@
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>This is the long description for Partial derivatives depend on what you hold constant. It is quite a long descrption!</v>
+        <v>This is the long description for Partial derivatives depend on (are defined by?) what you hold constant. It is quite a long descrption!</v>
       </c>
       <c r="K76" t="s">
         <v>15</v>
@@ -3570,21 +3576,20 @@
       </c>
       <c r="D83" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding some variables constant, Partial derivatives depend on the value(s) of what is held constant]</v>
+        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding some variables constant, The value of a partial derivative depend on the value(s) of what is held constant]</v>
       </c>
       <c r="E83" t="str">
         <f>"["&amp;B74&amp;", "&amp;B75&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[There might be experimental limits to how 'small' you can get, The derivative can have a physical interpretation, Partial derivatives depend on what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
+        <v>[There might be experimental limits to how 'small' you can get, The derivative can have a physical interpretation, Partial derivatives depend on (are defined by?) what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="G83" t="s">
         <v>101</v>
       </c>
-      <c r="I83" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Partial Derivative Machine Derivatives. It is quite a long descrption!</v>
+      <c r="I83" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="K83" t="s">
         <v>15</v>
@@ -3595,7 +3600,7 @@
         <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3603,14 +3608,14 @@
       </c>
       <c r="D84" t="str">
         <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding some variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives depend on what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
+        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding some variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives depend on (are defined by?) what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="E84" t="str">
         <f>"["&amp;B78&amp;", "&amp;B79&amp;", "&amp;B80&amp;"]"</f>
         <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G84" t="s">
         <v>101</v>
@@ -3645,17 +3650,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sketches of how to reorganize things a bit
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19304"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19310"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="126">
   <si>
     <t>Act or Con</t>
   </si>
@@ -381,7 +381,13 @@
     <t>[partial f/partial x rightarrow partial f/partial x fixing y, picture of PDM, data table (pic)]</t>
   </si>
   <si>
+    <t>pdm.jpg</t>
+  </si>
+  <si>
     <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>eefixme</t>
   </si>
   <si>
     <t>Chain Rules</t>
@@ -983,8 +989,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <pane ySplit="1" topLeftCell="E52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -3588,8 +3594,14 @@
       <c r="G83" t="s">
         <v>101</v>
       </c>
+      <c r="H83" t="s">
+        <v>118</v>
+      </c>
       <c r="I83" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="J83" t="s">
+        <v>120</v>
       </c>
       <c r="K83" t="s">
         <v>15</v>
@@ -3600,7 +3612,7 @@
         <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3615,7 +3627,7 @@
         <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G84" t="s">
         <v>101</v>
@@ -3650,17 +3662,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various small and big changes
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="133">
   <si>
     <t>Act or Con</t>
   </si>
@@ -123,7 +123,7 @@
     <t>"With respect to what" matters</t>
   </si>
   <si>
-    <t>Derivatives can be found while holding some variables constant</t>
+    <t>Derivatives can be found while holding one or more variables constant</t>
   </si>
   <si>
     <t>MTH 254</t>
@@ -141,7 +141,7 @@
     <t>[Contour Maps]</t>
   </si>
   <si>
-    <t>The value of a partial derivative depend on the value(s) of what is held constant</t>
+    <t>The value of a partial derivative depends on the value(s) of what is held constant</t>
   </si>
   <si>
     <t>A partial derivative can be expressed in terms of other partial derivatives</t>
@@ -324,46 +324,61 @@
     <t>Visualizing Curl</t>
   </si>
   <si>
-    <t>Differentials are small changes / differences</t>
+    <t>Differentials are small changes or differences</t>
+  </si>
+  <si>
+    <t>[df, graph???]</t>
+  </si>
+  <si>
+    <t>PH 423</t>
+  </si>
+  <si>
+    <t>diffgraph.jpg</t>
+  </si>
+  <si>
+    <t>Equations can be 'zapped with d' to relate differentials</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Individual differentials can be manipulated algebraically</t>
+  </si>
+  <si>
+    <t>Total differentials are linear</t>
   </si>
   <si>
     <t>[df]</t>
   </si>
   <si>
-    <t>PH 423</t>
-  </si>
-  <si>
-    <t>Equations can be 'zapped with d' to relate differentials</t>
-  </si>
-  <si>
-    <t>Individual differentials can be manipulated algebraically</t>
-  </si>
-  <si>
-    <t>Total differentials are linear</t>
-  </si>
-  <si>
     <t>Differentials are small chunks</t>
   </si>
   <si>
-    <t>There might be experimental limits to how 'small' you can get</t>
-  </si>
-  <si>
-    <t>The derivative can have a physical interpretation</t>
-  </si>
-  <si>
-    <t>Partial derivatives depend on (are defined by?) what you hold constant</t>
+    <t>There are experimental limits to how \textit{small} of a change can be measured</t>
+  </si>
+  <si>
+    <t>The derivative can be interpreted physically</t>
+  </si>
+  <si>
+    <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
+  </si>
+  <si>
+    <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
   </si>
   <si>
     <t>Partial derivatives are coefficients in a differentials equation</t>
   </si>
   <si>
-    <t>You can flip a partial derivative</t>
+    <t>$df = \left(\frac{\partial f}{\partial x}\right)_y dx + \left(\frac{\partial f}{\partial y}\right)_x dy$</t>
+  </si>
+  <si>
+    <t>You can flip a partial derivative if the same variable(s) are constant</t>
   </si>
   <si>
     <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
   </si>
   <si>
-    <t>There might be experimental limits on what quantities you can measure</t>
+    <t>There might be experimental limits on which quantities you can measure</t>
   </si>
   <si>
     <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
@@ -372,13 +387,16 @@
     <t>Zapping with d</t>
   </si>
   <si>
+    <t>LPsmall.jpg</t>
+  </si>
+  <si>
     <t>Energy and Integrals</t>
   </si>
   <si>
     <t>Partial Derivative Machine Derivatives</t>
   </si>
   <si>
-    <t>[partial f/partial x rightarrow partial f/partial x fixing y, picture of PDM, data table (pic)]</t>
+    <t>[$\frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$, picture of PDM, extable.jpg]</t>
   </si>
   <si>
     <t>pdm.jpg</t>
@@ -394,6 +412,9 @@
   </si>
   <si>
     <t>[partial f/partial x fixing y]</t>
+  </si>
+  <si>
+    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
   </si>
   <si>
     <t>$\frac{\partial f}{\partial x}$</t>
@@ -989,8 +1010,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="E52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
+      <pane ySplit="1" topLeftCell="E59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1066,8 +1087,8 @@
         <v>14</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>"This is the long description for " &amp;B2 &amp;". It is quite a long descrption!"</f>
-        <v>This is the long description for Difference / Change. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B2 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Difference / Change. It is quite a long description!</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -1097,8 +1118,8 @@
         <v>14</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I84" si="0">"This is the long description for " &amp;B3 &amp;". It is quite a long descrption!"</f>
-        <v>This is the long description for How much $f$ changes as $x$ changes. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B3 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for How much $f$ changes as $x$ changes. It is quite a long description!</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -1128,8 +1149,8 @@
         <v>14</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>"This is the long description for " &amp;B4 &amp;". It is quite a long descrption!"</f>
-        <v>This is the long description for The derivative is a ratio of small changes. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B4 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is a ratio of small changes. It is quite a long description!</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -1159,8 +1180,8 @@
         <v>14</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative can be approximated by the slope of a secant line. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B5 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative can be approximated by the slope of a secant line. It is quite a long description!</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
@@ -1190,8 +1211,8 @@
         <v>14</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative is the slope of a tangent line. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B6 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is the slope of a tangent line. It is quite a long description!</v>
       </c>
       <c r="K6" t="s">
         <v>15</v>
@@ -1221,8 +1242,8 @@
         <v>14</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative is a limit. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B7 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is a limit. It is quite a long description!</v>
       </c>
       <c r="K7" t="s">
         <v>15</v>
@@ -1252,8 +1273,8 @@
         <v>14</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative can be a function. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B8 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative can be a function. It is quite a long description!</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
@@ -1283,8 +1304,8 @@
         <v>14</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative of a constant is zero. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B9 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative of a constant is zero. It is quite a long description!</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
@@ -1314,8 +1335,8 @@
         <v>14</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative is a linear function. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B10 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is a linear function. It is quite a long description!</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
@@ -1345,8 +1366,8 @@
         <v>14</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Power law. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B11 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Power law. It is quite a long description!</v>
       </c>
       <c r="K11" t="s">
         <v>15</v>
@@ -1376,8 +1397,8 @@
         <v>14</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative at a cusp is undefined. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B12 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative at a cusp is undefined. It is quite a long description!</v>
       </c>
       <c r="K12" t="s">
         <v>15</v>
@@ -1407,8 +1428,8 @@
         <v>14</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Variables can be held constant. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B13 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Variables can be held constant. It is quite a long description!</v>
       </c>
       <c r="K13" t="s">
         <v>15</v>
@@ -1438,8 +1459,8 @@
         <v>14</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Product rule. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B14 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Product rule. It is quite a long description!</v>
       </c>
       <c r="K14" t="s">
         <v>15</v>
@@ -1469,8 +1490,8 @@
         <v>14</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Single variable chain rule. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B15 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Single variable chain rule. It is quite a long description!</v>
       </c>
       <c r="K15" t="s">
         <v>15</v>
@@ -1530,14 +1551,14 @@
         <v>14</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for "With respect to what" matters. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B17 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for "With respect to what" matters. It is quite a long description!</v>
       </c>
       <c r="K17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="31.5">
+    <row r="18" spans="1:11" ht="47.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1562,8 +1583,8 @@
         <v>33</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Derivatives can be found while holding some variables constant. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B18 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Derivatives can be found while holding one or more variables constant. It is quite a long description!</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
@@ -1593,8 +1614,8 @@
         <v>33</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for There is a  partial derivative in every direction at any point. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B19 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for There is a  partial derivative in every direction at any point. It is quite a long description!</v>
       </c>
       <c r="K19" t="s">
         <v>15</v>
@@ -1624,8 +1645,8 @@
         <v>33</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for There is a tangent line in every direction at every point. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B20 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for There is a tangent line in every direction at every point. It is quite a long description!</v>
       </c>
       <c r="K20" t="s">
         <v>15</v>
@@ -1655,8 +1676,8 @@
         <v>33</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative is related to the density of contour lines. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B21 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is related to the density of contour lines. It is quite a long description!</v>
       </c>
       <c r="K21" t="s">
         <v>15</v>
@@ -1686,8 +1707,8 @@
         <v>33</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The value of a partial derivative depend on the value(s) of what is held constant. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B22 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The value of a partial derivative depends on the value(s) of what is held constant. It is quite a long description!</v>
       </c>
       <c r="K22" t="s">
         <v>15</v>
@@ -1718,8 +1739,8 @@
         <v>33</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for A partial derivative can be expressed in terms of other partial derivatives. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B23 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for A partial derivative can be expressed in terms of other partial derivatives. It is quite a long description!</v>
       </c>
       <c r="K23" t="s">
         <v>15</v>
@@ -1749,8 +1770,8 @@
         <v>33</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient is a vector. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B24 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is a vector. It is quite a long description!</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="47.25">
@@ -1778,8 +1799,8 @@
         <v>33</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The magnitude of the gradient is the value of the slope in the steepest direction. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B25 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The magnitude of the gradient is the value of the slope in the steepest direction. It is quite a long description!</v>
       </c>
       <c r="K25" t="s">
         <v>15</v>
@@ -1809,8 +1830,8 @@
         <v>33</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient is perpendicular to contour lines. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B26 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is perpendicular to contour lines. It is quite a long description!</v>
       </c>
       <c r="K26" t="s">
         <v>15</v>
@@ -1841,8 +1862,8 @@
         <v>33</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for All partial derivatives can be found as a slope of a tangent plane. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B27 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for All partial derivatives can be found as a slope of a tangent plane. It is quite a long description!</v>
       </c>
       <c r="K27" t="s">
         <v>15</v>
@@ -1872,8 +1893,8 @@
         <v>33</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The components of the gradient are partial derivatives. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The components of the gradient are partial derivatives. It is quite a long description!</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
@@ -1903,8 +1924,8 @@
         <v>33</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative is local quantity. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B29 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is local quantity. It is quite a long description!</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
@@ -1934,8 +1955,8 @@
         <v>33</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Partial derivatives are functions. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B30 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Partial derivatives are functions. It is quite a long description!</v>
       </c>
       <c r="K30" t="s">
         <v>15</v>
@@ -1965,8 +1986,8 @@
         <v>33</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient is a function. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B31 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is a function. It is quite a long description!</v>
       </c>
       <c r="K31" t="s">
         <v>15</v>
@@ -1989,7 +2010,7 @@
       </c>
       <c r="E32" t="str">
         <f>"["&amp;B18&amp;"]"</f>
-        <v>[Derivatives can be found while holding some variables constant]</v>
+        <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
         <v>37</v>
@@ -1998,8 +2019,8 @@
         <v>33</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The heater II. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B32 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The heater II. It is quite a long description!</v>
       </c>
       <c r="J32" t="s">
         <v>50</v>
@@ -2025,7 +2046,7 @@
       </c>
       <c r="E33" t="str">
         <f>"["&amp;B19&amp;", "&amp;B20&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depend on the value(s) of what is held constant]</v>
+        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
         <v>52</v>
@@ -2034,8 +2055,8 @@
         <v>33</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The hot plate. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B33 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The hot plate. It is quite a long description!</v>
       </c>
       <c r="J33" t="s">
         <v>53</v>
@@ -2070,8 +2091,8 @@
         <v>33</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Chain Rule. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B34 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Chain Rule. It is quite a long description!</v>
       </c>
       <c r="J34" t="s">
         <v>56</v>
@@ -2105,8 +2126,8 @@
         <v>33</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Chain Rule Measurements. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B35 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Chain Rule Measurements. It is quite a long description!</v>
       </c>
       <c r="J35" t="s">
         <v>59</v>
@@ -2128,7 +2149,7 @@
       </c>
       <c r="D36" t="str">
         <f>"["&amp;B6&amp;", "&amp;B18&amp;", "&amp;B19&amp;", "&amp;B20&amp;"]"</f>
-        <v>[The derivative is the slope of a tangent line, Derivatives can be found while holding some variables constant, There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point]</v>
+        <v>[The derivative is the slope of a tangent line, Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point]</v>
       </c>
       <c r="E36" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
@@ -2141,8 +2162,8 @@
         <v>33</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The Hillside. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B36 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The Hillside. It is quite a long description!</v>
       </c>
       <c r="K36" t="s">
         <v>15</v>
@@ -2174,8 +2195,8 @@
         <v>33</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Directional Derivatives. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B37 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Directional Derivatives. It is quite a long description!</v>
       </c>
       <c r="J37" t="s">
         <v>63</v>
@@ -2208,8 +2229,8 @@
         <v>65</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. . It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B38 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. . It is quite a long description!</v>
       </c>
       <c r="K38" t="s">
         <v>15</v>
@@ -2239,8 +2260,8 @@
         <v>67</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The magnitude of $d\vec r$ is the length of a small step along a path. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B39 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The magnitude of $d\vec r$ is the length of a small step along a path. It is quite a long description!</v>
       </c>
       <c r="K39" t="s">
         <v>15</v>
@@ -2270,8 +2291,8 @@
         <v>67</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The direction of $d\vec r$ is ? . It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B40 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The direction of $d\vec r$ is ? . It is quite a long description!</v>
       </c>
       <c r="K40" t="s">
         <v>15</v>
@@ -2301,8 +2322,8 @@
         <v>65</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient can tell you a small change in a function in any direction (differentials edition). It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B41 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient can tell you a small change in a function in any direction (differentials edition). It is quite a long description!</v>
       </c>
       <c r="K41" t="s">
         <v>15</v>
@@ -2326,8 +2347,8 @@
         <v>13</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence is a scalar field. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B42 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a scalar field. It is quite a long description!</v>
       </c>
       <c r="K42" t="s">
         <v>15</v>
@@ -2446,7 +2467,7 @@
       </c>
       <c r="D47" t="str">
         <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[Derivatives can be found while holding some variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, The value of a partial derivative depend on the value(s) of what is held constant]</v>
+        <v>[Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="E47" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
@@ -2524,8 +2545,8 @@
         <v>67</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Differential form of $\vec r$ in spherical and cylindrical coordinates. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B49 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differential form of $\vec r$ in spherical and cylindrical coordinates. It is quite a long description!</v>
       </c>
       <c r="K49" t="s">
         <v>15</v>
@@ -2555,8 +2576,8 @@
         <v>67</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient's dimension is the same as real space. The gradient lives in the domain. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B50 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient's dimension is the same as real space. The gradient lives in the domain. It is quite a long description!</v>
       </c>
       <c r="K50" t="s">
         <v>15</v>
@@ -2587,8 +2608,8 @@
         <v>67</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The gradient is a local quantity. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B51 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is a local quantity. It is quite a long description!</v>
       </c>
       <c r="K51" t="s">
         <v>15</v>
@@ -2618,8 +2639,8 @@
         <v>67</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The electric field is the negative gradient of the electric potential. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B52 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The electric field is the negative gradient of the electric potential. It is quite a long description!</v>
       </c>
       <c r="K52" t="s">
         <v>15</v>
@@ -2649,8 +2670,8 @@
         <v>67</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence is related to the total flux through a closed surface. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B53 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is related to the total flux through a closed surface. It is quite a long description!</v>
       </c>
       <c r="K53" t="s">
         <v>15</v>
@@ -2680,8 +2701,8 @@
         <v>67</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence is a function. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B54 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a function. It is quite a long description!</v>
       </c>
       <c r="K54" t="s">
         <v>15</v>
@@ -2712,8 +2733,8 @@
         <v>67</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence is a local quantity. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B55 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a local quantity. It is quite a long description!</v>
       </c>
       <c r="K55" t="s">
         <v>15</v>
@@ -2743,8 +2764,8 @@
         <v>67</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence of the electric field is equal to. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B56 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the electric field is equal to. It is quite a long description!</v>
       </c>
       <c r="K56" t="s">
         <v>15</v>
@@ -2774,8 +2795,8 @@
         <v>67</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence of the magnetic field is zero. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B57 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the magnetic field is zero. It is quite a long description!</v>
       </c>
       <c r="K57" t="s">
         <v>15</v>
@@ -2805,8 +2826,8 @@
         <v>67</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The curl is related to the line integral around a closed loop. ("circulation"). It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B58 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl is related to the line integral around a closed loop. ("circulation"). It is quite a long description!</v>
       </c>
       <c r="K58" t="s">
         <v>15</v>
@@ -2836,8 +2857,8 @@
         <v>67</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for the curl is a (vector) function. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B59 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for the curl is a (vector) function. It is quite a long description!</v>
       </c>
       <c r="K59" t="s">
         <v>15</v>
@@ -2868,8 +2889,8 @@
         <v>67</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The curl is a local quantity. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B60 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl is a local quantity. It is quite a long description!</v>
       </c>
       <c r="K60" t="s">
         <v>15</v>
@@ -2899,8 +2920,8 @@
         <v>67</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The magnetic field is equal to the curl of the magnetic vector potential. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B61 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The magnetic field is equal to the curl of the magnetic vector potential. It is quite a long description!</v>
       </c>
       <c r="K61" t="s">
         <v>15</v>
@@ -2930,8 +2951,8 @@
         <v>67</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The curl of the electric field is zero in electrostatics. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B62 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl of the electric field is zero in electrostatics. It is quite a long description!</v>
       </c>
       <c r="K62" t="s">
         <v>15</v>
@@ -2961,8 +2982,8 @@
         <v>67</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The divergence of the curl is equal to mu times the current in magneto-statics. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B63 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the curl is equal to mu times the current in magneto-statics. It is quite a long description!</v>
       </c>
       <c r="K63" t="s">
         <v>15</v>
@@ -2994,8 +3015,8 @@
         <v>67</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Vector Differentials. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B64 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Vector Differentials. It is quite a long description!</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
@@ -3025,8 +3046,8 @@
         <v>67</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Acting out the Gradient. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B65 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Acting out the Gradient. It is quite a long description!</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
@@ -3058,8 +3079,8 @@
         <v>67</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Visualizing Gradient. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B66 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Visualizing Gradient. It is quite a long description!</v>
       </c>
       <c r="K66" t="s">
         <v>15</v>
@@ -3089,8 +3110,8 @@
         <v>67</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Visualizing Divergence. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B67 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Visualizing Divergence. It is quite a long description!</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
@@ -3120,8 +3141,8 @@
         <v>67</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Visualizing Curl. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B68 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Visualizing Curl. It is quite a long description!</v>
       </c>
       <c r="K68" t="s">
         <v>15</v>
@@ -3151,9 +3172,12 @@
       <c r="G69" t="s">
         <v>101</v>
       </c>
+      <c r="H69" t="s">
+        <v>102</v>
+      </c>
       <c r="I69" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Differentials are small changes / differences. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B69 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differentials are small changes or differences. It is quite a long description!</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>
@@ -3164,7 +3188,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3177,14 +3201,14 @@
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="G70" t="s">
         <v>101</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Equations can be 'zapped with d' to relate differentials. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B70 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Equations can be 'zapped with d' to relate differentials. It is quite a long description!</v>
       </c>
       <c r="K70" t="s">
         <v>15</v>
@@ -3195,7 +3219,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3214,8 +3238,8 @@
         <v>101</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Individual differentials can be manipulated algebraically. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B71 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Individual differentials can be manipulated algebraically. It is quite a long description!</v>
       </c>
       <c r="K71" t="s">
         <v>15</v>
@@ -3226,7 +3250,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3239,14 +3263,14 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G72" t="s">
         <v>101</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Total differentials are linear. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B72 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Total differentials are linear. It is quite a long description!</v>
       </c>
       <c r="K72" t="s">
         <v>15</v>
@@ -3257,7 +3281,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3270,25 +3294,25 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G73" t="s">
         <v>101</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Differentials are small chunks. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B73 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differentials are small chunks. It is quite a long description!</v>
       </c>
       <c r="K73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="31.5">
+    <row r="74" spans="1:11" ht="47.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3308,8 +3332,8 @@
         <v>101</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for There might be experimental limits to how 'small' you can get. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B74 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for There are experimental limits to how \textit{small} of a change can be measured. It is quite a long description!</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
@@ -3320,7 +3344,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3339,19 +3363,19 @@
         <v>101</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for The derivative can have a physical interpretation. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B75 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative can be interpreted physically. It is quite a long description!</v>
       </c>
       <c r="K75" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="31.5">
+    <row r="76" spans="1:11" ht="78.75">
       <c r="A76" t="s">
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3359,7 +3383,7 @@
       </c>
       <c r="D76" t="str">
         <f>"["&amp;B$18&amp;","&amp;B$22&amp;"]"</f>
-        <v>[Derivatives can be found while holding some variables constant,The value of a partial derivative depend on the value(s) of what is held constant]</v>
+        <v>[Derivatives can be found while holding one or more variables constant,The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -3370,9 +3394,12 @@
       <c r="G76" t="s">
         <v>101</v>
       </c>
+      <c r="H76" t="s">
+        <v>112</v>
+      </c>
       <c r="I76" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Partial derivatives depend on (are defined by?) what you hold constant. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B76 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative. It is quite a long description!</v>
       </c>
       <c r="K76" t="s">
         <v>15</v>
@@ -3383,7 +3410,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3391,7 +3418,7 @@
       </c>
       <c r="D77" t="str">
         <f>"["&amp;B$4&amp;","&amp;B$69&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes,Differentials are small changes / differences]</v>
+        <v>[The derivative is a ratio of small changes,Differentials are small changes or differences]</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -3402,9 +3429,12 @@
       <c r="G77" t="s">
         <v>101</v>
       </c>
+      <c r="H77" t="s">
+        <v>114</v>
+      </c>
       <c r="I77" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Partial derivatives are coefficients in a differentials equation. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B77 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Partial derivatives are coefficients in a differentials equation. It is quite a long description!</v>
       </c>
       <c r="K77" t="s">
         <v>15</v>
@@ -3415,7 +3445,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3423,7 +3453,7 @@
       </c>
       <c r="D78" t="str">
         <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
-        <v>[You can flip a derivative, Derivatives can be found while holding some variables constant]</v>
+        <v>[You can flip a derivative, Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -3435,7 +3465,7 @@
         <v>101</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -3446,7 +3476,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3465,8 +3495,8 @@
         <v>101</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for There might be experimental limits on what quantities you can measure. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B79 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for There might be experimental limits on which quantities you can measure. It is quite a long description!</v>
       </c>
       <c r="K79" t="s">
         <v>15</v>
@@ -3477,7 +3507,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3496,8 +3526,8 @@
         <v>101</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B80 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long description!</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
@@ -3508,7 +3538,7 @@
         <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3520,17 +3550,20 @@
       </c>
       <c r="E81" t="str">
         <f>"["&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B72&amp;"]"</f>
-        <v>[Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
+        <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G81" t="s">
         <v>101</v>
       </c>
+      <c r="H81" t="s">
+        <v>120</v>
+      </c>
       <c r="I81" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Zapping with d. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B81 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Zapping with d. It is quite a long description!</v>
       </c>
       <c r="K81" t="s">
         <v>15</v>
@@ -3541,7 +3574,7 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3549,7 +3582,7 @@
       </c>
       <c r="D82" t="str">
         <f>"["&amp;B69&amp;", "&amp;B71&amp;"]"</f>
-        <v>[Differentials are small changes / differences, Individual differentials can be manipulated algebraically]</v>
+        <v>[Differentials are small changes or differences, Individual differentials can be manipulated algebraically]</v>
       </c>
       <c r="E82" t="str">
         <f>"["&amp;B73&amp;"]"</f>
@@ -3562,8 +3595,8 @@
         <v>101</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Energy and Integrals. It is quite a long descrption!</v>
+        <f>"This is the long description for " &amp;B82 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Energy and Integrals. It is quite a long description!</v>
       </c>
       <c r="K82" t="s">
         <v>15</v>
@@ -3574,45 +3607,45 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
         <v>83</v>
       </c>
       <c r="D83" t="str">
-        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding some variables constant, The value of a partial derivative depend on the value(s) of what is held constant]</v>
+        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;", "&amp;B69&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding one or more variables constant, The value of a partial derivative depends on the value(s) of what is held constant, Differentials are small changes or differences]</v>
       </c>
       <c r="E83" t="str">
         <f>"["&amp;B74&amp;", "&amp;B75&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[There might be experimental limits to how 'small' you can get, The derivative can have a physical interpretation, Partial derivatives depend on (are defined by?) what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
+        <v>[There are experimental limits to how \textit{small} of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="G83" t="s">
         <v>101</v>
       </c>
       <c r="H83" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J83" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K83" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="31.5">
+    <row r="84" spans="1:11" ht="94.5">
       <c r="A84" t="s">
         <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3620,21 +3653,23 @@
       </c>
       <c r="D84" t="str">
         <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding some variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes / differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives depend on (are defined by?) what you hold constant, Partial derivatives are coefficients in a differentials equation]</v>
+        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding one or more variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="E84" t="str">
         <f>"["&amp;B78&amp;", "&amp;B79&amp;", "&amp;B80&amp;"]"</f>
-        <v>[You can flip a partial derivative, There might be experimental limits on what quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
+        <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G84" t="s">
         <v>101</v>
       </c>
-      <c r="I84" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>This is the long description for Chain Rules. It is quite a long descrption!</v>
+      <c r="H84" t="s">
+        <v>124</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="K84" t="s">
         <v>15</v>
@@ -3662,17 +3697,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix spacing, I hope
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="134">
   <si>
     <t>Act or Con</t>
   </si>
@@ -399,19 +399,22 @@
     <t>Partial Derivative Machine Derivatives</t>
   </si>
   <si>
-    <t>[$\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$, picture of PDM, Table]</t>
+    <t>[$\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$, pdm.jpg, Table]</t>
+  </si>
+  <si>
+    <t>PDMD.jpg</t>
+  </si>
+  <si>
+    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>eefixme</t>
+  </si>
+  <si>
+    <t>Chain Rules</t>
   </si>
   <si>
     <t>pdm.jpg</t>
-  </si>
-  <si>
-    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
-    <t>eefixme</t>
-  </si>
-  <si>
-    <t>Chain Rules</t>
   </si>
   <si>
     <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
@@ -1010,8 +1013,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="D64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+      <pane ySplit="1" topLeftCell="D79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -3665,10 +3668,10 @@
         <v>101</v>
       </c>
       <c r="H84" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K84" t="s">
         <v>15</v>
@@ -3696,17 +3699,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit title and new spreadsheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6700" yWindow="-23540" windowWidth="19200" windowHeight="22520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6700" yWindow="-23540" windowWidth="19200" windowHeight="22520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="137">
   <si>
     <t>Act or Con</t>
   </si>
@@ -162,6 +162,264 @@
     <t>The components of the gradient are partial derivatives</t>
   </si>
   <si>
+    <t>This is the long description for The components of the gradient are partial derivatives. It is quite a long description!</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>The heater II</t>
+  </si>
+  <si>
+    <t>mvheater2</t>
+  </si>
+  <si>
+    <t>The hot plate</t>
+  </si>
+  <si>
+    <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
+  </si>
+  <si>
+    <t>mvhotplate</t>
+  </si>
+  <si>
+    <t>Chain Rule</t>
+  </si>
+  <si>
+    <t>[partial f/partial x]</t>
+  </si>
+  <si>
+    <t>mvchain</t>
+  </si>
+  <si>
+    <t>The Hillside</t>
+  </si>
+  <si>
+    <t>[partial f/partial x, Inclinometer]</t>
+  </si>
+  <si>
+    <t>Directional Derivatives</t>
+  </si>
+  <si>
+    <t>[partial f/partial x, Inclinometer, Del f]</t>
+  </si>
+  <si>
+    <t>mvdderiv</t>
+  </si>
+  <si>
+    <t>The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. </t>
+  </si>
+  <si>
+    <t>MTH 255</t>
+  </si>
+  <si>
+    <t>The magnitude of $d\vec r$ is the length of a small step along a path</t>
+  </si>
+  <si>
+    <t>PH 422</t>
+  </si>
+  <si>
+    <t>The direction of $d\vec r$ is ? </t>
+  </si>
+  <si>
+    <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
+  </si>
+  <si>
+    <t>The divergence is a scalar field</t>
+  </si>
+  <si>
+    <t>concept</t>
+  </si>
+  <si>
+    <t>The Hill</t>
+  </si>
+  <si>
+    <t>[Contour Maps, Del dot f]</t>
+  </si>
+  <si>
+    <t>vchill</t>
+  </si>
+  <si>
+    <t>The Valley</t>
+  </si>
+  <si>
+    <t>vcvalley</t>
+  </si>
+  <si>
+    <t>Differential form of $\vec r$ in spherical and cylindrical coordinates</t>
+  </si>
+  <si>
+    <t>The gradient's dimension is the same as real space. The gradient lives in the domain</t>
+  </si>
+  <si>
+    <t>The gradient is a local quantity</t>
+  </si>
+  <si>
+    <t>The electric field is the negative gradient of the electric potential</t>
+  </si>
+  <si>
+    <t>The divergence is related to the total flux through a closed surface</t>
+  </si>
+  <si>
+    <t>The divergence is a function</t>
+  </si>
+  <si>
+    <t>The divergence is a local quantity</t>
+  </si>
+  <si>
+    <t>The divergence of the electric field is equal to</t>
+  </si>
+  <si>
+    <t>The divergence of the magnetic field is zero</t>
+  </si>
+  <si>
+    <t>The curl is related to the line integral around a closed loop. ("circulation")</t>
+  </si>
+  <si>
+    <t>the curl is a (vector) function</t>
+  </si>
+  <si>
+    <t>The curl is a local quantity</t>
+  </si>
+  <si>
+    <t>The magnetic field is equal to the curl of the magnetic vector potential</t>
+  </si>
+  <si>
+    <t>The curl of the electric field is zero in electrostatics</t>
+  </si>
+  <si>
+    <t>The divergence of the curl is equal to mu times the current in magneto-statics</t>
+  </si>
+  <si>
+    <t>Vector Differentials</t>
+  </si>
+  <si>
+    <t>[df, 3D plots]</t>
+  </si>
+  <si>
+    <t>Acting out the Gradient</t>
+  </si>
+  <si>
+    <t>Visualizing Gradient</t>
+  </si>
+  <si>
+    <t>[Kinesthetic, Vector Field Map, Contour Maps]</t>
+  </si>
+  <si>
+    <t>Visualizing Divergence</t>
+  </si>
+  <si>
+    <t>Visualizing Curl</t>
+  </si>
+  <si>
+    <t>Differentials are small changes or differences</t>
+  </si>
+  <si>
+    <t>[df]</t>
+  </si>
+  <si>
+    <t>PH 423</t>
+  </si>
+  <si>
+    <t>differentials.jpg</t>
+  </si>
+  <si>
+    <t>One typical notation used for derivatives is Leibniz notation ($e.g.,$ $df/dx$).  Physicists often think of the $df$ and $dx$ as distinct quantities (``differentials'') that can be measured, calculated, and manipulated independent of one another.  In particular, a differential can be thought of as the (small) change in a quantity when a small change is made to a physical system.  A diffferential can also be thought of as the difference between the values of a quantity between two different (nearby) physical states.  This line of thinking is also valuable for thinking about integration in physical situations.</t>
+  </si>
+  <si>
+    <t>Equations can be 'zapped with d' to relate differentials</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Individual differentials can be manipulated algebraically</t>
+  </si>
+  <si>
+    <t>Total differentials are linear</t>
+  </si>
+  <si>
+    <t>Differentials are small chunks</t>
+  </si>
+  <si>
+    <t>There are experimental limits to how $small$ of a change can be measured</t>
+  </si>
+  <si>
+    <t>The derivative can be interpreted physically</t>
+  </si>
+  <si>
+    <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
+  </si>
+  <si>
+    <t>[$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$]</t>
+  </si>
+  <si>
+    <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
+  </si>
+  <si>
+    <t>Partial derivatives are coefficients in a differentials equation</t>
+  </si>
+  <si>
+    <t>$df = \left(\frac{\partial f}{\partial x}\right)_y dx + \left(\frac{\partial f}{\partial y}\right)_x dy$</t>
+  </si>
+  <si>
+    <t>You can flip a partial derivative if the same variable(s) are constant</t>
+  </si>
+  <si>
+    <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
+  </si>
+  <si>
+    <t>There might be experimental limits on which quantities you can measure</t>
+  </si>
+  <si>
+    <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
+  </si>
+  <si>
+    <t>Zapping with d</t>
+  </si>
+  <si>
+    <t>LPsmall.jpg</t>
+  </si>
+  <si>
+    <t>Energy and Integrals</t>
+  </si>
+  <si>
+    <t>[PDM, df]</t>
+  </si>
+  <si>
+    <t>Partial Derivative Machine Derivatives</t>
+  </si>
+  <si>
+    <t>[PDM, $\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$,Table]</t>
+  </si>
+  <si>
+    <t>PDMD.jpg</t>
+  </si>
+  <si>
+    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>eefixme</t>
+  </si>
+  <si>
+    <t>Chain Rules</t>
+  </si>
+  <si>
+    <t>pdm.jpg</t>
+  </si>
+  <si>
+    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>$\frac{\partial f}{\partial x}$</t>
+  </si>
+  <si>
+    <t>Contour Maps</t>
+  </si>
+  <si>
+    <t>Inclinometer</t>
+  </si>
+  <si>
     <t>The derivative is local quantity</t>
   </si>
   <si>
@@ -171,262 +429,13 @@
     <t>The gradient is a function</t>
   </si>
   <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>The heater II</t>
-  </si>
-  <si>
-    <t>mvheater2</t>
-  </si>
-  <si>
-    <t>The hot plate</t>
-  </si>
-  <si>
-    <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
-  </si>
-  <si>
-    <t>mvhotplate</t>
-  </si>
-  <si>
-    <t>Chain Rule</t>
-  </si>
-  <si>
-    <t>[partial f/partial x]</t>
-  </si>
-  <si>
-    <t>mvchain</t>
-  </si>
-  <si>
     <t>Chain Rule Measurements</t>
   </si>
   <si>
-    <t>[partial f/partial x, Inclinometer]</t>
-  </si>
-  <si>
     <t>mvpchain</t>
   </si>
   <si>
-    <t>The Hillside</t>
-  </si>
-  <si>
-    <t>Directional Derivatives</t>
-  </si>
-  <si>
-    <t>[partial f/partial x, Inclinometer, Del f]</t>
-  </si>
-  <si>
-    <t>mvdderiv</t>
-  </si>
-  <si>
-    <t>The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. </t>
-  </si>
-  <si>
-    <t>MTH 255</t>
-  </si>
-  <si>
-    <t>The magnitude of $d\vec r$ is the length of a small step along a path</t>
-  </si>
-  <si>
-    <t>PH 422</t>
-  </si>
-  <si>
-    <t>The direction of $d\vec r$ is ? </t>
-  </si>
-  <si>
-    <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
-  </si>
-  <si>
-    <t>The divergence is a scalar field</t>
-  </si>
-  <si>
-    <t>concept</t>
-  </si>
-  <si>
-    <t>The Hill</t>
-  </si>
-  <si>
-    <t>[Contour Maps, Del dot f]</t>
-  </si>
-  <si>
-    <t>vchill</t>
-  </si>
-  <si>
-    <t>The Valley</t>
-  </si>
-  <si>
-    <t>vcvalley</t>
-  </si>
-  <si>
-    <t>Differential form of $\vec r$ in spherical and cylindrical coordinates</t>
-  </si>
-  <si>
-    <t>The gradient's dimension is the same as real space. The gradient lives in the domain</t>
-  </si>
-  <si>
-    <t>The gradient is a local quantity</t>
-  </si>
-  <si>
-    <t>The electric field is the negative gradient of the electric potential</t>
-  </si>
-  <si>
-    <t>The divergence is related to the total flux through a closed surface</t>
-  </si>
-  <si>
-    <t>The divergence is a function</t>
-  </si>
-  <si>
-    <t>The divergence is a local quantity</t>
-  </si>
-  <si>
-    <t>The divergence of the electric field is equal to</t>
-  </si>
-  <si>
-    <t>The divergence of the magnetic field is zero</t>
-  </si>
-  <si>
-    <t>The curl is related to the line integral around a closed loop. ("circulation")</t>
-  </si>
-  <si>
-    <t>the curl is a (vector) function</t>
-  </si>
-  <si>
-    <t>The curl is a local quantity</t>
-  </si>
-  <si>
-    <t>The magnetic field is equal to the curl of the magnetic vector potential</t>
-  </si>
-  <si>
-    <t>The curl of the electric field is zero in electrostatics</t>
-  </si>
-  <si>
-    <t>The divergence of the curl is equal to mu times the current in magneto-statics</t>
-  </si>
-  <si>
-    <t>Vector Differentials</t>
-  </si>
-  <si>
-    <t>[df, 3D plots]</t>
-  </si>
-  <si>
-    <t>Acting out the Gradient</t>
-  </si>
-  <si>
-    <t>Visualizing Gradient</t>
-  </si>
-  <si>
-    <t>[Kinesthetic, Vector Field Map, Contour Maps]</t>
-  </si>
-  <si>
-    <t>Visualizing Divergence</t>
-  </si>
-  <si>
-    <t>Visualizing Curl</t>
-  </si>
-  <si>
-    <t>Differentials are small changes or differences</t>
-  </si>
-  <si>
-    <t>[df, graph???]</t>
-  </si>
-  <si>
-    <t>PH 423</t>
-  </si>
-  <si>
-    <t>differentials.jpg</t>
-  </si>
-  <si>
-    <t>One typical notation used for derivatives is Leibniz notation ($e.g.,$ $df/dx$).  Physicists often think of the $df$ and $dx$ as distinct quantities (``differentials'') that can be measured, calculated, and manipulated independent of one another.  In particular, a differential can be thought of as the (small) change in a quantity when a small change is made to a physical system.  A diffferential can also be thought of as the difference between the values of a quantity between two different (nearby) physical states.  This line of thinking is also valuable for thinking about integration in physical situations.</t>
-  </si>
-  <si>
-    <t>Equations can be 'zapped with d' to relate differentials</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Individual differentials can be manipulated algebraically</t>
-  </si>
-  <si>
-    <t>Total differentials are linear</t>
-  </si>
-  <si>
-    <t>[df]</t>
-  </si>
-  <si>
-    <t>Differentials are small chunks</t>
-  </si>
-  <si>
-    <t>There are experimental limits to how $small$ of a change can be measured</t>
-  </si>
-  <si>
-    <t>The derivative can be interpreted physically</t>
-  </si>
-  <si>
-    <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
-  </si>
-  <si>
-    <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
-  </si>
-  <si>
-    <t>Partial derivatives are coefficients in a differentials equation</t>
-  </si>
-  <si>
-    <t>$df = \left(\frac{\partial f}{\partial x}\right)_y dx + \left(\frac{\partial f}{\partial y}\right)_x dy$</t>
-  </si>
-  <si>
-    <t>You can flip a partial derivative if the same variable(s) are constant</t>
-  </si>
-  <si>
-    <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
-  </si>
-  <si>
-    <t>There might be experimental limits on which quantities you can measure</t>
-  </si>
-  <si>
-    <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
-  </si>
-  <si>
-    <t>Zapping with d</t>
-  </si>
-  <si>
-    <t>LPsmall.jpg</t>
-  </si>
-  <si>
-    <t>Energy and Integrals</t>
-  </si>
-  <si>
-    <t>Partial Derivative Machine Derivatives</t>
-  </si>
-  <si>
-    <t>[PDM, $\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$,Table]</t>
-  </si>
-  <si>
-    <t>PDMD.jpg</t>
-  </si>
-  <si>
-    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
-    <t>eefixme</t>
-  </si>
-  <si>
-    <t>Chain Rules</t>
-  </si>
-  <si>
-    <t>pdm.jpg</t>
-  </si>
-  <si>
-    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
-    <t>$\frac{\partial f}{\partial x}$</t>
-  </si>
-  <si>
-    <t>Contour Maps</t>
-  </si>
-  <si>
-    <t>Inclinometer</t>
+    <t>[df,graph???]</t>
   </si>
 </sst>
 </file>
@@ -494,13 +503,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1348330</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>448733</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -538,13 +547,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>34750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>482600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -582,13 +591,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>34750</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>9380</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -626,13 +635,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>9379</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -670,13 +679,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1969379</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1010,11 +1019,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="C80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I84" sqref="I84"/>
+    <sheetView zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1880,7 +1889,6 @@
         <v>44</v>
       </c>
       <c r="C28">
-        <f>ROW()</f>
         <v>28</v>
       </c>
       <c r="D28" t="s">
@@ -1895,9 +1903,8 @@
       <c r="G28" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="1" t="str">
-        <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The components of the gradient are partial derivatives. It is quite a long description!</v>
+      <c r="I28" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
@@ -1905,128 +1912,140 @@
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <f>ROW()</f>
         <v>29</v>
       </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
+      <c r="D29" t="str">
+        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes, Variables can be held constant, "With respect to what" matters]</v>
+      </c>
+      <c r="E29" t="str">
+        <f>"["&amp;B18&amp;"]"</f>
+        <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="1" t="str">
         <f>"This is the long description for " &amp;B29 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The derivative is local quantity. It is quite a long description!</v>
+        <v>This is the long description for The heater II. It is quite a long description!</v>
+      </c>
+      <c r="J29" t="s">
+        <v>48</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75">
+    <row r="30" spans="1:11" ht="47.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <f>ROW()</f>
         <v>30</v>
       </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
+      <c r="D30" t="str">
+        <f>"["&amp;B6&amp;", "&amp;B8&amp;", "&amp;B12&amp;", "&amp;B17&amp;"]"</f>
+        <v>[The derivative is the slope of a tangent line, The derivative can be a function, The derivative at a cusp is undefined, "With respect to what" matters]</v>
+      </c>
+      <c r="E30" t="str">
+        <f>"["&amp;B19&amp;", "&amp;B20&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
+        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="1" t="str">
         <f>"This is the long description for " &amp;B30 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Partial derivatives are functions. It is quite a long description!</v>
+        <v>This is the long description for The hot plate. It is quite a long description!</v>
+      </c>
+      <c r="J30" t="s">
+        <v>51</v>
       </c>
       <c r="K30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75">
+    <row r="31" spans="1:11" ht="71.25" customHeight="1">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C31">
         <f>ROW()</f>
         <v>31</v>
       </c>
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>13</v>
+      <c r="D31" t="str">
+        <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;", "&amp;B15&amp;"]"</f>
+        <v>[The derivative can be a function, The derivative is a linear function, Variables can be held constant, Product rule, "With respect to what" matters, Single variable chain rule]</v>
+      </c>
+      <c r="E31" t="str">
+        <f>"["&amp;B23&amp;"]"</f>
+        <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s">
         <v>33</v>
       </c>
       <c r="I31" s="1" t="str">
         <f>"This is the long description for " &amp;B31 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The gradient is a function. It is quite a long description!</v>
+        <v>This is the long description for Chain Rule. It is quite a long description!</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
       </c>
       <c r="K31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75">
+    <row r="32" spans="1:11" ht="31.5">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
         <v>32</v>
       </c>
       <c r="D32" t="str">
-        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, Variables can be held constant, "With respect to what" matters]</v>
+        <f>"["&amp;B6&amp;", "&amp;B18&amp;", "&amp;B19&amp;", "&amp;B20&amp;"]"</f>
+        <v>[The derivative is the slope of a tangent line, Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point]</v>
       </c>
       <c r="E32" t="str">
-        <f>"["&amp;B18&amp;"]"</f>
-        <v>[Derivatives can be found while holding one or more variables constant]</v>
+        <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
+        <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
       </c>
       <c r="I32" s="1" t="str">
         <f>"This is the long description for " &amp;B32 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The heater II. It is quite a long description!</v>
-      </c>
-      <c r="J32" t="s">
-        <v>50</v>
+        <v>This is the long description for The Hillside. It is quite a long description!</v>
       </c>
       <c r="K32" t="s">
         <v>15</v>
@@ -2034,939 +2053,927 @@
     </row>
     <row r="33" spans="1:11" ht="47.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
         <v>33</v>
       </c>
       <c r="D33" t="str">
-        <f>"["&amp;B6&amp;", "&amp;B8&amp;", "&amp;B12&amp;", "&amp;B17&amp;"]"</f>
-        <v>[The derivative is the slope of a tangent line, The derivative can be a function, The derivative at a cusp is undefined, "With respect to what" matters]</v>
+        <f>"["&amp;B10&amp;", "&amp;B19&amp;", "&amp;B23&amp;"]"</f>
+        <v>[The derivative is a linear function, There is a  partial derivative in every direction at any point, A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="E33" t="str">
-        <f>"["&amp;B19&amp;", "&amp;B20&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
+        <f>"["&amp;B27&amp;", "&amp;B28&amp;"]"</f>
+        <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="I33" s="1" t="str">
         <f>"This is the long description for " &amp;B33 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The hot plate. It is quite a long description!</v>
+        <v>This is the long description for Directional Derivatives. It is quite a long description!</v>
       </c>
       <c r="J33" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="71.25" customHeight="1">
+    <row r="34" spans="1:11" ht="33.950000000000003" customHeight="1">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
         <v>34</v>
       </c>
-      <c r="D34" t="str">
-        <f>"["&amp;B8&amp;", "&amp;B10&amp;", "&amp;B13&amp;", "&amp;B14&amp;", "&amp;B17&amp;", "&amp;B15&amp;"]"</f>
-        <v>[The derivative can be a function, The derivative is a linear function, Variables can be held constant, Product rule, "With respect to what" matters, Single variable chain rule]</v>
-      </c>
-      <c r="E34" t="str">
-        <f>"["&amp;B23&amp;"]"</f>
-        <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="I34" s="1" t="str">
         <f>"This is the long description for " &amp;B34 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Chain Rule. It is quite a long description!</v>
-      </c>
-      <c r="J34" t="s">
-        <v>56</v>
+        <v>This is the long description for The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. . It is quite a long description!</v>
       </c>
       <c r="K34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="31.5">
+    <row r="35" spans="1:11" ht="33.950000000000003" customHeight="1">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
         <v>35</v>
       </c>
-      <c r="D35" t="str">
-        <f>"["&amp;B6&amp;", "&amp;B23&amp;"]"</f>
-        <v>[The derivative is the slope of a tangent line, A partial derivative can be expressed in terms of other partial derivatives]</v>
+      <c r="D35" t="s">
+        <v>13</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="I35" s="1" t="str">
         <f>"This is the long description for " &amp;B35 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Chain Rule Measurements. It is quite a long description!</v>
-      </c>
-      <c r="J35" t="s">
-        <v>59</v>
+        <v>This is the long description for The magnitude of $d\vec r$ is the length of a small step along a path. It is quite a long description!</v>
       </c>
       <c r="K35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="31.5">
+    <row r="36" spans="1:11" ht="33.950000000000003" customHeight="1">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
         <v>36</v>
       </c>
-      <c r="D36" t="str">
-        <f>"["&amp;B6&amp;", "&amp;B18&amp;", "&amp;B19&amp;", "&amp;B20&amp;"]"</f>
-        <v>[The derivative is the slope of a tangent line, Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point]</v>
-      </c>
-      <c r="E36" t="str">
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f>"This is the long description for " &amp;B36 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The direction of $d\vec r$ is ? . It is quite a long description!</v>
+      </c>
+      <c r="K36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="47.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <f>ROW()</f>
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f>"This is the long description for " &amp;B37 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient can tell you a small change in a function in any direction (differentials edition). It is quite a long description!</v>
+      </c>
+      <c r="K37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38">
+        <f>ROW()</f>
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f>"This is the long description for " &amp;B38 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a scalar field. It is quite a long description!</v>
+      </c>
+      <c r="K38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="51" customHeight="1">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <f>ROW()</f>
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="K39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30.95" customHeight="1">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <f>ROW()</f>
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="45" customHeight="1">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41">
+        <f>ROW()</f>
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="K41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="45.95" customHeight="1">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <f>ROW()</f>
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="K42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="31.5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43">
+        <f>ROW()</f>
+        <v>43</v>
+      </c>
+      <c r="D43" t="str">
+        <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
+        <v>[Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
+      </c>
+      <c r="E43" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" t="s">
+        <v>70</v>
+      </c>
+      <c r="K43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44">
+        <f>ROW()</f>
+        <v>44</v>
+      </c>
+      <c r="D44" t="e">
+        <f>"["&amp;Representations!#REF!&amp;"]"</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E44" t="str">
+        <f>"["&amp;B37&amp;"]"</f>
+        <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
+      </c>
+      <c r="F44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" t="s">
+        <v>72</v>
+      </c>
+      <c r="K44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="31.5">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <f>ROW()</f>
+        <v>45</v>
+      </c>
+      <c r="D45" t="str">
+        <f>"["&amp;B60&amp;"]"</f>
+        <v>[Vector Differentials]</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f>"This is the long description for " &amp;B45 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differential form of $\vec r$ in spherical and cylindrical coordinates. It is quite a long description!</v>
+      </c>
+      <c r="K45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="47.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46">
+        <f>ROW()</f>
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f>"This is the long description for " &amp;B46 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient's dimension is the same as real space. The gradient lives in the domain. It is quite a long description!</v>
+      </c>
+      <c r="K46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47">
+        <f>ROW()</f>
+        <v>47</v>
+      </c>
+      <c r="D47" t="str">
+        <f>"["&amp;Representations!B28&amp;"]"</f>
+        <v>[The derivative is local quantity]</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f>"This is the long description for " &amp;B47 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is a local quantity. It is quite a long description!</v>
+      </c>
+      <c r="K47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="31.5">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48">
+        <f>ROW()</f>
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" t="s">
+        <v>63</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f>"This is the long description for " &amp;B48 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The electric field is the negative gradient of the electric potential. It is quite a long description!</v>
+      </c>
+      <c r="K48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="31.5">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <f>ROW()</f>
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" t="s">
+        <v>63</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f>"This is the long description for " &amp;B49 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is related to the total flux through a closed surface. It is quite a long description!</v>
+      </c>
+      <c r="K49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.75">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50">
+        <f>ROW()</f>
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f>"This is the long description for " &amp;B50 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a function. It is quite a long description!</v>
+      </c>
+      <c r="K50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51">
+        <f>ROW()</f>
+        <v>51</v>
+      </c>
+      <c r="D51" t="str">
+        <f>"["&amp;Representations!B28&amp;"]"</f>
+        <v>[The derivative is local quantity]</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f>"This is the long description for " &amp;B51 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence is a local quantity. It is quite a long description!</v>
+      </c>
+      <c r="K51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="31.5">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52">
+        <f>ROW()</f>
+        <v>52</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f>"This is the long description for " &amp;B52 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the electric field is equal to. It is quite a long description!</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="31.5">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53">
+        <f>ROW()</f>
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" t="s">
+        <v>63</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f>"This is the long description for " &amp;B53 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the magnetic field is zero. It is quite a long description!</v>
+      </c>
+      <c r="K53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="31.5">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54">
+        <f>ROW()</f>
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>63</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <f>"This is the long description for " &amp;B54 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl is related to the line integral around a closed loop. ("circulation"). It is quite a long description!</v>
+      </c>
+      <c r="K54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.75">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55">
+        <f>ROW()</f>
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" t="s">
+        <v>63</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f>"This is the long description for " &amp;B55 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for the curl is a (vector) function. It is quite a long description!</v>
+      </c>
+      <c r="K55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56">
+        <f>ROW()</f>
+        <v>56</v>
+      </c>
+      <c r="D56" t="str">
+        <f>"["&amp;Representations!B28&amp;"]"</f>
+        <v>[The derivative is local quantity]</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f>"This is the long description for " &amp;B56 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl is a local quantity. It is quite a long description!</v>
+      </c>
+      <c r="K56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="31.5">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57">
+        <f>ROW()</f>
+        <v>57</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <f>"This is the long description for " &amp;B57 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The magnetic field is equal to the curl of the magnetic vector potential. It is quite a long description!</v>
+      </c>
+      <c r="K57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="31.5">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58">
+        <f>ROW()</f>
         <v>58</v>
       </c>
-      <c r="G36" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" s="1" t="str">
-        <f>"This is the long description for " &amp;B36 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The Hillside. It is quite a long description!</v>
-      </c>
-      <c r="K36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="47.25">
-      <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <f>"This is the long description for " &amp;B58 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The curl of the electric field is zero in electrostatics. It is quite a long description!</v>
+      </c>
+      <c r="K58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="47.25">
+      <c r="A59" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59">
+        <f>ROW()</f>
+        <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" t="s">
+        <v>63</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <f>"This is the long description for " &amp;B59 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The divergence of the curl is equal to mu times the current in magneto-statics. It is quite a long description!</v>
+      </c>
+      <c r="K59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.75">
+      <c r="A60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60">
+        <f>ROW()</f>
+        <v>60</v>
+      </c>
+      <c r="D60" t="str">
+        <f>"["&amp;B2&amp;", "&amp;B34&amp;"]"</f>
+        <v>[Difference / Change, The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. ]</v>
+      </c>
+      <c r="E60" t="str">
+        <f>"["&amp;B45&amp;"]"</f>
+        <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates]</v>
+      </c>
+      <c r="F60" t="s">
+        <v>89</v>
+      </c>
+      <c r="G60" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <f>"This is the long description for " &amp;B60 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Vector Differentials. It is quite a long description!</v>
+      </c>
+      <c r="K60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61">
+        <f>ROW()</f>
         <v>61</v>
       </c>
-      <c r="C37">
-        <f>ROW()</f>
-        <v>37</v>
-      </c>
-      <c r="D37" t="str">
-        <f>"["&amp;B10&amp;", "&amp;B19&amp;", "&amp;B23&amp;"]"</f>
-        <v>[The derivative is a linear function, There is a  partial derivative in every direction at any point, A partial derivative can be expressed in terms of other partial derivatives]</v>
-      </c>
-      <c r="E37" t="str">
-        <f>"["&amp;B27&amp;"]"</f>
-        <v>[All partial derivatives can be found as a slope of a tangent plane]</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="D61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <f>"This is the long description for " &amp;B61 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Acting out the Gradient. It is quite a long description!</v>
+      </c>
+      <c r="K61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="47.25">
+      <c r="A62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62">
+        <f>ROW()</f>
         <v>62</v>
       </c>
-      <c r="G37" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="1" t="str">
-        <f>"This is the long description for " &amp;B37 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Directional Derivatives. It is quite a long description!</v>
-      </c>
-      <c r="J37" t="s">
-        <v>63</v>
-      </c>
-      <c r="K37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="33.950000000000003" customHeight="1">
-      <c r="A38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38">
-        <f>ROW()</f>
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="1" t="str">
-        <f>"This is the long description for " &amp;B38 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. . It is quite a long description!</v>
-      </c>
-      <c r="K38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="33.950000000000003" customHeight="1">
-      <c r="A39" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39">
-        <f>ROW()</f>
-        <v>39</v>
-      </c>
-      <c r="D39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
-        <v>67</v>
-      </c>
-      <c r="I39" s="1" t="str">
-        <f>"This is the long description for " &amp;B39 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The magnitude of $d\vec r$ is the length of a small step along a path. It is quite a long description!</v>
-      </c>
-      <c r="K39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="33.950000000000003" customHeight="1">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40">
-        <f>ROW()</f>
-        <v>40</v>
-      </c>
-      <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" t="s">
-        <v>67</v>
-      </c>
-      <c r="I40" s="1" t="str">
-        <f>"This is the long description for " &amp;B40 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The direction of $d\vec r$ is ? . It is quite a long description!</v>
-      </c>
-      <c r="K40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="47.25">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41">
-        <f>ROW()</f>
-        <v>41</v>
-      </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" t="s">
-        <v>65</v>
-      </c>
-      <c r="I41" s="1" t="str">
-        <f>"This is the long description for " &amp;B41 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The gradient can tell you a small change in a function in any direction (differentials edition). It is quite a long description!</v>
-      </c>
-      <c r="K41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75">
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42">
-        <f>ROW()</f>
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="1" t="str">
-        <f>"This is the long description for " &amp;B42 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence is a scalar field. It is quite a long description!</v>
-      </c>
-      <c r="K42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="51" customHeight="1">
-      <c r="A43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43">
-        <f>ROW()</f>
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" t="s">
-        <v>65</v>
-      </c>
-      <c r="I43" s="1"/>
-      <c r="K43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="30.95" customHeight="1">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44">
-        <f>ROW()</f>
-        <v>44</v>
-      </c>
-      <c r="D44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>65</v>
-      </c>
-      <c r="I44" s="1"/>
-      <c r="K44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="45" customHeight="1">
-      <c r="A45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45">
-        <f>ROW()</f>
-        <v>45</v>
-      </c>
-      <c r="D45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>65</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="K45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="45.95" customHeight="1">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46">
-        <f>ROW()</f>
-        <v>46</v>
-      </c>
-      <c r="D46" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" t="s">
-        <v>65</v>
-      </c>
-      <c r="I46" s="1"/>
-      <c r="K46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="31.5">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47">
-        <f>ROW()</f>
-        <v>47</v>
-      </c>
-      <c r="D47" t="str">
-        <f>"["&amp;B18&amp;", "&amp;B19&amp;", "&amp;B21&amp;", "&amp;B22&amp;"]"</f>
-        <v>[Derivatives can be found while holding one or more variables constant, There is a  partial derivative in every direction at any point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
-      </c>
-      <c r="E47" t="str">
+      <c r="D62" t="str">
         <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
-      <c r="F47" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" t="s">
-        <v>65</v>
-      </c>
-      <c r="I47" s="1"/>
-      <c r="J47" t="s">
-        <v>74</v>
-      </c>
-      <c r="K47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48">
-        <f>ROW()</f>
-        <v>48</v>
-      </c>
-      <c r="D48" t="str">
-        <f>"["&amp;B28&amp;"]"</f>
-        <v>[The components of the gradient are partial derivatives]</v>
-      </c>
-      <c r="E48" t="str">
-        <f>"["&amp;B41&amp;"]"</f>
-        <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
-      </c>
-      <c r="F48" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" t="s">
-        <v>65</v>
-      </c>
-      <c r="I48" s="1"/>
-      <c r="J48" t="s">
-        <v>76</v>
-      </c>
-      <c r="K48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="31.5">
-      <c r="A49" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49">
-        <f>ROW()</f>
-        <v>49</v>
-      </c>
-      <c r="D49" t="str">
-        <f>"["&amp;B64&amp;"]"</f>
-        <v>[Vector Differentials]</v>
-      </c>
-      <c r="E49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I49" s="1" t="str">
-        <f>"This is the long description for " &amp;B49 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Differential form of $\vec r$ in spherical and cylindrical coordinates. It is quite a long description!</v>
-      </c>
-      <c r="K49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="47.25">
-      <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>78</v>
-      </c>
-      <c r="C50">
-        <f>ROW()</f>
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" t="s">
-        <v>67</v>
-      </c>
-      <c r="I50" s="1" t="str">
-        <f>"This is the long description for " &amp;B50 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The gradient's dimension is the same as real space. The gradient lives in the domain. It is quite a long description!</v>
-      </c>
-      <c r="K50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15.75">
-      <c r="A51" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51">
-        <f>ROW()</f>
-        <v>51</v>
-      </c>
-      <c r="D51" t="str">
-        <f>"["&amp;B29&amp;"]"</f>
-        <v>[The derivative is local quantity]</v>
-      </c>
-      <c r="E51" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" t="s">
-        <v>67</v>
-      </c>
-      <c r="I51" s="1" t="str">
-        <f>"This is the long description for " &amp;B51 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The gradient is a local quantity. It is quite a long description!</v>
-      </c>
-      <c r="K51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="31.5">
-      <c r="A52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" t="s">
-        <v>80</v>
-      </c>
-      <c r="C52">
-        <f>ROW()</f>
-        <v>52</v>
-      </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" t="s">
-        <v>67</v>
-      </c>
-      <c r="I52" s="1" t="str">
-        <f>"This is the long description for " &amp;B52 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The electric field is the negative gradient of the electric potential. It is quite a long description!</v>
-      </c>
-      <c r="K52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="31.5">
-      <c r="A53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53">
-        <f>ROW()</f>
-        <v>53</v>
-      </c>
-      <c r="D53" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" t="s">
-        <v>67</v>
-      </c>
-      <c r="I53" s="1" t="str">
-        <f>"This is the long description for " &amp;B53 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence is related to the total flux through a closed surface. It is quite a long description!</v>
-      </c>
-      <c r="K53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="15.75">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54">
-        <f>ROW()</f>
-        <v>54</v>
-      </c>
-      <c r="D54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" t="s">
-        <v>67</v>
-      </c>
-      <c r="I54" s="1" t="str">
-        <f>"This is the long description for " &amp;B54 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence is a function. It is quite a long description!</v>
-      </c>
-      <c r="K54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15.75">
-      <c r="A55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55">
-        <f>ROW()</f>
-        <v>55</v>
-      </c>
-      <c r="D55" t="str">
-        <f>"["&amp;B29&amp;"]"</f>
-        <v>[The derivative is local quantity]</v>
-      </c>
-      <c r="E55" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" t="s">
-        <v>67</v>
-      </c>
-      <c r="I55" s="1" t="str">
-        <f>"This is the long description for " &amp;B55 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence is a local quantity. It is quite a long description!</v>
-      </c>
-      <c r="K55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="31.5">
-      <c r="A56" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56">
-        <f>ROW()</f>
-        <v>56</v>
-      </c>
-      <c r="D56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" t="s">
-        <v>67</v>
-      </c>
-      <c r="I56" s="1" t="str">
-        <f>"This is the long description for " &amp;B56 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence of the electric field is equal to. It is quite a long description!</v>
-      </c>
-      <c r="K56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="31.5">
-      <c r="A57" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" t="s">
-        <v>85</v>
-      </c>
-      <c r="C57">
-        <f>ROW()</f>
-        <v>57</v>
-      </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" t="s">
-        <v>67</v>
-      </c>
-      <c r="I57" s="1" t="str">
-        <f>"This is the long description for " &amp;B57 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence of the magnetic field is zero. It is quite a long description!</v>
-      </c>
-      <c r="K57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="31.5">
-      <c r="A58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58">
-        <f>ROW()</f>
-        <v>58</v>
-      </c>
-      <c r="D58" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" t="s">
-        <v>67</v>
-      </c>
-      <c r="I58" s="1" t="str">
-        <f>"This is the long description for " &amp;B58 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The curl is related to the line integral around a closed loop. ("circulation"). It is quite a long description!</v>
-      </c>
-      <c r="K58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="15.75">
-      <c r="A59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" t="s">
-        <v>87</v>
-      </c>
-      <c r="C59">
-        <f>ROW()</f>
-        <v>59</v>
-      </c>
-      <c r="D59" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" t="s">
-        <v>13</v>
-      </c>
-      <c r="F59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" t="s">
-        <v>67</v>
-      </c>
-      <c r="I59" s="1" t="str">
-        <f>"This is the long description for " &amp;B59 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for the curl is a (vector) function. It is quite a long description!</v>
-      </c>
-      <c r="K59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="15.75">
-      <c r="A60" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60">
-        <f>ROW()</f>
-        <v>60</v>
-      </c>
-      <c r="D60" t="str">
-        <f>"["&amp;B29&amp;"]"</f>
-        <v>[The derivative is local quantity]</v>
-      </c>
-      <c r="E60" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" t="s">
-        <v>67</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f>"This is the long description for " &amp;B60 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The curl is a local quantity. It is quite a long description!</v>
-      </c>
-      <c r="K60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="31.5">
-      <c r="A61" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61">
-        <f>ROW()</f>
-        <v>61</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" t="s">
-        <v>67</v>
-      </c>
-      <c r="I61" s="1" t="str">
-        <f>"This is the long description for " &amp;B61 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The magnetic field is equal to the curl of the magnetic vector potential. It is quite a long description!</v>
-      </c>
-      <c r="K61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="31.5">
-      <c r="A62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62">
-        <f>ROW()</f>
-        <v>62</v>
-      </c>
-      <c r="D62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" t="s">
-        <v>13</v>
+      <c r="E62" t="str">
+        <f>"["&amp;B46&amp;", "&amp;B47&amp;"]"</f>
+        <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F62" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="G62" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I62" s="1" t="str">
         <f>"This is the long description for " &amp;B62 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The curl of the electric field is zero in electrostatics. It is quite a long description!</v>
+        <v>This is the long description for Visualizing Gradient. It is quite a long description!</v>
       </c>
       <c r="K62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="47.25">
+    <row r="63" spans="1:11" ht="15.75">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -2982,11 +2989,11 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I63" s="1" t="str">
         <f>"This is the long description for " &amp;B63 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The divergence of the curl is equal to mu times the current in magneto-statics. It is quite a long description!</v>
+        <v>This is the long description for Visualizing Divergence. It is quite a long description!</v>
       </c>
       <c r="K63" t="s">
         <v>15</v>
@@ -2994,127 +3001,126 @@
     </row>
     <row r="64" spans="1:11" ht="15.75">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
         <v>64</v>
       </c>
-      <c r="D64" t="str">
-        <f>"["&amp;B2&amp;", "&amp;B38&amp;"]"</f>
-        <v>[Difference / Change, The components of $d \vec r$ is an arbitrary small change between two arbitrary position vectors. ]</v>
-      </c>
-      <c r="E64" t="str">
-        <f>"["&amp;B49&amp;"]"</f>
-        <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates]</v>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I64" s="1" t="str">
         <f>"This is the long description for " &amp;B64 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Vector Differentials. It is quite a long description!</v>
+        <v>This is the long description for Visualizing Curl. It is quite a long description!</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.75">
+    <row r="65" spans="1:11" ht="126">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
         <v>65</v>
       </c>
-      <c r="D65" t="s">
-        <v>13</v>
+      <c r="D65" t="str">
+        <f>"["&amp;B$2&amp;"]"</f>
+        <v>[Difference / Change]</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="G65" t="s">
-        <v>67</v>
-      </c>
-      <c r="I65" s="1" t="str">
-        <f>"This is the long description for " &amp;B65 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Acting out the Gradient. It is quite a long description!</v>
+        <v>97</v>
+      </c>
+      <c r="H65" t="s">
+        <v>98</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="47.25">
+    <row r="66" spans="1:11" ht="31.5">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
         <v>66</v>
       </c>
-      <c r="D66" t="str">
-        <f>"["&amp;B25&amp;", "&amp;B26&amp;"]"</f>
-        <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
-      </c>
-      <c r="E66" t="str">
-        <f>"["&amp;B50&amp;", "&amp;B51&amp;"]"</f>
-        <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
+      <c r="D66" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
       </c>
       <c r="F66" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G66" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="I66" s="1" t="str">
         <f>"This is the long description for " &amp;B66 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Gradient. It is quite a long description!</v>
+        <v>This is the long description for Equations can be 'zapped with d' to relate differentials. It is quite a long description!</v>
       </c>
       <c r="K66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.75">
+    <row r="67" spans="1:11" ht="31.5">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67">
+        <f>ROW()</f>
+        <v>67</v>
+      </c>
+      <c r="D67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" t="s">
         <v>97</v>
-      </c>
-      <c r="C67">
-        <f>ROW()</f>
-        <v>67</v>
-      </c>
-      <c r="D67" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" t="s">
-        <v>13</v>
-      </c>
-      <c r="F67" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" t="s">
-        <v>67</v>
       </c>
       <c r="I67" s="1" t="str">
         <f>"This is the long description for " &amp;B67 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Divergence. It is quite a long description!</v>
+        <v>This is the long description for Individual differentials can be manipulated algebraically. It is quite a long description!</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
@@ -3122,10 +3128,10 @@
     </row>
     <row r="68" spans="1:11" ht="15.75">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3138,79 +3144,77 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="G68" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="I68" s="1" t="str">
         <f>"This is the long description for " &amp;B68 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Curl. It is quite a long description!</v>
+        <v>This is the long description for Total differentials are linear. It is quite a long description!</v>
       </c>
       <c r="K68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="126">
+    <row r="69" spans="1:11" ht="15.75">
       <c r="A69" t="s">
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
         <v>69</v>
       </c>
-      <c r="D69" t="str">
-        <f>"["&amp;B$2&amp;"]"</f>
-        <v>[Difference / Change]</v>
+      <c r="D69" t="s">
+        <v>13</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G69" t="s">
-        <v>101</v>
-      </c>
-      <c r="H69" t="s">
-        <v>102</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
+      </c>
+      <c r="I69" s="1" t="str">
+        <f>"This is the long description for " &amp;B69 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Differentials are small chunks. It is quite a long description!</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="31.5">
+    <row r="70" spans="1:11" ht="47.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
         <v>70</v>
       </c>
-      <c r="D70" t="s">
-        <v>13</v>
+      <c r="D70" t="str">
+        <f>"["&amp;B$4&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes]</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I70" s="1" t="str">
         <f>"This is the long description for " &amp;B70 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Equations can be 'zapped with d' to relate differentials. It is quite a long description!</v>
+        <v>This is the long description for There are experimental limits to how $small$ of a change can be measured. It is quite a long description!</v>
       </c>
       <c r="K70" t="s">
         <v>15</v>
@@ -3237,17 +3241,17 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I71" s="1" t="str">
         <f>"This is the long description for " &amp;B71 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Individual differentials can be manipulated algebraically. It is quite a long description!</v>
+        <v>This is the long description for The derivative can be interpreted physically. It is quite a long description!</v>
       </c>
       <c r="K71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.75">
+    <row r="72" spans="1:11" ht="110.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -3258,8 +3262,9 @@
         <f>ROW()</f>
         <v>72</v>
       </c>
-      <c r="D72" t="s">
-        <v>13</v>
+      <c r="D72" t="str">
+        <f>"["&amp;B$18&amp;","&amp;B$22&amp;"]"</f>
+        <v>[Derivatives can be found while holding one or more variables constant,The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -3268,61 +3273,68 @@
         <v>108</v>
       </c>
       <c r="G72" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+      <c r="H72" t="s">
+        <v>109</v>
       </c>
       <c r="I72" s="1" t="str">
         <f>"This is the long description for " &amp;B72 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Total differentials are linear. It is quite a long description!</v>
+        <v>This is the long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative. It is quite a long description!</v>
       </c>
       <c r="K72" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.75">
+    <row r="73" spans="1:11" ht="50.25" customHeight="1">
       <c r="A73" t="s">
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
         <v>73</v>
       </c>
-      <c r="D73" t="s">
-        <v>13</v>
+      <c r="D73" t="str">
+        <f>"["&amp;B$4&amp;","&amp;B$65&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes,Differentials are small changes or differences]</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+      <c r="H73" t="s">
+        <v>111</v>
       </c>
       <c r="I73" s="1" t="str">
         <f>"This is the long description for " &amp;B73 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Differentials are small chunks. It is quite a long description!</v>
+        <v>This is the long description for Partial derivatives are coefficients in a differentials equation. It is quite a long description!</v>
       </c>
       <c r="K73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="47.25">
+    <row r="74" spans="1:11" ht="78.75">
       <c r="A74" t="s">
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
         <v>74</v>
       </c>
       <c r="D74" t="str">
-        <f>"["&amp;B$4&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes]</v>
+        <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
+        <v>[You can flip a derivative, Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -3331,11 +3343,10 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>101</v>
-      </c>
-      <c r="I74" s="1" t="str">
-        <f>"This is the long description for " &amp;B74 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for There are experimental limits to how $small$ of a change can be measured. It is quite a long description!</v>
+        <v>97</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
@@ -3346,7 +3357,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3362,30 +3373,29 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I75" s="1" t="str">
         <f>"This is the long description for " &amp;B75 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The derivative can be interpreted physically. It is quite a long description!</v>
+        <v>This is the long description for There might be experimental limits on which quantities you can measure. It is quite a long description!</v>
       </c>
       <c r="K75" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="78.75">
+    <row r="76" spans="1:11" ht="47.25">
       <c r="A76" t="s">
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
         <v>76</v>
       </c>
-      <c r="D76" t="str">
-        <f>"["&amp;B$18&amp;","&amp;B$22&amp;"]"</f>
-        <v>[Derivatives can be found while holding one or more variables constant,The value of a partial derivative depends on the value(s) of what is held constant]</v>
+      <c r="D76" t="s">
+        <v>13</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -3394,289 +3404,164 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>101</v>
-      </c>
-      <c r="H76" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="I76" s="1" t="str">
         <f>"This is the long description for " &amp;B76 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative. It is quite a long description!</v>
+        <v>This is the long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long description!</v>
       </c>
       <c r="K76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="50.25" customHeight="1">
+    <row r="77" spans="1:11" ht="15.75">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
         <v>77</v>
       </c>
       <c r="D77" t="str">
-        <f>"["&amp;B$4&amp;","&amp;B$69&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes,Differentials are small changes or differences]</v>
-      </c>
-      <c r="E77" t="s">
-        <v>13</v>
+        <f>"["&amp;B2&amp;", "&amp;B4&amp;", "&amp;B5&amp;", "&amp;B7&amp;", "&amp;B8&amp;", "&amp;B13&amp;"]"</f>
+        <v>[Difference / Change, The derivative is a ratio of small changes, The derivative can be approximated by the slope of a secant line, The derivative is a limit, The derivative can be a function, Variables can be held constant]</v>
+      </c>
+      <c r="E77" t="str">
+        <f>"["&amp;B65&amp;", "&amp;B66&amp;", "&amp;B67&amp;", "&amp;B68&amp;"]"</f>
+        <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F77" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="G77" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H77" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I77" s="1" t="str">
         <f>"This is the long description for " &amp;B77 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Partial derivatives are coefficients in a differentials equation. It is quite a long description!</v>
+        <v>This is the long description for Zapping with d. It is quite a long description!</v>
       </c>
       <c r="K77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="78.75">
+    <row r="78" spans="1:11" ht="15.75">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
         <v>78</v>
       </c>
       <c r="D78" t="str">
-        <f>"["&amp;B16&amp;", "&amp;B18&amp;"]"</f>
-        <v>[You can flip a derivative, Derivatives can be found while holding one or more variables constant]</v>
-      </c>
-      <c r="E78" t="s">
-        <v>13</v>
+        <f>"["&amp;B65&amp;", "&amp;B67&amp;"]"</f>
+        <v>[Differentials are small changes or differences, Individual differentials can be manipulated algebraically]</v>
+      </c>
+      <c r="E78" t="str">
+        <f>"["&amp;B69&amp;"]"</f>
+        <v>[Differentials are small chunks]</v>
       </c>
       <c r="F78" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="G78" t="s">
-        <v>101</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+      <c r="I78" s="1" t="str">
+        <f>"This is the long description for " &amp;B78 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Energy and Integrals. It is quite a long description!</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="31.5">
+    <row r="79" spans="1:11" ht="93" customHeight="1">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B79" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
         <v>79</v>
       </c>
-      <c r="D79" t="s">
-        <v>13</v>
-      </c>
-      <c r="E79" t="s">
-        <v>13</v>
+      <c r="D79" t="str">
+        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;", "&amp;B65&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding one or more variables constant, The value of a partial derivative depends on the value(s) of what is held constant, Differentials are small changes or differences]</v>
+      </c>
+      <c r="E79" t="str">
+        <f>"["&amp;B70&amp;", "&amp;B71&amp;", "&amp;B72&amp;", "&amp;B73&amp;"]"</f>
+        <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F79" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="G79" t="s">
-        <v>101</v>
-      </c>
-      <c r="I79" s="1" t="str">
-        <f>"This is the long description for " &amp;B79 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for There might be experimental limits on which quantities you can measure. It is quite a long description!</v>
+        <v>97</v>
+      </c>
+      <c r="H79" t="s">
+        <v>122</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J79" t="s">
+        <v>124</v>
       </c>
       <c r="K79" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="47.25">
+    <row r="80" spans="1:11" ht="94.5">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
         <v>80</v>
       </c>
-      <c r="D80" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" t="s">
-        <v>13</v>
+      <c r="D80" t="str">
+        <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B65&amp;", "&amp;B66&amp;", "&amp;B67&amp;", "&amp;B72&amp;", "&amp;B73&amp;"]"</f>
+        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding one or more variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
+      </c>
+      <c r="E80" t="str">
+        <f>"["&amp;B74&amp;", "&amp;B75&amp;", "&amp;B76&amp;"]"</f>
+        <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F80" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="G80" t="s">
-        <v>101</v>
-      </c>
-      <c r="I80" s="1" t="str">
-        <f>"This is the long description for " &amp;B80 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for. It is quite a long description!</v>
+        <v>97</v>
+      </c>
+      <c r="H80" t="s">
+        <v>126</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.75">
-      <c r="A81" t="s">
-        <v>48</v>
-      </c>
-      <c r="B81" t="s">
-        <v>120</v>
-      </c>
-      <c r="C81">
-        <f>ROW()</f>
-        <v>81</v>
-      </c>
-      <c r="D81" t="str">
-        <f>"["&amp;B2&amp;", "&amp;B4&amp;", "&amp;B5&amp;", "&amp;B7&amp;", "&amp;B8&amp;", "&amp;B13&amp;"]"</f>
-        <v>[Difference / Change, The derivative is a ratio of small changes, The derivative can be approximated by the slope of a secant line, The derivative is a limit, The derivative can be a function, Variables can be held constant]</v>
-      </c>
-      <c r="E81" t="str">
-        <f>"["&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B72&amp;"]"</f>
-        <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
-      </c>
-      <c r="F81" t="s">
-        <v>108</v>
-      </c>
-      <c r="G81" t="s">
-        <v>101</v>
-      </c>
-      <c r="H81" t="s">
-        <v>121</v>
-      </c>
-      <c r="I81" s="1" t="str">
-        <f>"This is the long description for " &amp;B81 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Zapping with d. It is quite a long description!</v>
-      </c>
-      <c r="K81" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="15.75">
-      <c r="A82" t="s">
-        <v>48</v>
-      </c>
-      <c r="B82" t="s">
-        <v>122</v>
-      </c>
-      <c r="C82">
-        <f>ROW()</f>
-        <v>82</v>
-      </c>
-      <c r="D82" t="str">
-        <f>"["&amp;B69&amp;", "&amp;B71&amp;"]"</f>
-        <v>[Differentials are small changes or differences, Individual differentials can be manipulated algebraically]</v>
-      </c>
-      <c r="E82" t="str">
-        <f>"["&amp;B73&amp;"]"</f>
-        <v>[Differentials are small chunks]</v>
-      </c>
-      <c r="F82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" t="s">
-        <v>101</v>
-      </c>
-      <c r="I82" s="1" t="str">
-        <f>"This is the long description for " &amp;B82 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Energy and Integrals. It is quite a long description!</v>
-      </c>
-      <c r="K82" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="93" customHeight="1">
-      <c r="A83" t="s">
-        <v>48</v>
-      </c>
-      <c r="B83" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83">
-        <f>ROW()</f>
-        <v>83</v>
-      </c>
-      <c r="D83" t="str">
-        <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B22&amp;", "&amp;B69&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, Variables can be held constant, Derivatives can be found while holding one or more variables constant, The value of a partial derivative depends on the value(s) of what is held constant, Differentials are small changes or differences]</v>
-      </c>
-      <c r="E83" t="str">
-        <f>"["&amp;B74&amp;", "&amp;B75&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
-      </c>
-      <c r="F83" t="s">
-        <v>124</v>
-      </c>
-      <c r="G83" t="s">
-        <v>101</v>
-      </c>
-      <c r="H83" t="s">
-        <v>125</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J83" t="s">
-        <v>127</v>
-      </c>
-      <c r="K83" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="94.5">
-      <c r="A84" t="s">
-        <v>48</v>
-      </c>
-      <c r="B84" t="s">
-        <v>128</v>
-      </c>
-      <c r="C84">
-        <f>ROW()</f>
-        <v>84</v>
-      </c>
-      <c r="D84" t="str">
-        <f>"["&amp;B4&amp;", "&amp;B8&amp;", "&amp;B13&amp;", "&amp;B18&amp;", "&amp;B23&amp;", "&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B76&amp;", "&amp;B77&amp;"]"</f>
-        <v>[The derivative is a ratio of small changes, The derivative can be a function, Variables can be held constant, Derivatives can be found while holding one or more variables constant, A partial derivative can be expressed in terms of other partial derivatives, Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
-      </c>
-      <c r="E84" t="str">
-        <f>"["&amp;B78&amp;", "&amp;B79&amp;", "&amp;B80&amp;"]"</f>
-        <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
-      </c>
-      <c r="F84">
-        <v>21</v>
-      </c>
-      <c r="G84" t="s">
-        <v>101</v>
-      </c>
-      <c r="H84" t="s">
-        <v>129</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K84" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="81" ht="15.75"/>
+    <row r="82" ht="15.75"/>
+    <row r="83" ht="15.75"/>
+    <row r="84" ht="15.75"/>
+    <row r="85" ht="15.75"/>
+    <row r="87" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3686,10 +3571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EFD8F-45BF-44EB-A2B4-FA9451BFAEEC}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3699,17 +3584,180 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="71.25" customHeight="1"/>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28">
+        <f>ROW()</f>
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The derivative is local quantity. It is quite a long description!</v>
+      </c>
+      <c r="K28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f>"This is the long description for " &amp;B29 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Partial derivatives are functions. It is quite a long description!</v>
+      </c>
+      <c r="K29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
         <v>133</v>
+      </c>
+      <c r="C30">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f>"This is the long description for " &amp;B30 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for The gradient is a function. It is quite a long description!</v>
+      </c>
+      <c r="K30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="63">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34">
+        <f>ROW()</f>
+        <v>34</v>
+      </c>
+      <c r="D34" t="str">
+        <f>"["&amp;Sheet1!B6&amp;", "&amp;Sheet1!B23&amp;"]"</f>
+        <v>[The derivative is the slope of a tangent line, A partial derivative can be expressed in terms of other partial derivatives]</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f>"This is the long description for " &amp;B34 &amp;". It is quite a long description!"</f>
+        <v>This is the long description for Chain Rule Measurements. It is quite a long description!</v>
+      </c>
+      <c r="J34" t="s">
+        <v>135</v>
+      </c>
+      <c r="K34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="409.6">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69">
+        <f>ROW()</f>
+        <v>69</v>
+      </c>
+      <c r="D69" t="str">
+        <f>"["&amp;B$2&amp;"]"</f>
+        <v>[]</v>
+      </c>
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" t="s">
+        <v>136</v>
+      </c>
+      <c r="G69" t="s">
+        <v>97</v>
+      </c>
+      <c r="H69" t="s">
+        <v>98</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K69" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits that I did not have to do
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19321"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Mike's Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_21E2BB697F9D6CFAA84D0C82B8CBFECAF4C19DEE" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6700" yWindow="-23540" windowWidth="19200" windowHeight="22520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6700" yWindow="-23540" windowWidth="19200" windowHeight="22520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="170">
   <si>
     <t>Act or Con</t>
   </si>
@@ -171,6 +172,12 @@
     <t>The heater II</t>
   </si>
   <si>
+    <t>mvheater.png</t>
+  </si>
+  <si>
+    <t>This small group activity is designed to help students interpret partial derivatives using contour diagrams. Students work in small groups to determine rates of change using a contour diagram showing isotherms over time and space. The whole class wrap-up discussion emphasizes giving a physical interpretation for the derivative, the value of units in thinking about functions and derivatives, and the need to specify “with respect to what” when finding derivatives in multivariable contexts.</t>
+  </si>
+  <si>
     <t>mvheater2</t>
   </si>
   <si>
@@ -180,6 +187,12 @@
     <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
   </si>
   <si>
+    <t>mvhotplate.png</t>
+  </si>
+  <si>
+    <t>This small group activity using surfaces introduces a geometric interpretation of partial derivatives in terms of measured ratios of small changes. Students work in small groups to identify locations on their surface with particular properties. The whole class wrap-up discussion emphasizes the equivalence of multiple representations of partial derivatives.</t>
+  </si>
+  <si>
     <t>mvhotplate</t>
   </si>
   <si>
@@ -198,12 +211,21 @@
     <t>[partial f/partial x, Inclinometer]</t>
   </si>
   <si>
+    <t>mvhillside</t>
+  </si>
+  <si>
     <t>Directional Derivatives</t>
   </si>
   <si>
     <t>[partial f/partial x, Inclinometer, Del f]</t>
   </si>
   <si>
+    <t>MathSurfaces1.png</t>
+  </si>
+  <si>
+    <t>This small group activity using surfaces relates the geometric definition of directional derivatives to the components of the gradient vector. Students work in small groups to measure a directional derivative directly, then compare its components with measured partial derivatives in rectangular coordinates. The whole class wrap-up discussion emphasizes the relationship between the geometric gradient vector and directional derivatives.</t>
+  </si>
+  <si>
     <t>mvdderiv</t>
   </si>
   <si>
@@ -237,12 +259,24 @@
     <t>[Contour Maps, Del dot f]</t>
   </si>
   <si>
+    <t>vchill.jpg</t>
+  </si>
+  <si>
+    <t>This small group activity is designed to reinforce the geometric definition of the gradient. Students work in small groups to construct the gradient vector at different points on a hill. Then, students compare and contrast their findings to reinforce that the gradient is a vector field, but also that it is a local quantity. The whole class wrap-up discussion emphasizes that the gradient lives in the domain, not on the graph.</t>
+  </si>
+  <si>
     <t>vchill</t>
   </si>
   <si>
     <t>The Valley</t>
   </si>
   <si>
+    <t>vcvalley.jpg</t>
+  </si>
+  <si>
+    <t>This small group activity is designed to reinforce the geometry of line integrals, and to set the stage for path independence, and builds on the Hill activity.  Students work in small groups to evaluate the elevation change along different paths. The whole class wrap-up discussion reinforces the importance of a “Use what you know!” strategy to evaluate line integrals, and emphasizes that different paths with the same endpoints must have the same elevation gain.</t>
+  </si>
+  <si>
     <t>vcvalley</t>
   </si>
   <si>
@@ -297,21 +331,69 @@
     <t>[df, 3D plots]</t>
   </si>
   <si>
+    <t>vfdrvectorcurvi.jpg</t>
+  </si>
+  <si>
+    <t>We use the vector differential to create a unified view of calculus. Students have a lot of difficulty writing down exact differentials and writing down equations for vectors in curvilinear coordinates. This activity allows students to use geometric reasoning to practice both of these skills.  In particular, students are provided with a variety of alternate tangible representations for rectangular, cylindrical, and spherical coordinates, including oatmeal cans, globes, pineapples, and pumpkins.</t>
+  </si>
+  <si>
+    <t>vfdrvectorcurvi</t>
+  </si>
+  <si>
     <t>Acting out the Gradient</t>
   </si>
   <si>
+    <t>[Kinesthetic]</t>
+  </si>
+  <si>
+    <t>vfactinggrad.jpg</t>
+  </si>
+  <si>
+    <t>Oftentimes, students are not correctly interpreting situations geometrically when it seems they are. This activity is designed to test the ability of a class to represent the gradient physically for a function $f(x,y)$ that represents an elliptical hill. In the activity, the students themselves as points distributed throughout the classroom represent a vector field, using their right arm as a vector pointing in the direction of the gradient. The instructor will also have the opportunity to clarify the proper gradient direction (in the $xy$-plan) for students that are pointing incorrectly (``up'' the hill).</t>
+  </si>
+  <si>
+    <t>vfactinggrad</t>
+  </si>
+  <si>
     <t>Visualizing Gradient</t>
   </si>
   <si>
     <t>[Kinesthetic, Vector Field Map, Contour Maps]</t>
   </si>
   <si>
+    <t>vfgradient.jpg</t>
+  </si>
+  <si>
+    <t>Building a geometric understanding of the gradient can be challenging for students, particularly in physics classrooms when their only prior exposure to the gradient is in mathematics courses. This activity is a follow-up to Acting out the Gradient, in which students use Mathematica to calculate and visualize the gradient for different representations of scalar fields.  Students explicitly compare and contrast these different representations, in particular identifying that the gradient is always perpendicular to constant surfaces.</t>
+  </si>
+  <si>
+    <t>vfgradient</t>
+  </si>
+  <si>
     <t>Visualizing Divergence</t>
   </si>
   <si>
+    <t>vfdivergence.jpg</t>
+  </si>
+  <si>
+    <t>The traditional discussion of divergence in vector calculus derives an algebraic expression in rectangular coordinates. We prefer to give a geometric derivation as flux per unit volume through an appropriately shaped box. In this activity, students learn how to predict the value of the divergence at any point by looking at the vector field near that point.  The activity is an excellent one for fostering representational fluency, as students can be asked to engage with vector field maps on paper, plots in Mathematica, and symbolic expressions for vector fields.  A nice extension is to have students consider vector fields that have different fundamental symmetries and to recognize that they can adjust the shape of the infinitesimal box to take advantage of such symmetry.</t>
+  </si>
+  <si>
+    <t>vfdivergence</t>
+  </si>
+  <si>
     <t>Visualizing Curl</t>
   </si>
   <si>
+    <t>vfcurlvis.jpg</t>
+  </si>
+  <si>
+    <t>The traditional discussion of curl in vector calculus derives an algebraic expression in rectangular coordinates. As with divergence (see the Visualizing Divergence activity), we prefer to give a geometric derivation as circulation per unit area around an appropriately shaped closed curve. In this activity, students learn how to predict the value of the curl at any point by looking at the vector field near that point.  The activity is an excellent one for fostering representational fluency, as students can be asked to engage with vector field maps on paper, plots in Mathematica, and symbolic expressions for vector fields.  A nice extension is to have students consider vector fields that have different fundamental symmetries and to recognize that they can adjust the shape of the infinitesimal box to take advantage of such symmetry.</t>
+  </si>
+  <si>
+    <t>vfcurlvis</t>
+  </si>
+  <si>
     <t>Differentials are small changes or differences</t>
   </si>
   <si>
@@ -381,12 +463,27 @@
     <t>LPsmall.jpg</t>
   </si>
   <si>
+    <t>We would like our students to have both a practical and mathematical understanding of a total differential. In particular, with this activity students learn what the consequences of ``zapping'' a function with the operator ``d'' are. This activity also opens up a conversation on infinitesimals, and their relation to total differentials. The use of variables not associated with the Partial Derivative Machine in this activity allows students to apply the mathematical techniques they have been practicing during the course to a less familiar physical system.</t>
+  </si>
+  <si>
+    <t>inzapd</t>
+  </si>
+  <si>
     <t>Energy and Integrals</t>
   </si>
   <si>
     <t>[PDM, df]</t>
   </si>
   <si>
+    <t>inpotentiallab.jpg</t>
+  </si>
+  <si>
+    <t>This integrated lab activity is designed to ask upper-division undergraduate students to measure the change in potential energy in an elastic system (PDM) between two different states. Students use the Partial Derivative Machine (PDM) to verify experimentally that the forces and dimensions of their system are state variables as well as measure the relationships between these quantities to compute the potential energy of their system. The whole class discussion focuses on the meaning of integration of discrete experimental data.</t>
+  </si>
+  <si>
+    <t>inpotentiallab</t>
+  </si>
+  <si>
     <t>Partial Derivative Machine Derivatives</t>
   </si>
   <si>
@@ -399,7 +496,7 @@
     <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
   </si>
   <si>
-    <t>eefixme</t>
+    <t>inisowidth</t>
   </si>
   <si>
     <t>Chain Rules</t>
@@ -409,6 +506,9 @@
   </si>
   <si>
     <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>incycchainrule</t>
   </si>
   <si>
     <t>$\frac{\partial f}{\partial x}$</t>
@@ -1021,9 +1121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="E56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1910,7 +2010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75">
+    <row r="29" spans="1:11" ht="94.5">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1935,23 +2035,25 @@
       <c r="G29" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="1" t="str">
-        <f>"This is the long description for " &amp;B29 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The heater II. It is quite a long description!</v>
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="J29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="47.25">
+    <row r="30" spans="1:11" ht="78.75">
       <c r="A30" t="s">
         <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <f>ROW()</f>
@@ -1966,17 +2068,19 @@
         <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="1" t="str">
-        <f>"This is the long description for " &amp;B30 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The hot plate. It is quite a long description!</v>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="J30" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K30" t="s">
         <v>15</v>
@@ -1987,7 +2091,7 @@
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <f>ROW()</f>
@@ -2002,7 +2106,7 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G31" t="s">
         <v>33</v>
@@ -2012,7 +2116,7 @@
         <v>This is the long description for Chain Rule. It is quite a long description!</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K31" t="s">
         <v>15</v>
@@ -2023,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2038,7 +2142,7 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
@@ -2047,16 +2151,19 @@
         <f>"This is the long description for " &amp;B32 &amp;". It is quite a long description!"</f>
         <v>This is the long description for The Hillside. It is quite a long description!</v>
       </c>
+      <c r="J32" t="s">
+        <v>61</v>
+      </c>
       <c r="K32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="47.25">
+    <row r="33" spans="1:11" ht="94.5">
       <c r="A33" t="s">
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2071,17 +2178,19 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
-      <c r="I33" s="1" t="str">
-        <f>"This is the long description for " &amp;B33 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Directional Derivatives. It is quite a long description!</v>
+      <c r="H33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="J33" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
@@ -2092,7 +2201,7 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2108,7 +2217,7 @@
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I34" s="1" t="str">
         <f>"This is the long description for " &amp;B34 &amp;". It is quite a long description!"</f>
@@ -2123,7 +2232,7 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2139,7 +2248,7 @@
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I35" s="1" t="str">
         <f>"This is the long description for " &amp;B35 &amp;". It is quite a long description!"</f>
@@ -2154,7 +2263,7 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2170,7 +2279,7 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I36" s="1" t="str">
         <f>"This is the long description for " &amp;B36 &amp;". It is quite a long description!"</f>
@@ -2185,7 +2294,7 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2201,7 +2310,7 @@
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I37" s="1" t="str">
         <f>"This is the long description for " &amp;B37 &amp;". It is quite a long description!"</f>
@@ -2213,7 +2322,7 @@
     </row>
     <row r="38" spans="1:11" ht="15.75">
       <c r="B38" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2254,7 +2363,7 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I39" s="1"/>
       <c r="K39" t="s">
@@ -2279,7 +2388,7 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I40" s="1"/>
       <c r="K40" t="s">
@@ -2288,7 +2397,7 @@
     </row>
     <row r="41" spans="1:11" ht="45" customHeight="1">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2304,7 +2413,7 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I41" s="1"/>
       <c r="K41" t="s">
@@ -2329,19 +2438,19 @@
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I42" s="1"/>
       <c r="K42" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="31.5">
+    <row r="43" spans="1:11" ht="94.5">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C43">
         <f>ROW()</f>
@@ -2356,25 +2465,30 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F43" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>61</v>
-      </c>
-      <c r="I43" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H43" t="s">
+        <v>77</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="J43" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="K43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75">
+    <row r="44" spans="1:11" ht="94.5">
       <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C44">
         <f>ROW()</f>
@@ -2392,11 +2506,16 @@
         <v>37</v>
       </c>
       <c r="G44" t="s">
-        <v>61</v>
-      </c>
-      <c r="I44" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="J44" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="K44" t="s">
         <v>15</v>
@@ -2407,7 +2526,7 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C45">
         <f>ROW()</f>
@@ -2424,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I45" s="1" t="str">
         <f>"This is the long description for " &amp;B45 &amp;". It is quite a long description!"</f>
@@ -2439,7 +2558,7 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C46">
         <f>ROW()</f>
@@ -2455,7 +2574,7 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I46" s="1" t="str">
         <f>"This is the long description for " &amp;B46 &amp;". It is quite a long description!"</f>
@@ -2470,7 +2589,7 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2487,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I47" s="1" t="str">
         <f>"This is the long description for " &amp;B47 &amp;". It is quite a long description!"</f>
@@ -2502,7 +2621,7 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2518,7 +2637,7 @@
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I48" s="1" t="str">
         <f>"This is the long description for " &amp;B48 &amp;". It is quite a long description!"</f>
@@ -2533,7 +2652,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2549,7 +2668,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I49" s="1" t="str">
         <f>"This is the long description for " &amp;B49 &amp;". It is quite a long description!"</f>
@@ -2564,7 +2683,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -2580,7 +2699,7 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I50" s="1" t="str">
         <f>"This is the long description for " &amp;B50 &amp;". It is quite a long description!"</f>
@@ -2595,7 +2714,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2612,7 +2731,7 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I51" s="1" t="str">
         <f>"This is the long description for " &amp;B51 &amp;". It is quite a long description!"</f>
@@ -2627,7 +2746,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -2643,7 +2762,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I52" s="1" t="str">
         <f>"This is the long description for " &amp;B52 &amp;". It is quite a long description!"</f>
@@ -2658,7 +2777,7 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -2674,7 +2793,7 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I53" s="1" t="str">
         <f>"This is the long description for " &amp;B53 &amp;". It is quite a long description!"</f>
@@ -2689,7 +2808,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -2705,7 +2824,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I54" s="1" t="str">
         <f>"This is the long description for " &amp;B54 &amp;". It is quite a long description!"</f>
@@ -2720,7 +2839,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -2736,7 +2855,7 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I55" s="1" t="str">
         <f>"This is the long description for " &amp;B55 &amp;". It is quite a long description!"</f>
@@ -2751,7 +2870,7 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -2768,7 +2887,7 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I56" s="1" t="str">
         <f>"This is the long description for " &amp;B56 &amp;". It is quite a long description!"</f>
@@ -2783,7 +2902,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -2799,7 +2918,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I57" s="1" t="str">
         <f>"This is the long description for " &amp;B57 &amp;". It is quite a long description!"</f>
@@ -2814,7 +2933,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -2830,7 +2949,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I58" s="1" t="str">
         <f>"This is the long description for " &amp;B58 &amp;". It is quite a long description!"</f>
@@ -2845,7 +2964,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -2861,7 +2980,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I59" s="1" t="str">
         <f>"This is the long description for " &amp;B59 &amp;". It is quite a long description!"</f>
@@ -2871,12 +2990,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.75">
+    <row r="60" spans="1:11" ht="94.5">
       <c r="A60" t="s">
         <v>46</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -2891,25 +3010,30 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates]</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="G60" t="s">
-        <v>63</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f>"This is the long description for " &amp;B60 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Vector Differentials. It is quite a long description!</v>
+        <v>70</v>
+      </c>
+      <c r="H60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J60" t="s">
+        <v>103</v>
       </c>
       <c r="K60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.75">
+    <row r="61" spans="1:11" ht="126">
       <c r="A61" t="s">
         <v>46</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -2922,25 +3046,30 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="G61" t="s">
-        <v>63</v>
-      </c>
-      <c r="I61" s="1" t="str">
-        <f>"This is the long description for " &amp;B61 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Acting out the Gradient. It is quite a long description!</v>
+        <v>70</v>
+      </c>
+      <c r="H61" t="s">
+        <v>106</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J61" t="s">
+        <v>108</v>
       </c>
       <c r="K61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="47.25">
+    <row r="62" spans="1:11" ht="110.25">
       <c r="A62" t="s">
         <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -2955,25 +3084,30 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F62" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="G62" t="s">
-        <v>63</v>
-      </c>
-      <c r="I62" s="1" t="str">
-        <f>"This is the long description for " &amp;B62 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Gradient. It is quite a long description!</v>
+        <v>70</v>
+      </c>
+      <c r="H62" t="s">
+        <v>111</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J62" t="s">
+        <v>113</v>
       </c>
       <c r="K62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.75">
+    <row r="63" spans="1:11" ht="157.5">
       <c r="A63" t="s">
         <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -2989,22 +3123,27 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>63</v>
-      </c>
-      <c r="I63" s="1" t="str">
-        <f>"This is the long description for " &amp;B63 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Divergence. It is quite a long description!</v>
+        <v>70</v>
+      </c>
+      <c r="H63" t="s">
+        <v>115</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J63" t="s">
+        <v>117</v>
       </c>
       <c r="K63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.75">
+    <row r="64" spans="1:11" ht="157.5">
       <c r="A64" t="s">
         <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3020,11 +3159,16 @@
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>63</v>
-      </c>
-      <c r="I64" s="1" t="str">
-        <f>"This is the long description for " &amp;B64 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Visualizing Curl. It is quite a long description!</v>
+        <v>70</v>
+      </c>
+      <c r="H64" t="s">
+        <v>119</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J64" t="s">
+        <v>121</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
@@ -3035,7 +3179,7 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3049,16 +3193,16 @@
         <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G65" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H65" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
@@ -3069,7 +3213,7 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3082,10 +3226,10 @@
         <v>13</v>
       </c>
       <c r="F66" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I66" s="1" t="str">
         <f>"This is the long description for " &amp;B66 &amp;". It is quite a long description!"</f>
@@ -3100,7 +3244,7 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3116,7 +3260,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I67" s="1" t="str">
         <f>"This is the long description for " &amp;B67 &amp;". It is quite a long description!"</f>
@@ -3131,7 +3275,7 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3144,10 +3288,10 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G68" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I68" s="1" t="str">
         <f>"This is the long description for " &amp;B68 &amp;". It is quite a long description!"</f>
@@ -3162,7 +3306,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3175,10 +3319,10 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G69" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I69" s="1" t="str">
         <f>"This is the long description for " &amp;B69 &amp;". It is quite a long description!"</f>
@@ -3193,7 +3337,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3210,7 +3354,7 @@
         <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I70" s="1" t="str">
         <f>"This is the long description for " &amp;B70 &amp;". It is quite a long description!"</f>
@@ -3225,7 +3369,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3241,7 +3385,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I71" s="1" t="str">
         <f>"This is the long description for " &amp;B71 &amp;". It is quite a long description!"</f>
@@ -3256,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3270,13 +3414,13 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="G72" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H72" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="I72" s="1" t="str">
         <f>"This is the long description for " &amp;B72 &amp;". It is quite a long description!"</f>
@@ -3291,7 +3435,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3308,10 +3452,10 @@
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H73" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="I73" s="1" t="str">
         <f>"This is the long description for " &amp;B73 &amp;". It is quite a long description!"</f>
@@ -3326,7 +3470,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3343,10 +3487,10 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
@@ -3357,7 +3501,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3373,7 +3517,7 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I75" s="1" t="str">
         <f>"This is the long description for " &amp;B75 &amp;". It is quite a long description!"</f>
@@ -3388,7 +3532,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3404,7 +3548,7 @@
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="I76" s="1" t="str">
         <f>"This is the long description for " &amp;B76 &amp;". It is quite a long description!"</f>
@@ -3414,12 +3558,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.75">
+    <row r="77" spans="1:11" ht="110.25">
       <c r="A77" t="s">
         <v>46</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3434,28 +3578,30 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F77" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G77" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H77" t="s">
-        <v>117</v>
-      </c>
-      <c r="I77" s="1" t="str">
-        <f>"This is the long description for " &amp;B77 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Zapping with d. It is quite a long description!</v>
+        <v>144</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J77" t="s">
+        <v>146</v>
       </c>
       <c r="K77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="15.75">
+    <row r="78" spans="1:11" ht="110.25">
       <c r="A78" t="s">
         <v>46</v>
       </c>
       <c r="B78" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3470,14 +3616,19 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F78" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="G78" t="s">
-        <v>97</v>
-      </c>
-      <c r="I78" s="1" t="str">
-        <f>"This is the long description for " &amp;B78 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Energy and Integrals. It is quite a long description!</v>
+        <v>124</v>
+      </c>
+      <c r="H78" t="s">
+        <v>149</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J78" t="s">
+        <v>151</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -3488,7 +3639,7 @@
         <v>46</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3503,19 +3654,19 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F79" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="G79" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H79" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J79" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="K79" t="s">
         <v>15</v>
@@ -3526,7 +3677,7 @@
         <v>46</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3541,16 +3692,19 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F80" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G80" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H80" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>127</v>
+        <v>159</v>
+      </c>
+      <c r="J80" t="s">
+        <v>160</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
@@ -3573,7 +3727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EFD8F-45BF-44EB-A2B4-FA9451BFAEEC}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
+    <sheetView topLeftCell="A17" workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
@@ -3584,17 +3738,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.5">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="31.5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="71.25" customHeight="1"/>
@@ -3603,7 +3757,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="C28">
         <f>ROW()</f>
@@ -3634,7 +3788,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C29">
         <f>ROW()</f>
@@ -3665,7 +3819,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="C30">
         <f>ROW()</f>
@@ -3696,7 +3850,7 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -3710,7 +3864,7 @@
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
         <v>33</v>
@@ -3720,7 +3874,7 @@
         <v>This is the long description for Chain Rule Measurements. It is quite a long description!</v>
       </c>
       <c r="J34" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="K34" t="s">
         <v>15</v>
@@ -3731,7 +3885,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3745,16 +3899,16 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="G69" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H69" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
edits by Mike and Paul
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Mike's Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_21E2BB697F9D6CFAA84D0C82B8CBFECAF4C19DEE" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D916B437-619D-A841-9460-EF6305ADA5F3}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6700" yWindow="-23540" windowWidth="19200" windowHeight="22520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="840" windowWidth="14400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179016" concurrentCalc="0"/>
+  <calcPr calcId="179020" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="184">
   <si>
     <t>Act or Con</t>
   </si>
@@ -82,6 +82,9 @@
     <t>The derivative is a ratio of small changes</t>
   </si>
   <si>
+    <t>One can view $\frac{df}{dx}$ as a fraction where $df$ is a small change in $f$ and $dx$ is a small change in $x$.</t>
+  </si>
+  <si>
     <t>The derivative can be approximated by the slope of a secant line</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t>You can flip a derivative</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>In other words, $\frac{dy}{dx} = \frac{1}{\frac{dx}{dy}}$.  Note that this concept is challenging to express in Newton's notation, but arises naturally if implicit differentiation is covered.</t>
   </si>
   <si>
@@ -130,6 +136,9 @@
     <t>MTH 254</t>
   </si>
   <si>
+    <t xml:space="preserve">Derivatives of multivariable functions can be found by holding one ore more variables constant (subject to physical limitations). </t>
+  </si>
+  <si>
     <t>There is a  partial derivative in every direction at any point</t>
   </si>
   <si>
@@ -151,6 +160,9 @@
     <t>The gradient is a vector</t>
   </si>
   <si>
+    <t xml:space="preserve">For an $n-dimensional$ function $f$, the gradient of $f$ at a point is an $n$ dimensional vector </t>
+  </si>
+  <si>
     <t>The magnitude of the gradient is the value of the slope in the steepest direction</t>
   </si>
   <si>
@@ -166,9 +178,15 @@
     <t>Partial derivatives are functions</t>
   </si>
   <si>
+    <t xml:space="preserve">The partial derivative of a function (unless taken at a single point) is itself a function. </t>
+  </si>
+  <si>
     <t>The gradient is a function</t>
   </si>
   <si>
+    <t>The gradient of a function (unless taken at a single point) is itself a function</t>
+  </si>
+  <si>
     <t>The components of the gradient are partial derivatives</t>
   </si>
   <si>
@@ -178,10 +196,10 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>The heater II</t>
-  </si>
-  <si>
-    <t>mvheater2.png</t>
+    <t>The Heater II</t>
+  </si>
+  <si>
+    <t>mvheater2.jpg</t>
   </si>
   <si>
     <t>This small group activity is designed to help students interpret partial derivatives using contour diagrams. Students work in small groups to determine rates of change using a contour diagram showing isotherms over time and space. The whole class wrap-up discussion emphasizes giving a physical interpretation for the derivative, the value of units in thinking about functions and derivatives, and the need to specify “with respect to what” when finding derivatives in multivariable contexts.</t>
@@ -190,13 +208,13 @@
     <t>mvheater2</t>
   </si>
   <si>
-    <t>The hot plate</t>
+    <t>The Hot Plate</t>
   </si>
   <si>
     <t>[partial f/partial x, Contour Maps, Inclinometer]</t>
   </si>
   <si>
-    <t>mvhotplate.PNG</t>
+    <t>mvhotplate.jpg</t>
   </si>
   <si>
     <t>This small group activity using surfaces introduces a geometric interpretation of partial derivatives in terms of measured ratios of small changes. Students work in small groups to identify locations on their surface with particular properties. The whole class wrap-up discussion emphasizes the equivalence of multiple representations of partial derivatives.</t>
@@ -211,7 +229,7 @@
     <t>[partial f/partial x]</t>
   </si>
   <si>
-    <t>TreeDiagram.png</t>
+    <t>TreeDiagram.jpg</t>
   </si>
   <si>
     <t>This activity is still in development!</t>
@@ -247,7 +265,7 @@
     <t>[partial f/partial x, Inclinometer, Del f]</t>
   </si>
   <si>
-    <t>MathSurfaces1.png</t>
+    <t>MathSurfaces1.jpg</t>
   </si>
   <si>
     <t>This small group activity using surfaces relates the geometric definition of directional derivatives to the components of the gradient vector. Students work in small groups to measure a directional derivative directly, then compare its components with measured partial derivatives in rectangular coordinates. The whole class wrap-up discussion emphasizes the relationship between the geometric gradient vector and directional derivatives.</t>
@@ -274,6 +292,9 @@
     <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
   </si>
   <si>
+    <t>[df=\vec \nabla f \cdot d \vec r]</t>
+  </si>
+  <si>
     <t>The divergence is a scalar field</t>
   </si>
   <si>
@@ -322,6 +343,9 @@
     <t>The divergence is a function</t>
   </si>
   <si>
+    <t>The diverence of a function (unless taken at a single point) is itself a function</t>
+  </si>
+  <si>
     <t>The divergence is a local quantity</t>
   </si>
   <si>
@@ -448,10 +472,16 @@
     <t>Total differentials are linear</t>
   </si>
   <si>
+    <t>No matter how complicated a multivariable function is when written as an equation, the total differential of that function wil be linear in the differential terms. In other words: $dF(x,y,z)=A dx + B dy + C dz.$</t>
+  </si>
+  <si>
     <t>Differentials are small chunks</t>
   </si>
   <si>
     <t>There are experimental limits to how $small$ of a change can be measured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While it is relativly easy to imagine very, very small changes in physical values, there are often experimental limits on how small of a change can be measured. When designing and conducting experiments, there is a tension between these experimental limitations and normative representations of functions as smooth lines or </t>
   </si>
   <si>
     <t>The derivative can be interpreted physically</t>
@@ -585,18 +615,23 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -611,50 +646,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1348330</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>448733</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D6B4133-7B61-404A-932A-2467211E32E0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1007533" y="18177933"/>
-          <a:ext cx="1348330" cy="431800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -682,7 +673,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -726,7 +717,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -770,7 +761,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -814,7 +805,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1131,63 +1122,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="H12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.875" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37.625" customWidth="1"/>
     <col min="5" max="5" width="39.625" customWidth="1"/>
     <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="7" max="7" width="13.875" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="72.625" customWidth="1"/>
     <col min="10" max="10" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75">
+    <row r="2" spans="1:11" ht="32.1">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1210,15 +1201,15 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="str">
-        <f>"A long description for "&amp;B2 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I15" si="0">"A long description for "&amp;B2 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Difference / Change is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="31.5">
+    <row r="3" spans="1:11" ht="32.1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1241,15 +1232,15 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f>"A long description for "&amp;B3 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for How much $f$ changes as $x$ changes is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="32.1">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1272,20 +1263,19 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1" t="str">
-        <f>"A long description for "&amp;B4 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The derivative is a ratio of small changes is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="31.5">
+    <row r="5" spans="1:11" ht="32.1">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <f>ROW()</f>
@@ -1303,20 +1293,20 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1" t="str">
-        <f>"A long description for "&amp;B5 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative can be approximated by the slope of a secant line is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.5">
+    <row r="6" spans="1:11" ht="32.1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <f>ROW()</f>
@@ -1334,20 +1324,20 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1" t="str">
-        <f>"A long description for "&amp;B6 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative is the slope of a tangent line is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75">
+    <row r="7" spans="1:11" ht="32.1">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <f>ROW()</f>
@@ -1365,20 +1355,20 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="1" t="str">
-        <f>"A long description for "&amp;B7 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative is a limit is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75">
+    <row r="8" spans="1:11" ht="32.1">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <f>ROW()</f>
@@ -1396,20 +1386,20 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="1" t="str">
-        <f>"A long description for "&amp;B8 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative can be a function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75">
+    <row r="9" spans="1:11" ht="32.1">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <f>ROW()</f>
@@ -1427,20 +1417,20 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="1" t="str">
-        <f>"A long description for "&amp;B9 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative of a constant is zero is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75">
+    <row r="10" spans="1:11" ht="32.1">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <f>ROW()</f>
@@ -1458,20 +1448,20 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="1" t="str">
-        <f>"A long description for "&amp;B10 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative is a linear function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75">
+    <row r="11" spans="1:11" ht="32.1">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <f>ROW()</f>
@@ -1489,20 +1479,20 @@
       <c r="G11" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="1" t="str">
-        <f>"A long description for "&amp;B11 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for Power law is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
+    <row r="12" spans="1:11" ht="32.1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <f>ROW()</f>
@@ -1520,20 +1510,20 @@
       <c r="G12" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="1" t="str">
-        <f>"A long description for "&amp;B12 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for The derivative at a cusp is undefined is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75">
+    <row r="13" spans="1:11" ht="32.1">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <f>ROW()</f>
@@ -1551,20 +1541,20 @@
       <c r="G13" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="1" t="str">
-        <f>"A long description for "&amp;B13 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for Variables can be held constant is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75">
+    <row r="14" spans="1:11" ht="32.1">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <f>ROW()</f>
@@ -1582,20 +1572,20 @@
       <c r="G14" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="1" t="str">
-        <f>"A long description for "&amp;B14 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for Product rule is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
+    <row r="15" spans="1:11" ht="32.1">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <f>ROW()</f>
@@ -1613,8 +1603,8 @@
       <c r="G15" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="1" t="str">
-        <f>"A long description for "&amp;B15 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
         <v>A long description for Single variable chain rule is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K15" t="s">
@@ -1626,14 +1616,14 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <f>ROW()</f>
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -1644,19 +1634,19 @@
       <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>30</v>
+      <c r="I16" t="s">
+        <v>32</v>
       </c>
       <c r="K16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75">
+    <row r="17" spans="1:11" ht="32.1">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <f>ROW()</f>
@@ -1674,8 +1664,8 @@
       <c r="G17" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="1" t="str">
-        <f>"A long description for "&amp;B17 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17:I27" si="1">"A long description for "&amp;B17 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for "With respect to what" matters is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K17" t="s">
@@ -1687,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <f>ROW()</f>
@@ -1704,22 +1694,21 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f>"A long description for "&amp;B18 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for Derivatives can be found while holding one or more variables constant is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="31.5">
+    <row r="19" spans="1:11" ht="32.1">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <f>ROW()</f>
@@ -1735,53 +1724,53 @@
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f>"A long description for "&amp;B19 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for There is a  partial derivative in every direction at any point is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="31.5">
+    <row r="20" spans="1:11" ht="32.1">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <f>ROW()</f>
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
         <v>35</v>
       </c>
-      <c r="C20">
-        <f>ROW()</f>
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f>"A long description for "&amp;B20 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for There is a tangent line in every direction at every point is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="31.5">
+    <row r="21" spans="1:11" ht="32.1">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <f>ROW()</f>
@@ -1794,25 +1783,25 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f>"A long description for "&amp;B21 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for The derivative is related to the density of contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="47.25">
+    <row r="22" spans="1:11" ht="48">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <f>ROW()</f>
@@ -1828,22 +1817,22 @@
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f>"A long description for "&amp;B22 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for The value of a partial derivative depends on the value(s) of what is held constant is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="31.5">
+    <row r="23" spans="1:11" ht="32.1">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <f>ROW()</f>
@@ -1860,22 +1849,22 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f>"A long description for "&amp;B23 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for A partial derivative can be expressed in terms of other partial derivatives is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75">
+    <row r="24" spans="1:11" ht="32.1">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <f>ROW()</f>
@@ -1891,19 +1880,18 @@
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f>"A long description for "&amp;B24 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The gradient is a vector is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="47.25">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="48">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25">
         <f>ROW()</f>
@@ -1920,22 +1908,22 @@
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f>"A long description for "&amp;B25 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for The magnitude of the gradient is the value of the slope in the steepest direction is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="31.5">
+    <row r="26" spans="1:11" ht="32.1">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C26">
         <f>ROW()</f>
@@ -1948,25 +1936,25 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f>"A long description for "&amp;B26 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for The gradient is perpendicular to contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="31.5">
+    <row r="27" spans="1:11" ht="48">
       <c r="A27" t="s">
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <f>ROW()</f>
@@ -1983,22 +1971,22 @@
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f>"A long description for "&amp;B27 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>35</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
         <v>A long description for All partial derivatives can be found as a slope of a tangent plane is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75">
+    <row r="28" spans="1:11" ht="32.1">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <f>ROW()</f>
@@ -2014,9 +2002,9 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
-      </c>
-      <c r="I28" s="1" t="str">
+        <v>35</v>
+      </c>
+      <c r="I28" t="str">
         <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
         <v>This is the long description for The derivative is local quantity. It is quite a long description!</v>
       </c>
@@ -2024,12 +2012,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C29">
         <f>ROW()</f>
@@ -2045,22 +2033,21 @@
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="1" t="str">
-        <f>"This is the long description for " &amp;B29 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for Partial derivatives are functions. It is quite a long description!</v>
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>50</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <f>ROW()</f>
@@ -2076,22 +2063,21 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="1" t="str">
-        <f>"This is the long description for " &amp;B30 &amp;". It is quite a long description!"</f>
-        <v>This is the long description for The gradient is a function. It is quite a long description!</v>
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
       </c>
       <c r="K30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="31.5">
+    <row r="31" spans="1:11" ht="32.1">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>28</v>
@@ -2106,10 +2092,10 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
       </c>
       <c r="K31" t="s">
         <v>15</v>
@@ -2117,10 +2103,10 @@
     </row>
     <row r="32" spans="1:11" ht="94.5">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2135,19 +2121,19 @@
         <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="I32" t="s">
+        <v>58</v>
       </c>
       <c r="J32" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K32" t="s">
         <v>15</v>
@@ -2155,10 +2141,10 @@
     </row>
     <row r="33" spans="1:11" ht="78.75">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2173,19 +2159,19 @@
         <v>[There is a  partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H33" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="I33" t="s">
+        <v>63</v>
       </c>
       <c r="J33" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
@@ -2193,10 +2179,10 @@
     </row>
     <row r="34" spans="1:11" ht="71.25" customHeight="1">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2211,30 +2197,30 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="I34" t="s">
+        <v>68</v>
       </c>
       <c r="J34" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="31.5">
+    <row r="35" spans="1:11" ht="48">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2248,28 +2234,28 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
-      </c>
-      <c r="I35" s="1" t="str">
+        <v>35</v>
+      </c>
+      <c r="I35" t="str">
         <f>"This is the long description for " &amp;B35 &amp;". It is quite a long description!"</f>
         <v>This is the long description for Chain Rule Measurements. It is quite a long description!</v>
       </c>
       <c r="J35" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="63">
+    <row r="36" spans="1:11" ht="96">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2284,19 +2270,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H36" t="s">
-        <v>68</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
+      </c>
+      <c r="I36" t="s">
+        <v>75</v>
       </c>
       <c r="J36" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K36" t="s">
         <v>15</v>
@@ -2304,10 +2290,10 @@
     </row>
     <row r="37" spans="1:11" ht="94.5">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2322,30 +2308,30 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F37" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="I37" t="s">
+        <v>80</v>
       </c>
       <c r="J37" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="K37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="33.950000000000003" customHeight="1">
+    <row r="38" spans="1:11" ht="48">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2361,9 +2347,9 @@
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="I38" t="str">
         <f>"A long description for "&amp;B38 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Each component of $d \vec r$ is an arbitrary small change between two arbitrary position vectors.  is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -2376,7 +2362,7 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2392,9 +2378,9 @@
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="1" t="str">
+        <v>85</v>
+      </c>
+      <c r="I39" t="str">
         <f>"A long description for "&amp;B39 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The magnitude of $d\vec r$ is the length of a small step along a path is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -2407,7 +2393,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
@@ -2423,9 +2409,9 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>79</v>
-      </c>
-      <c r="I40" s="1" t="str">
+        <v>85</v>
+      </c>
+      <c r="I40" t="str">
         <f>"A long description for "&amp;B40 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The direction of $d\vec r$ is tangent to a path is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -2433,12 +2419,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="47.25">
+    <row r="41" spans="1:11" ht="48">
       <c r="A41" t="s">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2451,12 +2437,12 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="I41" t="str">
         <f>"A long description for "&amp;B41 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The gradient can tell you a small change in a function in any direction (differentials edition) is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -2464,12 +2450,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75">
+    <row r="42" spans="1:11" ht="32.1">
       <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
@@ -2484,7 +2470,7 @@
       <c r="F42" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="1" t="str">
+      <c r="I42" t="str">
         <f>"A long description for "&amp;B42 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The divergence is a scalar field is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -2510,9 +2496,8 @@
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>77</v>
-      </c>
-      <c r="I43" s="1"/>
+        <v>83</v>
+      </c>
       <c r="K43" t="s">
         <v>15</v>
       </c>
@@ -2535,34 +2520,32 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" s="1"/>
+        <v>83</v>
+      </c>
       <c r="K44" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="45" customHeight="1">
       <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45">
+        <f>ROW()</f>
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
         <v>83</v>
       </c>
-      <c r="C45">
-        <f>ROW()</f>
-        <v>45</v>
-      </c>
-      <c r="D45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>77</v>
-      </c>
-      <c r="I45" s="1"/>
       <c r="K45" t="s">
         <v>15</v>
       </c>
@@ -2585,19 +2568,18 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" s="1"/>
+        <v>83</v>
+      </c>
       <c r="K46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="94.5">
+    <row r="47" spans="1:11" ht="111.95">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2612,30 +2594,30 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H47" t="s">
-        <v>68</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
+      </c>
+      <c r="I47" t="s">
+        <v>93</v>
       </c>
       <c r="J47" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="94.5">
+    <row r="48" spans="1:11" ht="96">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2650,30 +2632,30 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G48" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H48" t="s">
-        <v>89</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
+      </c>
+      <c r="I48" t="s">
+        <v>97</v>
       </c>
       <c r="J48" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="K48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="31.5">
+    <row r="49" spans="1:11" ht="32.1">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2690,22 +2672,22 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>79</v>
-      </c>
-      <c r="I49" s="1" t="str">
-        <f>"A long description for "&amp;B49 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" ref="I49:I63" si="2">"A long description for "&amp;B49 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Differential form of $\vec r$ in spherical and cylindrical coordinates is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K49" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="47.25">
+    <row r="50" spans="1:11" ht="48">
       <c r="A50" t="s">
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -2721,22 +2703,22 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I50" s="1" t="str">
-        <f>"A long description for "&amp;B50 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The gradient's dimension is the same as real space. The gradient lives in the domain is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.75">
+    <row r="51" spans="1:11" ht="32.1">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2753,22 +2735,22 @@
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>79</v>
-      </c>
-      <c r="I51" s="1" t="str">
-        <f>"A long description for "&amp;B51 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The gradient is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="31.5">
+    <row r="52" spans="1:11" ht="32.1">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -2784,22 +2766,22 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>79</v>
-      </c>
-      <c r="I52" s="1" t="str">
-        <f>"A long description for "&amp;B52 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The electric field is the negative gradient of the electric potential is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="31.5">
+    <row r="53" spans="1:11" ht="32.1">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -2815,22 +2797,22 @@
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>79</v>
-      </c>
-      <c r="I53" s="1" t="str">
-        <f>"A long description for "&amp;B53 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The divergence is related to the total flux through a closed surface is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.75">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -2846,22 +2828,21 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>79</v>
-      </c>
-      <c r="I54" s="1" t="str">
-        <f>"A long description for "&amp;B54 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The divergence is a function is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>85</v>
+      </c>
+      <c r="I54" t="s">
+        <v>105</v>
       </c>
       <c r="K54" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.75">
+    <row r="55" spans="1:11" ht="32.1">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -2878,22 +2859,22 @@
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>79</v>
-      </c>
-      <c r="I55" s="1" t="str">
-        <f>"A long description for "&amp;B55 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The divergence is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="31.5">
+    <row r="56" spans="1:11" ht="32.1">
       <c r="A56" t="s">
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -2909,22 +2890,22 @@
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>79</v>
-      </c>
-      <c r="I56" s="1" t="str">
-        <f>"A long description for "&amp;B56 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The divergence of the electric field is equal to is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="31.5">
+    <row r="57" spans="1:11" ht="32.1">
       <c r="A57" t="s">
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -2940,22 +2921,22 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>79</v>
-      </c>
-      <c r="I57" s="1" t="str">
-        <f>"A long description for "&amp;B57 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The divergence of the magnetic field is zero is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="31.5">
+    <row r="58" spans="1:11" ht="48">
       <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -2971,22 +2952,22 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>79</v>
-      </c>
-      <c r="I58" s="1" t="str">
-        <f>"A long description for "&amp;B58 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The curl is related to the line integral around a closed loop. ("circulation") is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K58" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.75">
+    <row r="59" spans="1:11" ht="32.1">
       <c r="A59" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -3002,22 +2983,22 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>79</v>
-      </c>
-      <c r="I59" s="1" t="str">
-        <f>"A long description for "&amp;B59 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for the curl is a (vector) function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K59" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.75">
+    <row r="60" spans="1:11" ht="32.1">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -3034,22 +3015,22 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>79</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f>"A long description for "&amp;B60 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The curl is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="31.5">
+    <row r="61" spans="1:11" ht="32.1">
       <c r="A61" t="s">
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -3065,22 +3046,22 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>79</v>
-      </c>
-      <c r="I61" s="1" t="str">
-        <f>"A long description for "&amp;B61 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The magnetic field is equal to the curl of the magnetic vector potential is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="31.5">
+    <row r="62" spans="1:11" ht="32.1">
       <c r="A62" t="s">
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -3096,22 +3077,22 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>79</v>
-      </c>
-      <c r="I62" s="1" t="str">
-        <f>"A long description for "&amp;B62 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The curl of the electric field is zero in electrostatics is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="47.25">
+    <row r="63" spans="1:11" ht="48">
       <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -3127,22 +3108,22 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>79</v>
-      </c>
-      <c r="I63" s="1" t="str">
-        <f>"A long description for "&amp;B63 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>85</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="2"/>
         <v>A long description for The divergence of the curl is equal to mu times the current in magneto-statics is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="94.5">
+    <row r="64" spans="1:11" ht="96">
       <c r="A64" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3157,30 +3138,30 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F64" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G64" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H64" t="s">
-        <v>109</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
+      </c>
+      <c r="I64" t="s">
+        <v>118</v>
       </c>
       <c r="J64" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="126">
+    <row r="65" spans="1:11" ht="128.1">
       <c r="A65" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3195,30 +3176,30 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F65" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G65" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H65" t="s">
-        <v>114</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
+      </c>
+      <c r="I65" t="s">
+        <v>123</v>
       </c>
       <c r="J65" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="110.25">
+    <row r="66" spans="1:11" ht="111.95">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3233,30 +3214,30 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G66" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H66" t="s">
-        <v>119</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
+      </c>
+      <c r="I66" t="s">
+        <v>128</v>
       </c>
       <c r="J66" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="157.5">
+    <row r="67" spans="1:11" ht="159.94999999999999">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3271,30 +3252,30 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F67" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="G67" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H67" t="s">
-        <v>124</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
+      </c>
+      <c r="I67" t="s">
+        <v>133</v>
       </c>
       <c r="J67" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="157.5">
+    <row r="68" spans="1:11" ht="159.94999999999999">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3309,30 +3290,30 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F68" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="G68" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H68" t="s">
-        <v>128</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
+      </c>
+      <c r="I68" t="s">
+        <v>137</v>
       </c>
       <c r="J68" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="126">
+    <row r="69" spans="1:11" ht="128.1">
       <c r="A69" t="s">
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3346,27 +3327,27 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H69" t="s">
-        <v>134</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
+      </c>
+      <c r="I69" t="s">
+        <v>143</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="31.5">
+    <row r="70" spans="1:11" ht="32.1">
       <c r="A70" t="s">
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3379,25 +3360,25 @@
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="G70" t="s">
-        <v>133</v>
-      </c>
-      <c r="I70" s="1" t="str">
-        <f>"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>141</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" ref="I70:I77" si="3">"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Equations can be 'zapped with d' to relate differentials is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K70" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="31.5">
+    <row r="71" spans="1:11" ht="32.1">
       <c r="A71" t="s">
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3413,22 +3394,22 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>133</v>
-      </c>
-      <c r="I71" s="1" t="str">
-        <f>"A long description for "&amp;B71 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>141</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="3"/>
         <v>A long description for Individual differentials can be manipulated algebraically is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.75">
+    <row r="72" spans="1:11" ht="48">
       <c r="A72" t="s">
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3441,56 +3422,55 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>133</v>
-      </c>
-      <c r="I72" s="1" t="str">
-        <f>"A long description for "&amp;B72 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for Total differentials are linear is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>141</v>
+      </c>
+      <c r="I72" t="s">
+        <v>148</v>
       </c>
       <c r="K72" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.75">
+    <row r="73" spans="1:11" ht="32.1">
       <c r="A73" t="s">
         <v>11</v>
       </c>
       <c r="B73" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73">
+        <f>ROW()</f>
+        <v>73</v>
+      </c>
+      <c r="D73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" t="s">
         <v>140</v>
       </c>
-      <c r="C73">
-        <f>ROW()</f>
-        <v>73</v>
-      </c>
-      <c r="D73" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" t="s">
-        <v>132</v>
-      </c>
       <c r="G73" t="s">
-        <v>133</v>
-      </c>
-      <c r="I73" s="1" t="str">
-        <f>"A long description for "&amp;B73 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for Differentials are small chunks is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>141</v>
+      </c>
+      <c r="I73" t="str">
+        <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
+        <v>$df$ can be viewed as a small chunk of $f$. When combined with 'The derivative is a ratio of small changes', it's easy to relate differentials to derivatives.</v>
       </c>
       <c r="K73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="47.25">
+    <row r="74" spans="1:11" ht="78.75">
       <c r="A74" t="s">
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3507,22 +3487,21 @@
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>133</v>
-      </c>
-      <c r="I74" s="1" t="str">
-        <f>"A long description for "&amp;B74 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for There are experimental limits to how $small$ of a change can be measured is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>141</v>
+      </c>
+      <c r="I74" t="s">
+        <v>151</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="31.5">
+    <row r="75" spans="1:11" ht="32.1">
       <c r="A75" t="s">
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3538,22 +3517,22 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>133</v>
-      </c>
-      <c r="I75" s="1" t="str">
-        <f>"A long description for "&amp;B75 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>141</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="3"/>
         <v>A long description for The derivative can be interpreted physically is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K75" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="110.25">
+    <row r="76" spans="1:11" ht="96">
       <c r="A76" t="s">
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3567,16 +3546,16 @@
         <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="G76" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H76" t="s">
-        <v>145</v>
-      </c>
-      <c r="I76" s="1" t="str">
-        <f>"A long description for "&amp;B76 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>155</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="3"/>
         <v>A long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K76" t="s">
@@ -3588,7 +3567,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3605,25 +3584,25 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H77" t="s">
-        <v>147</v>
-      </c>
-      <c r="I77" s="1" t="str">
-        <f>"A long description for "&amp;B77 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
+        <v>157</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="3"/>
         <v>A long description for Partial derivatives are coefficients in a differentials equation is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="78.75">
+    <row r="78" spans="1:11" ht="80.099999999999994">
       <c r="A78" t="s">
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3640,21 +3619,21 @@
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>133</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
+      </c>
+      <c r="I78" t="s">
+        <v>159</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="31.5">
+    <row r="79" spans="1:11" ht="48">
       <c r="A79" t="s">
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3670,9 +3649,9 @@
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>133</v>
-      </c>
-      <c r="I79" s="1" t="str">
+        <v>141</v>
+      </c>
+      <c r="I79" t="str">
         <f>"A long description for "&amp;B79 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for There might be experimental limits on which quantities you can measure is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -3680,12 +3659,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="47.25">
+    <row r="80" spans="1:11" ht="48">
       <c r="A80" t="s">
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3701,9 +3680,9 @@
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>133</v>
-      </c>
-      <c r="I80" s="1" t="str">
+        <v>141</v>
+      </c>
+      <c r="I80" t="str">
         <f>"A long description for "&amp;B80 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Differentials allow the finding of partial derivatives when a variable cannot be solved for is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
@@ -3711,12 +3690,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="110.25">
+    <row r="81" spans="1:11" ht="111.95">
       <c r="A81" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B81" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3731,30 +3710,30 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G81" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H81" t="s">
-        <v>153</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="I81" t="s">
+        <v>164</v>
       </c>
       <c r="J81" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="K81" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="110.25">
+    <row r="82" spans="1:11" ht="111.95">
       <c r="A82" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3769,19 +3748,19 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F82" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G82" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H82" t="s">
-        <v>158</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
+      </c>
+      <c r="I82" t="s">
+        <v>169</v>
       </c>
       <c r="J82" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="K82" t="s">
         <v>15</v>
@@ -3789,10 +3768,10 @@
     </row>
     <row r="83" spans="1:11" ht="93" customHeight="1">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -3807,30 +3786,30 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="G83" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H83" t="s">
-        <v>163</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
+      </c>
+      <c r="I83" t="s">
+        <v>174</v>
       </c>
       <c r="J83" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="K83" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="94.5">
+    <row r="84" spans="1:11" ht="240">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -3845,33 +3824,30 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G84" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H84" t="s">
-        <v>167</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
+      </c>
+      <c r="I84" t="s">
+        <v>178</v>
       </c>
       <c r="J84" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="K84" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.75"/>
-    <row r="86" spans="1:11" ht="15.75"/>
-    <row r="87" spans="1:11" ht="15.75"/>
-    <row r="88" spans="1:11" ht="15.75"/>
-    <row r="89" spans="1:11" ht="15.75"/>
-    <row r="91" spans="1:11" ht="15.75"/>
-    <row r="92" spans="1:11" ht="15.75"/>
-    <row r="93" spans="1:11" ht="15.75"/>
   </sheetData>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="A long description">
+      <formula>NOT(ISERROR(SEARCH("A long description",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -3886,42 +3862,33 @@
       <selection activeCell="A34" sqref="A34:K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="47.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="31.5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="31.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="71.25" customHeight="1"/>
-    <row r="28" spans="9:9">
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="9:9">
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="9:9">
-      <c r="I30" s="1"/>
-    </row>
     <row r="69" spans="1:11" ht="409.6">
       <c r="A69" t="s">
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3935,16 +3902,16 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G69" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H69" t="s">
-        <v>134</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
+      </c>
+      <c r="I69" t="s">
+        <v>143</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
changes by mike and fix error in parse_list when given empty string
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827A923D-11CA-384A-A682-892EA15CA3AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5C55F-D180-A94E-BA0F-B558CA1C4D8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-13320" windowWidth="38400" windowHeight="22700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="-13320" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="214">
   <si>
     <t>Act or Con</t>
   </si>
@@ -362,9 +361,6 @@
     <t>Vector Differentials</t>
   </si>
   <si>
-    <t>[df, 3D plots]</t>
-  </si>
-  <si>
     <t>vfdrvectorcurvi.jpg</t>
   </si>
   <si>
@@ -434,9 +430,6 @@
     <t>Differentials are small changes or differences</t>
   </si>
   <si>
-    <t>[df]</t>
-  </si>
-  <si>
     <t>PH 423</t>
   </si>
   <si>
@@ -449,9 +442,6 @@
     <t>Equations can be 'zapped with d' to relate differentials</t>
   </si>
   <si>
-    <t>[p]</t>
-  </si>
-  <si>
     <t>Individual differentials can be manipulated algebraically</t>
   </si>
   <si>
@@ -470,9 +460,6 @@
     <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
   </si>
   <si>
-    <t>[$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$]</t>
-  </si>
-  <si>
     <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
   </si>
   <si>
@@ -602,9 +589,6 @@
     <t>The divergence at a point is a scalar. Taking the divergence of a function yields a scalar at every value in the domain of that function: a scalar field</t>
   </si>
   <si>
-    <t>[$df=\vec \nabla f \cdot d \vec r$]</t>
-  </si>
-  <si>
     <t>Always or just when taking a derivative?</t>
   </si>
   <si>
@@ -639,16 +623,68 @@
   </si>
   <si>
     <t>There is a partial derivative in every direction at any point</t>
+  </si>
+  <si>
+    <t>Name the Experiment (x3)</t>
+  </si>
+  <si>
+    <t>Mixed Partials</t>
+  </si>
+  <si>
+    <t>Maxwell's Relations</t>
+  </si>
+  <si>
+    <t>[$\Delta x$]</t>
+  </si>
+  <si>
+    <t>[$\frac{\Delta f}{\Delta x}$]</t>
+  </si>
+  <si>
+    <t>[$\frac{d f}{d x},\frac{\partial f}{\partial x},\left(\frac{\partial f}{\partial x}\right)_y$]</t>
+  </si>
+  <si>
+    <t>[$\left(\frac{\partial f}{\partial x}\right)_y$]</t>
+  </si>
+  <si>
+    <t>$df=\vec \nabla f \cdot d \vec r$</t>
+  </si>
+  <si>
+    <t>[$\vec \Nabla f, d\vec r$]</t>
+  </si>
+  <si>
+    <t>[$\vec \nabla \cdot \vec v$]</t>
+  </si>
+  <si>
+    <t>[$\vec \nabla \times \vec v$]</t>
+  </si>
+  <si>
+    <t>[$d \vec r$]</t>
+  </si>
+  <si>
+    <t>[Experiment]</t>
+  </si>
+  <si>
+    <t>[$df$]</t>
+  </si>
+  <si>
+    <t>[$df$, 3D plots]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -682,7 +718,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -692,11 +728,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -715,27 +754,9 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -753,460 +774,9 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -1359,8 +929,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>569310</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1404,7 +974,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1969379</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1737,16 +1307,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" customWidth="1"/>
@@ -1794,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -1815,13 +1385,13 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -1851,7 +1421,7 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -1875,7 +1445,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1918,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -1926,7 +1496,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C6">
         <f>ROW()</f>
@@ -1952,7 +1522,7 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -2172,7 +1742,7 @@
         <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2199,7 +1769,7 @@
         <v>14</v>
       </c>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K14" t="s">
         <v>15</v>
@@ -2229,16 +1799,16 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="K15" t="s">
         <v>15</v>
       </c>
       <c r="L15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2256,7 +1826,7 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -2293,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K17" t="s">
         <v>15</v>
@@ -2318,7 +1888,7 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>205</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
@@ -2335,7 +1905,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C19">
         <f>ROW()</f>
@@ -2441,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>205</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
@@ -2867,7 +2437,7 @@
         <v>33</v>
       </c>
       <c r="I35" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="J35" t="s">
         <v>69</v>
@@ -3066,14 +2636,13 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="G41" t="s">
         <v>80</v>
       </c>
-      <c r="I41" t="str">
-        <f>"A long description for "&amp;B41 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The gradient can tell you a small change in a function in any direction (differentials edition) is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I41" t="s">
+        <v>206</v>
       </c>
       <c r="K41" t="s">
         <v>15</v>
@@ -3097,10 +2666,10 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>13</v>
+        <v>208</v>
       </c>
       <c r="I42" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K42" t="s">
         <v>15</v>
@@ -3121,8 +2690,8 @@
       <c r="E43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>13</v>
+      <c r="F43" t="s">
+        <v>208</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>80</v>
@@ -3134,7 +2703,7 @@
         <v>15</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
@@ -3152,8 +2721,8 @@
       <c r="E44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>13</v>
+      <c r="F44" t="s">
+        <v>209</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>80</v>
@@ -3165,7 +2734,7 @@
         <v>15</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,7 +2765,7 @@
         <v>15</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3227,7 +2796,7 @@
         <v>15</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="112" x14ac:dyDescent="0.2">
@@ -3306,7 +2875,7 @@
         <v>15</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -3328,7 +2897,7 @@
         <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
+        <v>210</v>
       </c>
       <c r="G49" t="s">
         <v>82</v>
@@ -3490,7 +3059,7 @@
         <v>82</v>
       </c>
       <c r="I54" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K54" t="s">
         <v>15</v>
@@ -3797,19 +3366,19 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F64" t="s">
-        <v>111</v>
+        <v>213</v>
       </c>
       <c r="G64" t="s">
         <v>82</v>
       </c>
       <c r="H64" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" t="s">
         <v>112</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>113</v>
-      </c>
-      <c r="J64" t="s">
-        <v>114</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
@@ -3820,7 +3389,7 @@
         <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3835,19 +3404,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G65" t="s">
         <v>82</v>
       </c>
       <c r="H65" t="s">
+        <v>116</v>
+      </c>
+      <c r="I65" t="s">
         <v>117</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>118</v>
-      </c>
-      <c r="J65" t="s">
-        <v>119</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
@@ -3858,7 +3427,7 @@
         <v>52</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3873,19 +3442,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G66" t="s">
         <v>82</v>
       </c>
       <c r="H66" t="s">
+        <v>121</v>
+      </c>
+      <c r="I66" t="s">
         <v>122</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>123</v>
-      </c>
-      <c r="J66" t="s">
-        <v>124</v>
       </c>
       <c r="K66" t="s">
         <v>15</v>
@@ -3896,7 +3465,7 @@
         <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3911,19 +3480,19 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G67" t="s">
         <v>82</v>
       </c>
       <c r="H67" t="s">
+        <v>126</v>
+      </c>
+      <c r="I67" t="s">
         <v>127</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>128</v>
-      </c>
-      <c r="J67" t="s">
-        <v>129</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
@@ -3934,7 +3503,7 @@
         <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3949,19 +3518,19 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G68" t="s">
         <v>82</v>
       </c>
       <c r="H68" t="s">
+        <v>130</v>
+      </c>
+      <c r="I68" t="s">
         <v>131</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>132</v>
-      </c>
-      <c r="J68" t="s">
-        <v>133</v>
       </c>
       <c r="K68" t="s">
         <v>15</v>
@@ -3972,7 +3541,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3986,16 +3555,16 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
+        <v>212</v>
+      </c>
+      <c r="G69" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" t="s">
         <v>135</v>
       </c>
-      <c r="G69" t="s">
-        <v>136</v>
-      </c>
-      <c r="H69" t="s">
-        <v>137</v>
-      </c>
       <c r="I69" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>
@@ -4006,7 +3575,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -4019,10 +3588,10 @@
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="G70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ref="I70:I77" si="3">"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -4032,7 +3601,7 @@
         <v>15</v>
       </c>
       <c r="L70" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -4040,7 +3609,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -4056,7 +3625,7 @@
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="3"/>
@@ -4071,7 +3640,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -4084,13 +3653,13 @@
         <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="G72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I72" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K72" t="s">
         <v>15</v>
@@ -4101,7 +3670,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -4114,10 +3683,10 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="G73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I73" t="str">
         <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
@@ -4132,7 +3701,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -4146,13 +3715,13 @@
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>13</v>
+        <v>211</v>
       </c>
       <c r="G74" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I74" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
@@ -4163,7 +3732,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -4179,16 +3748,16 @@
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I75" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K75" t="s">
         <v>15</v>
       </c>
       <c r="L75" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="96" x14ac:dyDescent="0.2">
@@ -4196,7 +3765,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -4210,13 +3779,13 @@
         <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="G76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="3"/>
@@ -4231,7 +3800,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -4248,10 +3817,10 @@
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H77" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="3"/>
@@ -4266,7 +3835,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -4280,13 +3849,13 @@
         <v>13</v>
       </c>
       <c r="F78" t="s">
-        <v>13</v>
+        <v>205</v>
       </c>
       <c r="G78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I78" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K78" t="s">
         <v>15</v>
@@ -4297,7 +3866,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -4310,13 +3879,13 @@
         <v>13</v>
       </c>
       <c r="F79" t="s">
-        <v>13</v>
+        <v>211</v>
       </c>
       <c r="G79" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I79" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K79" t="s">
         <v>15</v>
@@ -4327,7 +3896,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -4340,14 +3909,14 @@
       <c r="E80" t="s">
         <v>13</v>
       </c>
-      <c r="F80" t="s">
-        <v>13</v>
+      <c r="F80" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="G80" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I80" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
@@ -4358,7 +3927,7 @@
         <v>52</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -4372,20 +3941,20 @@
         <f>"["&amp;B69&amp;", "&amp;B70&amp;", "&amp;B71&amp;", "&amp;B72&amp;"]"</f>
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
-      <c r="F81" t="s">
-        <v>135</v>
+      <c r="F81" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="G81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H81" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I81" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J81" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K81" t="s">
         <v>15</v>
@@ -4396,7 +3965,7 @@
         <v>52</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -4411,19 +3980,19 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F82" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G82" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H82" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I82" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J82" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K82" t="s">
         <v>15</v>
@@ -4434,7 +4003,7 @@
         <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -4449,19 +4018,19 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G83" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H83" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I83" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J83" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K83" t="s">
         <v>15</v>
@@ -4472,7 +4041,7 @@
         <v>52</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -4486,62 +4055,97 @@
         <f>"["&amp;B78&amp;", "&amp;B79&amp;", "&amp;B80&amp;"]"</f>
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
-      <c r="F84" t="s">
-        <v>135</v>
+      <c r="F84" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="G84" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H84" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I84" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J84" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K84" t="s">
         <v>15</v>
       </c>
       <c r="L84" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L85" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L87" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L88" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L89" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="A long description">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="A long description">
       <formula>NOT(ISERROR(SEARCH("A long description",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="A long description">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="A long description">
       <formula>NOT(ISERROR(SEARCH("A long description",I46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(L2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$D1="[]"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" dxfId="8" priority="3">
+  <conditionalFormatting sqref="E1:E84 E86:E1048576">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>AND($E1="[]",$A1="Activity")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="7" priority="2">
+  <conditionalFormatting sqref="F82:F83 F85:F1048576 F1:F79">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$F1="[]"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="J1:J84 J86:J1048576">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND($J1="",$A1="Activity")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85">
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>AND($E85="[]",$L85="Activity")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J85">
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>AND($J85="",$L85="Activity")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4565,17 +4169,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4584,7 +4188,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -4598,16 +4202,16 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G69" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" t="s">
+        <v>135</v>
+      </c>
+      <c r="I69" t="s">
         <v>136</v>
-      </c>
-      <c r="H69" t="s">
-        <v>137</v>
-      </c>
-      <c r="I69" t="s">
-        <v>138</v>
       </c>
       <c r="K69" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
work on representations page and long description
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5C55F-D180-A94E-BA0F-B558CA1C4D8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5C55F-D180-A94E-BA0F-B558CA1C4D8A}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-13320" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179020" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="215">
   <si>
     <t>Act or Con</t>
   </si>
@@ -61,6 +61,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Concept</t>
   </si>
   <si>
@@ -70,24 +73,45 @@
     <t>[]</t>
   </si>
   <si>
+    <t>[$\Delta x$]</t>
+  </si>
+  <si>
     <t>MTH 251</t>
   </si>
   <si>
+    <t>Understanding difference (how far apart two values are at one time) and change (how far apart the value of a single parameter is at two different times) is necessary for understanding derivatives.</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
     <t>How much $f$ changes as $x$ changes</t>
   </si>
   <si>
+    <t xml:space="preserve">Conceptually, a derivative can be thought of as how much one value changes as another value changes. </t>
+  </si>
+  <si>
     <t>The derivative is a ratio of small changes</t>
   </si>
   <si>
+    <t>[$\frac{\Delta f}{\Delta x}$]</t>
+  </si>
+  <si>
     <t>One can view $\frac{df}{dx}$ as a fraction where $df$ is a small change in $f$ and $dx$ is a small change in $x$.</t>
   </si>
   <si>
     <t>The derivative can be approximated by the slope of a secant line</t>
   </si>
   <si>
+    <t>Do we need to define a secant line? That seems like too much.</t>
+  </si>
+  <si>
+    <t>The derivative at a point is the slope of a tangent line at that point</t>
+  </si>
+  <si>
+    <t>Do we need to define a tangent line? That seems like too much.</t>
+  </si>
+  <si>
     <t>The derivative is a limit</t>
   </si>
   <si>
@@ -109,30 +133,54 @@
     <t>Variables can be held constant</t>
   </si>
   <si>
+    <t>Always or just when taking a derivative?</t>
+  </si>
+  <si>
     <t>Product rule</t>
   </si>
   <si>
+    <t>$\frac{d}{dt}(xy)=x\frac{dy}{dt}+y\frac{dx}{dt}$</t>
+  </si>
+  <si>
     <t>Single variable chain rule</t>
   </si>
   <si>
+    <t>$\frac{df}{dy}=\frac{df}{dx}\frac{dx}{dy}$</t>
+  </si>
+  <si>
+    <t>Add more</t>
+  </si>
+  <si>
     <t>You can flip a derivative</t>
   </si>
   <si>
+    <t>[$\frac{d f}{d x},\frac{\partial f}{\partial x},\left(\frac{\partial f}{\partial x}\right)_y$]</t>
+  </si>
+  <si>
     <t>In other words, $\frac{dy}{dx} = \frac{1}{\frac{dx}{dy}}$.  Note that this concept is challenging to express in Newton's notation, but arises naturally if implicit differentiation is covered.</t>
   </si>
   <si>
     <t>"With respect to what" matters</t>
   </si>
   <si>
+    <t xml:space="preserve">Taking derivatives of the same function with respect to different variables will produce different results. In physics, these different results might have different dimensions and thus the derivative can have wildly different physical interpretations based off of "'with respect to' what". </t>
+  </si>
+  <si>
     <t>Derivatives can be found while holding one or more variables constant</t>
   </si>
   <si>
+    <t>[$\left(\frac{\partial f}{\partial x}\right)_y$]</t>
+  </si>
+  <si>
     <t>MTH 254</t>
   </si>
   <si>
     <t xml:space="preserve">Derivatives of multivariable functions can be found by holding one ore more variables constant (subject to physical limitations). </t>
   </si>
   <si>
+    <t>There is a partial derivative in every direction at any point</t>
+  </si>
+  <si>
     <t>There is a tangent line in every direction at every point</t>
   </si>
   <si>
@@ -235,6 +283,9 @@
     <t>[partial f/partial x, Inclinometer]</t>
   </si>
   <si>
+    <t>This small group activity using surfaces combines practice with the multivariable chain rule while emphasizing numerical representations of derivatives. Students work in small groups to measure partial derivatives in both rectangular and polar coordinates, then verify their results using the chain rule. The whole class wrap-up discussion emphasizes the relationship between a directional derivative in the r-direction and derivatives in x- and y-directions using the chain rule.</t>
+  </si>
+  <si>
     <t>mvpchain</t>
   </si>
   <si>
@@ -283,9 +334,27 @@
     <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
   </si>
   <si>
+    <t>[$\vec \Nabla f, d\vec r$]</t>
+  </si>
+  <si>
+    <t>$df=\vec \nabla f \cdot d \vec r$</t>
+  </si>
+  <si>
     <t>The divergence is a scalar field</t>
   </si>
   <si>
+    <t>[$\vec \nabla \cdot \vec v$]</t>
+  </si>
+  <si>
+    <t>The divergence at a point is a scalar. Taking the divergence of a function yields a scalar at every value in the domain of that function: a scalar field</t>
+  </si>
+  <si>
+    <t>Put into words</t>
+  </si>
+  <si>
+    <t>[$\vec \nabla \times \vec v$]</t>
+  </si>
+  <si>
     <t>concept</t>
   </si>
   <si>
@@ -313,9 +382,15 @@
     <t>vcvalley</t>
   </si>
   <si>
+    <t>Correct prereq concept?</t>
+  </si>
+  <si>
     <t>Differential form of $\vec r$ in spherical and cylindrical coordinates</t>
   </si>
   <si>
+    <t>[$d \vec r$]</t>
+  </si>
+  <si>
     <t>The gradient's dimension is the same as real space. The gradient lives in the domain</t>
   </si>
   <si>
@@ -331,6 +406,9 @@
     <t>The divergence is a function</t>
   </si>
   <si>
+    <t>The divergence of a function (unless taken at a single point) is itself a function</t>
+  </si>
+  <si>
     <t>The divergence is a local quantity</t>
   </si>
   <si>
@@ -361,6 +439,9 @@
     <t>Vector Differentials</t>
   </si>
   <si>
+    <t>[$df$, 3D plots]</t>
+  </si>
+  <si>
     <t>vfdrvectorcurvi.jpg</t>
   </si>
   <si>
@@ -430,251 +511,173 @@
     <t>Differentials are small changes or differences</t>
   </si>
   <si>
+    <t>[$df$]</t>
+  </si>
+  <si>
     <t>PH 423</t>
   </si>
   <si>
     <t>differentials.jpg</t>
   </si>
   <si>
+    <t>One typical notation used for derivatives is Leibniz notation ($e.g.,$ $df/dx$).  Physicists often think of the $df$ and $dx$ as distinct quantities (``differentials'') that can be measured, calculated, and manipulated independent of one another.  In particular, a differential can be thought of as the (small) change in a quantity when a small change is made to a physical system.  A differential can also be thought of as the difference between the values of a quantity between two different (nearby) physical states.  This line of thinking is also valuable for thinking about integration in physical situations.</t>
+  </si>
+  <si>
+    <t>Equations can be 'zapped with d' to relate differentials</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>70 How is zapping with d different than taking the total derivative?</t>
+  </si>
+  <si>
+    <t>Individual differentials can be manipulated algebraically</t>
+  </si>
+  <si>
+    <t>Total differentials are linear</t>
+  </si>
+  <si>
+    <t>No matter how complicated a multivariable function is when written as an equation, the total differential of that function will be linear in the differential terms. In other words: $dF(x,y,z)=A dx + B dy + C dz.$</t>
+  </si>
+  <si>
+    <t>Differentials are small chunks</t>
+  </si>
+  <si>
+    <t>There are experimental limits to how $small$ of a change can be measured</t>
+  </si>
+  <si>
+    <t>[Experiment]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While it is relatively easy to imagine very, very small changes in physical values, there are often experimental limits on how small of a change can be measured. When designing and conducting experiments, there is a tension between these experimental limitations and normative representations of functions as smooth lines or </t>
+  </si>
+  <si>
+    <t>The derivative can be interpreted physically</t>
+  </si>
+  <si>
+    <t>While the consituents of a derivative (the $f$ and $x$ in $\frac{df}{dx}$) can have physical interpretations, the derivative itself can have a different physical interepretation. For example, $\frac{dx}{dt}$ is a velocity.</t>
+  </si>
+  <si>
+    <t>Better example needed</t>
+  </si>
+  <si>
+    <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
+  </si>
+  <si>
+    <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
+  </si>
+  <si>
+    <t>Partial derivatives are coefficients in a differentials equation</t>
+  </si>
+  <si>
+    <t>$df = \left(\frac{\partial f}{\partial x}\right)_y dx + \left(\frac{\partial f}{\partial y}\right)_x dy$</t>
+  </si>
+  <si>
+    <t>You can flip a partial derivative if the same variable(s) are constant</t>
+  </si>
+  <si>
+    <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
+  </si>
+  <si>
+    <t>There might be experimental limits on which quantities you can measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While it may be possible to conceptualize a particular derivative, such as $\left(\frac{\partial U}{\partial S}\right)_{V},$ Where $U$ is internal energy, $S$ is entropy, and $V$ is volume, that does not mean that the particular derivative can be directly measured. In the above example, the entropty $S$ is not measurable. </t>
+  </si>
+  <si>
+    <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because total differentials are linear, one can find the total differential and then solve algebraically to obtain partial derivatives that might not be obtainable though differentiation. </t>
+  </si>
+  <si>
+    <t>Zapping with d</t>
+  </si>
+  <si>
+    <t>LPsmall.jpg</t>
+  </si>
+  <si>
+    <t>We would like our students to have both a practical and mathematical understanding of a total differential. In particular, with this activity students learn what the consequences of ``zapping'' a function with the operator ``d'' are. This activity also opens up a conversation on infinitesimals, and their relation to total differentials. The use of variables not associated with the Partial Derivative Machine in this activity allows students to apply the mathematical techniques they have been practicing during the course to a less familiar physical system.</t>
+  </si>
+  <si>
+    <t>inzapd</t>
+  </si>
+  <si>
+    <t>Energy and Integrals</t>
+  </si>
+  <si>
+    <t>[PDM, df]</t>
+  </si>
+  <si>
+    <t>inpotentiallab.jpg</t>
+  </si>
+  <si>
+    <t>This integrated lab activity is designed to ask upper-division undergraduate students to measure the change in potential energy in an elastic system (PDM) between two different states. Students use the Partial Derivative Machine (PDM) to verify experimentally that the forces and dimensions of their system are state variables as well as measure the relationships between these quantities to compute the potential energy of their system. The whole class discussion focuses on the meaning of integration of discrete experimental data.</t>
+  </si>
+  <si>
+    <t>inpotentiallab</t>
+  </si>
+  <si>
+    <t>Partial Derivative Machine Derivatives</t>
+  </si>
+  <si>
+    <t>[PDM, $\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$,Table]</t>
+  </si>
+  <si>
+    <t>PDMD.jpg</t>
+  </si>
+  <si>
+    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>inisowidth</t>
+  </si>
+  <si>
+    <t>Chain Rules</t>
+  </si>
+  <si>
+    <t>pdm.jpg</t>
+  </si>
+  <si>
+    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
+  </si>
+  <si>
+    <t>incycchainrule</t>
+  </si>
+  <si>
+    <t>Not the correct description!</t>
+  </si>
+  <si>
+    <t>Name the Experiment (x3)</t>
+  </si>
+  <si>
+    <t>Mixed Partials</t>
+  </si>
+  <si>
+    <t>Maxwell's Relations</t>
+  </si>
+  <si>
+    <t>$\frac{\partial f}{\partial x}$</t>
+  </si>
+  <si>
+    <t>Contour Maps</t>
+  </si>
+  <si>
+    <t>Inclinometer</t>
+  </si>
+  <si>
+    <t>[df,graph???]</t>
+  </si>
+  <si>
     <t>One typical notation used for derivatives is Leibniz notation ($e.g.,$ $df/dx$).  Physicists often think of the $df$ and $dx$ as distinct quantities (``differentials'') that can be measured, calculated, and manipulated independent of one another.  In particular, a differential can be thought of as the (small) change in a quantity when a small change is made to a physical system.  A diffferential can also be thought of as the difference between the values of a quantity between two different (nearby) physical states.  This line of thinking is also valuable for thinking about integration in physical situations.</t>
-  </si>
-  <si>
-    <t>Equations can be 'zapped with d' to relate differentials</t>
-  </si>
-  <si>
-    <t>Individual differentials can be manipulated algebraically</t>
-  </si>
-  <si>
-    <t>Total differentials are linear</t>
-  </si>
-  <si>
-    <t>Differentials are small chunks</t>
-  </si>
-  <si>
-    <t>There are experimental limits to how $small$ of a change can be measured</t>
-  </si>
-  <si>
-    <t>The derivative can be interpreted physically</t>
-  </si>
-  <si>
-    <t>Partial derivatives that do not have the same variable(s) held constant are not the same derivative</t>
-  </si>
-  <si>
-    <t>$\left(\frac{\partial f}{\partial x}\right)_y \neq \left(\frac{\partial f}{\partial x}\right)_z$</t>
-  </si>
-  <si>
-    <t>Partial derivatives are coefficients in a differentials equation</t>
-  </si>
-  <si>
-    <t>$df = \left(\frac{\partial f}{\partial x}\right)_y dx + \left(\frac{\partial f}{\partial y}\right)_x dy$</t>
-  </si>
-  <si>
-    <t>You can flip a partial derivative if the same variable(s) are constant</t>
-  </si>
-  <si>
-    <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
-  </si>
-  <si>
-    <t>There might be experimental limits on which quantities you can measure</t>
-  </si>
-  <si>
-    <t>Differentials allow the finding of partial derivatives when a variable cannot be solved for</t>
-  </si>
-  <si>
-    <t>Zapping with d</t>
-  </si>
-  <si>
-    <t>LPsmall.jpg</t>
-  </si>
-  <si>
-    <t>We would like our students to have both a practical and mathematical understanding of a total differential. In particular, with this activity students learn what the consequences of ``zapping'' a function with the operator ``d'' are. This activity also opens up a conversation on infinitesimals, and their relation to total differentials. The use of variables not associated with the Partial Derivative Machine in this activity allows students to apply the mathematical techniques they have been practicing during the course to a less familiar physical system.</t>
-  </si>
-  <si>
-    <t>inzapd</t>
-  </si>
-  <si>
-    <t>Energy and Integrals</t>
-  </si>
-  <si>
-    <t>[PDM, df]</t>
-  </si>
-  <si>
-    <t>inpotentiallab.jpg</t>
-  </si>
-  <si>
-    <t>This integrated lab activity is designed to ask upper-division undergraduate students to measure the change in potential energy in an elastic system (PDM) between two different states. Students use the Partial Derivative Machine (PDM) to verify experimentally that the forces and dimensions of their system are state variables as well as measure the relationships between these quantities to compute the potential energy of their system. The whole class discussion focuses on the meaning of integration of discrete experimental data.</t>
-  </si>
-  <si>
-    <t>inpotentiallab</t>
-  </si>
-  <si>
-    <t>Partial Derivative Machine Derivatives</t>
-  </si>
-  <si>
-    <t>[PDM, $\textrm{Leibniz Notation}\\ \frac{\partial f}{\partial x} \rightarrow \left(\frac{\partial f}{\partial x}\right)_y$,Table]</t>
-  </si>
-  <si>
-    <t>PDMD.jpg</t>
-  </si>
-  <si>
-    <t>In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
-    <t>inisowidth</t>
-  </si>
-  <si>
-    <t>Chain Rules</t>
-  </si>
-  <si>
-    <t>pdm.jpg</t>
-  </si>
-  <si>
-    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
-    <t>incycchainrule</t>
-  </si>
-  <si>
-    <t>$\frac{\partial f}{\partial x}$</t>
-  </si>
-  <si>
-    <t>Contour Maps</t>
-  </si>
-  <si>
-    <t>Inclinometer</t>
-  </si>
-  <si>
-    <t>[df,graph???]</t>
-  </si>
-  <si>
-    <t>The divergence of a function (unless taken at a single point) is itself a function</t>
-  </si>
-  <si>
-    <t>One typical notation used for derivatives is Leibniz notation ($e.g.,$ $df/dx$).  Physicists often think of the $df$ and $dx$ as distinct quantities (``differentials'') that can be measured, calculated, and manipulated independent of one another.  In particular, a differential can be thought of as the (small) change in a quantity when a small change is made to a physical system.  A differential can also be thought of as the difference between the values of a quantity between two different (nearby) physical states.  This line of thinking is also valuable for thinking about integration in physical situations.</t>
-  </si>
-  <si>
-    <t>No matter how complicated a multivariable function is when written as an equation, the total differential of that function will be linear in the differential terms. In other words: $dF(x,y,z)=A dx + B dy + C dz.$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While it is relatively easy to imagine very, very small changes in physical values, there are often experimental limits on how small of a change can be measured. When designing and conducting experiments, there is a tension between these experimental limitations and normative representations of functions as smooth lines or </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taking derivatives of the same function with respect to different variables will produce different results. In physics, these different results might have different dimensions and thus the derivative can have wildly different physical interpretations based off of "'with respect to' what". </t>
-  </si>
-  <si>
-    <t>Understanding difference (how far apart two values are at one time) and change (how far apart the value of a single parameter is at two different times) is necessary for understanding derivatives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conceptually, a derivative can be thought of as how much one value changes as another value changes. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">While it may be possible to conceptualize a particular derivative, such as $\left(\frac{\partial U}{\partial S}\right)_{V},$ Where $U$ is internal energy, $S$ is entropy, and $V$ is volume, that does not mean that the particular derivative can be directly measured. In the above example, the entropty $S$ is not measurable. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Because total differentials are linear, one can find the total differential and then solve algebraically to obtain partial derivatives that might not be obtainable though differentiation. </t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>70 How is zapping with d different than taking the total derivative?</t>
-  </si>
-  <si>
-    <t>Not the correct description!</t>
-  </si>
-  <si>
-    <t>Put into words</t>
-  </si>
-  <si>
-    <t>The divergence at a point is a scalar. Taking the divergence of a function yields a scalar at every value in the domain of that function: a scalar field</t>
-  </si>
-  <si>
-    <t>Always or just when taking a derivative?</t>
-  </si>
-  <si>
-    <t>The derivative at a point is the slope of a tangent line at that point</t>
-  </si>
-  <si>
-    <t>Do we need to define a tangent line? That seems like too much.</t>
-  </si>
-  <si>
-    <t>Do we need to define a secant line? That seems like too much.</t>
-  </si>
-  <si>
-    <t>This small group activity using surfaces combines practice with the multivariable chain rule while emphasizing numerical representations of derivatives. Students work in small groups to measure partial derivatives in both rectangular and polar coordinates, then verify their results using the chain rule. The whole class wrap-up discussion emphasizes the relationship between a directional derivative in the r-direction and derivatives in x- and y-directions using the chain rule.</t>
-  </si>
-  <si>
-    <t>While the consituents of a derivative (the $f$ and $x$ in $\frac{df}{dx}$) can have physical interpretations, the derivative itself can have a different physical interepretation. For example, $\frac{dx}{dt}$ is a velocity.</t>
-  </si>
-  <si>
-    <t>Better example needed</t>
-  </si>
-  <si>
-    <t>Correct prereq concept?</t>
-  </si>
-  <si>
-    <t>Add more</t>
-  </si>
-  <si>
-    <t>$\frac{df}{dy}=\frac{df}{dx}\frac{dx}{dy}$</t>
-  </si>
-  <si>
-    <t>$\frac{d}{dt}(xy)=x\frac{dy}{dt}+y\frac{dx}{dt}$</t>
-  </si>
-  <si>
-    <t>There is a partial derivative in every direction at any point</t>
-  </si>
-  <si>
-    <t>Name the Experiment (x3)</t>
-  </si>
-  <si>
-    <t>Mixed Partials</t>
-  </si>
-  <si>
-    <t>Maxwell's Relations</t>
-  </si>
-  <si>
-    <t>[$\Delta x$]</t>
-  </si>
-  <si>
-    <t>[$\frac{\Delta f}{\Delta x}$]</t>
-  </si>
-  <si>
-    <t>[$\frac{d f}{d x},\frac{\partial f}{\partial x},\left(\frac{\partial f}{\partial x}\right)_y$]</t>
-  </si>
-  <si>
-    <t>[$\left(\frac{\partial f}{\partial x}\right)_y$]</t>
-  </si>
-  <si>
-    <t>$df=\vec \nabla f \cdot d \vec r$</t>
-  </si>
-  <si>
-    <t>[$\vec \Nabla f, d\vec r$]</t>
-  </si>
-  <si>
-    <t>[$\vec \nabla \cdot \vec v$]</t>
-  </si>
-  <si>
-    <t>[$\vec \nabla \times \vec v$]</t>
-  </si>
-  <si>
-    <t>[$d \vec r$]</t>
-  </si>
-  <si>
-    <t>[Experiment]</t>
-  </si>
-  <si>
-    <t>[$df$]</t>
-  </si>
-  <si>
-    <t>[$df$, 3D plots]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -737,6 +740,9 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -764,9 +770,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -1309,27 +1312,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
-    <col min="12" max="12" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
+    <col min="3" max="3" width="9.625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.625" customWidth="1"/>
+    <col min="5" max="5" width="39.625" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.625" customWidth="1"/>
+    <col min="10" max="10" width="11.875" customWidth="1"/>
+    <col min="12" max="12" width="33.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1364,517 +1367,517 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="48">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <f>ROW()</f>
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="32.1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <f>ROW()</f>
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
-        <f>ROW()</f>
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
       <c r="I3" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="32.1">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <f>ROW()</f>
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="32.1">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <f>ROW()</f>
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I13" si="0">"A long description for "&amp;B5 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The derivative can be approximated by the slope of a secant line is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="32.1">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <f>ROW()</f>
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative at a point is the slope of a tangent line at that point is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="32.1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <f>ROW()</f>
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative is a limit is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="32.1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <f>ROW()</f>
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative can be a function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="32.1">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <f>ROW()</f>
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative of a constant is zero is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="32.1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <f>ROW()</f>
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative is a linear function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="32.1">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <f>ROW()</f>
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <f>ROW()</f>
-        <v>11</v>
-      </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>A long description for Power law is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32.1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <f>ROW()</f>
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>A long description for The derivative at a cusp is undefined is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="32.1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <f>ROW()</f>
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>A long description for Variables can be held constant is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <f>ROW()</f>
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <f>ROW()</f>
         <v>15</v>
       </c>
-      <c r="L13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <f>ROW()</f>
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <f>ROW()</f>
-        <v>15</v>
-      </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>196</v>
+        <v>39</v>
       </c>
       <c r="K15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="96">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <f>ROW()</f>
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>204</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="63.95">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C17">
         <f>ROW()</f>
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="K17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="48">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C18">
         <f>ROW()</f>
@@ -1885,151 +1888,151 @@
         <v>[Variables can be held constant]</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>205</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="32.1">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <f>ROW()</f>
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ref="I19:I27" si="1">"A long description for "&amp;B19 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for There is a partial derivative in every direction at any point is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="32.1">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <f>ROW()</f>
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
         <v>A long description for There is a tangent line in every direction at every point is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="32.1">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <f>ROW()</f>
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
         <v>A long description for The derivative is related to the density of contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="48">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <f>ROW()</f>
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>205</v>
+        <v>47</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
         <v>A long description for The value of a partial derivative depends on the value(s) of what is held constant is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="32.1">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <f>ROW()</f>
@@ -2040,55 +2043,55 @@
         <v>[Single variable chain rule]</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
         <v>A long description for A partial derivative can be expressed in terms of other partial derivatives is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="32.1">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <f>ROW()</f>
         <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="48">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <f>ROW()</f>
@@ -2099,59 +2102,59 @@
         <v>[The derivative at a point is the slope of a tangent line at that point]</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
         <v>A long description for The magnitude of the gradient is the value of the slope in the steepest direction is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="32.1">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C26">
         <f>ROW()</f>
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
         <v>A long description for The gradient is perpendicular to contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="48">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <f>ROW()</f>
@@ -2162,148 +2165,148 @@
         <v>[The derivative at a point is the slope of a tangent line at that point,There is a partial derivative in every direction at any point]</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
         <v>A long description for All partial derivatives can be found as a slope of a tangent plane is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="32.1">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <f>ROW()</f>
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I28" t="str">
         <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
         <v>This is the long description for The derivative is local quantity. It is quite a long description!</v>
       </c>
       <c r="K28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <f>ROW()</f>
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="K29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
         <v>48</v>
       </c>
-      <c r="C30">
-        <f>ROW()</f>
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" t="s">
-        <v>33</v>
-      </c>
       <c r="I30" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="K30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="32.1">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C31">
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I31" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="96">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2318,30 +2321,30 @@
         <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G32" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="I32" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="J32" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="K32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="96">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2356,30 +2359,30 @@
         <v>[There is a partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H33" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I33" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="J33" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="71.25" customHeight="1">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2394,30 +2397,30 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="I34" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="J34" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="K34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="96">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2428,30 +2431,30 @@
         <v>[The derivative at a point is the slope of a tangent line at that point, A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="111.95">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="G35" t="s">
-        <v>33</v>
-      </c>
-      <c r="I35" t="s">
-        <v>191</v>
-      </c>
-      <c r="J35" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="112" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>52</v>
-      </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2466,30 +2469,30 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" t="s">
+        <v>90</v>
+      </c>
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="96">
+      <c r="A37" t="s">
         <v>68</v>
       </c>
-      <c r="G36" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" t="s">
-        <v>71</v>
-      </c>
-      <c r="I36" t="s">
-        <v>72</v>
-      </c>
-      <c r="J36" t="s">
-        <v>73</v>
-      </c>
-      <c r="K36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="96" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>52</v>
-      </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2504,30 +2507,30 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="I37" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="J37" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="K37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="48">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2538,28 +2541,28 @@
         <v>[Difference / Change]</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="I38" t="str">
         <f>"A long description for "&amp;B38 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Each component of $d \vec r$ is an arbitrary small change between two arbitrary position vectors.  is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="33.950000000000003" customHeight="1">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2570,59 +2573,59 @@
         <v>[Difference / Change]</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I39" t="str">
         <f>"A long description for "&amp;B39 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The magnitude of $d\vec r$ is the length of a small step along a path is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="33.950000000000003" customHeight="1">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
         <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I40" t="str">
         <f>"A long description for "&amp;B40 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The direction of $d\vec r$ is tangent to a path is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="48">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2633,51 +2636,51 @@
         <v>[Difference / Change]</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>207</v>
+        <v>102</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="I41" t="s">
-        <v>206</v>
+        <v>103</v>
       </c>
       <c r="K41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="32.1">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
         <v>42</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F42" t="s">
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="I42" t="s">
-        <v>186</v>
+        <v>106</v>
       </c>
       <c r="K42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="51" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1">
@@ -2685,30 +2688,30 @@
         <v>43</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30.95" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1">
@@ -2716,30 +2719,30 @@
         <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>209</v>
+        <v>108</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="45" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1">
@@ -2747,30 +2750,30 @@
         <v>45</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45.95" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1">
@@ -2778,33 +2781,33 @@
         <v>46</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="111.95">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2819,30 +2822,30 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" t="s">
         <v>88</v>
       </c>
-      <c r="G47" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" t="s">
-        <v>71</v>
-      </c>
       <c r="I47" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="J47" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="K47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="96">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2857,33 +2860,33 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H48" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="I48" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="J48" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="K48" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="32.1">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2894,59 +2897,59 @@
         <v>[Vector Differentials]</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
       <c r="G49" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" ref="I49:I63" si="2">"A long description for "&amp;B49 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Differential form of $\vec r$ in spherical and cylindrical coordinates is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="48">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
         <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The gradient's dimension is the same as real space. The gradient lives in the domain is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="32.1">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2957,120 +2960,120 @@
         <v>[]</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The gradient is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="32.1">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
         <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G52" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The electric field is the negative gradient of the electric potential is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="32.1">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53">
+        <f>ROW()</f>
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
         <v>99</v>
-      </c>
-      <c r="C53">
-        <f>ROW()</f>
-        <v>53</v>
-      </c>
-      <c r="D53" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" t="s">
-        <v>82</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The divergence is related to the total flux through a closed surface is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
         <v>54</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I54" t="s">
-        <v>173</v>
+        <v>126</v>
       </c>
       <c r="K54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="32.1">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -3081,152 +3084,152 @@
         <v>[]</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The divergence is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="32.1">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
         <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The divergence of the electric field is equal to is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="32.1">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
         <v>57</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The divergence of the magnetic field is zero is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="48">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
         <v>58</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The curl is related to the line integral around a closed loop. ("circulation") is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="32.1">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
         <v>59</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G59" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="2"/>
         <v>A long description for the curl is a (vector) function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="32.1">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -3237,121 +3240,121 @@
         <v>[]</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G60" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The curl is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="32.1">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
         <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G61" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The magnetic field is equal to the curl of the magnetic vector potential is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="32.1">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
         <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The curl of the electric field is zero in electrostatics is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="48">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
         <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="2"/>
         <v>A long description for The divergence of the curl is equal to mu times the current in magneto-statics is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="96">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3366,30 +3369,30 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F64" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="G64" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H64" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="I64" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="J64" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="K64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="128" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="128.1">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3404,30 +3407,30 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F65" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="G65" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H65" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="I65" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="J65" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="K65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="111.95">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3442,30 +3445,30 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="G66" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H66" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="I66" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="J66" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="K66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="159.94999999999999">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3480,30 +3483,30 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F67" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="G67" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H67" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="I67" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="J67" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="K67" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="159.94999999999999">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3518,30 +3521,30 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F68" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="G68" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="H68" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="I68" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="J68" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="K68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="128" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="128.1">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3552,156 +3555,156 @@
         <v>[Difference / Change]</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G69" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H69" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="I69" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="K69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="31.5">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
         <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>13</v>
+        <v>166</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G70" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ref="I70:I77" si="3">"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Equations can be 'zapped with d' to relate differentials is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K70" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L70" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="32.1">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
         <v>71</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="3"/>
         <v>A long description for Individual differentials can be manipulated algebraically is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="48.95" customHeight="1">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
         <v>72</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F72" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G72" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I72" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="32.1">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
         <v>73</v>
       </c>
       <c r="D73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G73" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I73" t="str">
         <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
         <v>$df$ can be viewed as a small chunk of $f$. When combined with 'The derivative is a ratio of small changes', it's easy to relate differentials to derivatives.</v>
       </c>
       <c r="K73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="80.099999999999994">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3712,60 +3715,60 @@
         <v>[The derivative is a ratio of small changes]</v>
       </c>
       <c r="E74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F74" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="G74" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I74" t="s">
+        <v>174</v>
+      </c>
+      <c r="K74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="48">
+      <c r="A75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75">
+        <f>ROW()</f>
+        <v>75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>162</v>
+      </c>
+      <c r="I75" t="s">
         <v>176</v>
       </c>
-      <c r="K74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>11</v>
-      </c>
-      <c r="B75" t="s">
-        <v>142</v>
-      </c>
-      <c r="C75">
-        <f>ROW()</f>
-        <v>75</v>
-      </c>
-      <c r="D75" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" t="s">
-        <v>13</v>
-      </c>
-      <c r="G75" t="s">
-        <v>134</v>
-      </c>
-      <c r="I75" t="s">
-        <v>192</v>
-      </c>
       <c r="K75" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L75" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="96">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3776,31 +3779,31 @@
         <v>[Derivatives can be found while holding one or more variables constant,The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>205</v>
+        <v>47</v>
       </c>
       <c r="G76" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H76" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="3"/>
         <v>A long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K76" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="50.25" customHeight="1">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3811,31 +3814,31 @@
         <v>[The derivative is a ratio of small changes,Differentials are small changes or differences]</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H77" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="3"/>
         <v>A long description for Partial derivatives are coefficients in a differentials equation is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K77" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="80.099999999999994">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3846,57 +3849,57 @@
         <v>[You can flip a derivative, Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="E78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>205</v>
+        <v>47</v>
       </c>
       <c r="G78" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I78" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="K78" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="63.95">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
         <v>79</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="G79" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I79" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="K79" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="48">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3907,27 +3910,27 @@
         <v>[Total differentials are linear]</v>
       </c>
       <c r="E80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G80" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="I80" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="K80" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="111.95">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B81" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3942,30 +3945,30 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G81" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H81" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I81" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="J81" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="K81" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="111.95">
       <c r="A82" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3980,30 +3983,30 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F82" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="G82" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H82" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="I82" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="J82" t="s">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="K82" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="93" customHeight="1">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -4018,30 +4021,30 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="G83" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H83" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="I83" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="J83" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="K83" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="240" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="240">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -4056,50 +4059,50 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="G84" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H84" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="I84" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="J84" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="K84" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L84" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="L85" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="L86" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="L87" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="L88" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="L89" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4129,22 +4132,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82:F83 F85:F1048576 F1:F79">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$F1="[]"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J84 J86:J1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($J1="",$A1="Activity")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>AND($E85="[]",$L85="Activity")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85">
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>AND($J85="",$L85="Activity")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4158,37 +4161,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EFD8F-45BF-44EB-A2B4-FA9451BFAEEC}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
       <selection activeCell="A34" sqref="A34:K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="71.25" customHeight="1"/>
+    <row r="69" spans="1:11" ht="409.6">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -4199,22 +4202,22 @@
         <v>[]</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="G69" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="H69" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="I69" t="s">
-        <v>136</v>
+        <v>214</v>
       </c>
       <c r="K69" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
follow Paul's lead in creating sections for experiment
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -160,9 +160,6 @@
     <t>You can flip a derivative</t>
   </si>
   <si>
-    <t>[$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$]</t>
-  </si>
-  <si>
     <t>In other words, $\frac{dy}{dx} = \frac{1}{\frac{dx}{dy}}$.  Note that this concept is challenging to express in Newton's notation, but arises naturally if implicit differentiation is covered.</t>
   </si>
   <si>
@@ -593,6 +590,9 @@
   </si>
   <si>
     <t>You can flip a partial derivative if the same variable(s) are constant</t>
+  </si>
+  <si>
+    <t>[$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$]</t>
   </si>
   <si>
     <t>In other words, \[\left(\frac{\partial y}{\partial x}\right)_z = \frac1{\left(\frac{\partial x}{\partial y}\right)_z}. \]  Note that this equality is only true if the same variables are being held fixed on each side of the equality.  This therefore relies on the thermodynamics notation that specifies what quantities are being held fixed for a partial derivative.</t>
@@ -1323,8 +1323,8 @@
   <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1821,7 +1821,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="96">
+    <row r="16" spans="1:12" ht="47.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1839,14 +1839,14 @@
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
@@ -1857,7 +1857,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <f>ROW()</f>
@@ -1876,7 +1876,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
@@ -1887,7 +1887,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <f>ROW()</f>
@@ -1901,13 +1901,13 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>50</v>
-      </c>
-      <c r="I18" t="s">
-        <v>51</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
@@ -1918,23 +1918,23 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <f>ROW()</f>
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
         <v>52</v>
       </c>
-      <c r="C19">
-        <f>ROW()</f>
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" t="s">
-        <v>53</v>
-      </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ref="I19:I27" si="1">"A long description for "&amp;B19 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -1949,7 +1949,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <f>ROW()</f>
@@ -1962,10 +1962,10 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
@@ -1980,23 +1980,23 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21">
+        <f>ROW()</f>
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
         <v>55</v>
       </c>
-      <c r="C21">
-        <f>ROW()</f>
-        <v>21</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" t="s">
-        <v>56</v>
-      </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
@@ -2011,7 +2011,7 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22">
         <f>ROW()</f>
@@ -2024,10 +2024,10 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" t="s">
         <v>49</v>
-      </c>
-      <c r="G22" t="s">
-        <v>50</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
@@ -2042,7 +2042,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23">
         <f>ROW()</f>
@@ -2056,10 +2056,10 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
@@ -2074,26 +2074,26 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <f>ROW()</f>
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
         <v>60</v>
       </c>
-      <c r="C24">
-        <f>ROW()</f>
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" t="s">
         <v>61</v>
-      </c>
-      <c r="G24" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="48">
@@ -2101,7 +2101,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <f>ROW()</f>
@@ -2115,10 +2115,10 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
@@ -2133,7 +2133,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26">
         <f>ROW()</f>
@@ -2146,10 +2146,10 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
@@ -2164,7 +2164,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27">
         <f>ROW()</f>
@@ -2178,10 +2178,10 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
@@ -2196,7 +2196,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28">
         <f>ROW()</f>
@@ -2212,7 +2212,7 @@
         <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I28" t="str">
         <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
@@ -2227,26 +2227,26 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" t="s">
         <v>67</v>
-      </c>
-      <c r="C29">
-        <f>ROW()</f>
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>68</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -2257,26 +2257,26 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
         <v>69</v>
-      </c>
-      <c r="C30">
-        <f>ROW()</f>
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" t="s">
-        <v>70</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
@@ -2287,7 +2287,7 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31">
         <v>28</v>
@@ -2299,13 +2299,13 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" t="s">
         <v>72</v>
-      </c>
-      <c r="G31" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" t="s">
-        <v>73</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="32" spans="1:11" ht="96">
       <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
         <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>75</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2331,19 +2331,19 @@
         <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" t="s">
         <v>76</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>77</v>
-      </c>
-      <c r="J32" t="s">
-        <v>78</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="33" spans="1:12" ht="96">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2369,19 +2369,19 @@
         <v>[There is a partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" t="s">
         <v>80</v>
       </c>
-      <c r="G33" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>81</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>82</v>
-      </c>
-      <c r="J33" t="s">
-        <v>83</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
@@ -2389,10 +2389,10 @@
     </row>
     <row r="34" spans="1:12" ht="71.25" customHeight="1">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2407,19 +2407,19 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" t="s">
         <v>85</v>
       </c>
-      <c r="G34" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>86</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>87</v>
-      </c>
-      <c r="J34" t="s">
-        <v>88</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
@@ -2427,10 +2427,10 @@
     </row>
     <row r="35" spans="1:12" ht="96">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2444,16 +2444,16 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
         <v>90</v>
       </c>
-      <c r="G35" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>91</v>
-      </c>
-      <c r="J35" t="s">
-        <v>92</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="36" spans="1:12" ht="111.95">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2479,19 +2479,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H36" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" t="s">
         <v>94</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>95</v>
-      </c>
-      <c r="J36" t="s">
-        <v>96</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
@@ -2499,10 +2499,10 @@
     </row>
     <row r="37" spans="1:12" ht="96">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2517,19 +2517,19 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" t="s">
         <v>98</v>
       </c>
-      <c r="G37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>99</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>100</v>
-      </c>
-      <c r="J37" t="s">
-        <v>101</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
@@ -2540,7 +2540,7 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2554,10 +2554,10 @@
         <v>14</v>
       </c>
       <c r="F38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" t="s">
         <v>103</v>
-      </c>
-      <c r="G38" t="s">
-        <v>104</v>
       </c>
       <c r="I38" t="str">
         <f>"A long description for "&amp;B38 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2572,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2586,10 +2586,10 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I39" t="str">
         <f>"A long description for "&amp;B39 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2604,7 +2604,7 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
@@ -2617,10 +2617,10 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I40" t="str">
         <f>"A long description for "&amp;B40 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2635,7 +2635,7 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2649,13 +2649,13 @@
         <v>14</v>
       </c>
       <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" t="s">
         <v>109</v>
-      </c>
-      <c r="G41" t="s">
-        <v>104</v>
-      </c>
-      <c r="I41" t="s">
-        <v>110</v>
       </c>
       <c r="K41" t="s">
         <v>18</v>
@@ -2666,23 +2666,23 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42">
+        <f>ROW()</f>
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" t="s">
         <v>111</v>
       </c>
-      <c r="C42">
-        <f>ROW()</f>
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
         <v>112</v>
-      </c>
-      <c r="I42" t="s">
-        <v>113</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
@@ -2704,10 +2704,10 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2716,7 +2716,7 @@
         <v>18</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30.95" customHeight="1">
@@ -2735,10 +2735,10 @@
         <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2747,12 +2747,12 @@
         <v>18</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="45" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1">
@@ -2769,7 +2769,7 @@
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2778,7 +2778,7 @@
         <v>18</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="45.95" customHeight="1">
@@ -2800,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2809,15 +2809,15 @@
         <v>18</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="111.95">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2832,19 +2832,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" t="s">
+        <v>93</v>
+      </c>
+      <c r="I47" t="s">
         <v>118</v>
       </c>
-      <c r="G47" t="s">
-        <v>104</v>
-      </c>
-      <c r="H47" t="s">
-        <v>94</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>119</v>
-      </c>
-      <c r="J47" t="s">
-        <v>120</v>
       </c>
       <c r="K47" t="s">
         <v>18</v>
@@ -2852,10 +2852,10 @@
     </row>
     <row r="48" spans="1:12" ht="96">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2870,25 +2870,25 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H48" t="s">
+        <v>121</v>
+      </c>
+      <c r="I48" t="s">
         <v>122</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>123</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="K48" t="s">
-        <v>18</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="32.1">
@@ -2896,7 +2896,7 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2910,10 +2910,10 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" ref="I49:I63" si="2">"A long description for "&amp;B49 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2928,7 +2928,7 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -2941,10 +2941,10 @@
         <v>14</v>
       </c>
       <c r="F50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
@@ -2959,7 +2959,7 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2972,10 +2972,10 @@
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="2"/>
@@ -2990,7 +2990,7 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -3003,10 +3003,10 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="2"/>
@@ -3021,7 +3021,7 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -3034,10 +3034,10 @@
         <v>14</v>
       </c>
       <c r="F53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="2"/>
@@ -3052,26 +3052,26 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54">
+        <f>ROW()</f>
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" t="s">
+        <v>111</v>
+      </c>
+      <c r="G54" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54" t="s">
         <v>131</v>
-      </c>
-      <c r="C54">
-        <f>ROW()</f>
-        <v>54</v>
-      </c>
-      <c r="D54" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" t="s">
-        <v>112</v>
-      </c>
-      <c r="G54" t="s">
-        <v>106</v>
-      </c>
-      <c r="I54" t="s">
-        <v>132</v>
       </c>
       <c r="K54" t="s">
         <v>18</v>
@@ -3082,7 +3082,7 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -3095,10 +3095,10 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="2"/>
@@ -3113,7 +3113,7 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -3126,10 +3126,10 @@
         <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="2"/>
@@ -3144,7 +3144,7 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -3157,10 +3157,10 @@
         <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="2"/>
@@ -3175,7 +3175,7 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -3188,10 +3188,10 @@
         <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="2"/>
@@ -3206,7 +3206,7 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -3219,10 +3219,10 @@
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="2"/>
@@ -3237,7 +3237,7 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -3250,10 +3250,10 @@
         <v>14</v>
       </c>
       <c r="F60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="2"/>
@@ -3268,7 +3268,7 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -3281,10 +3281,10 @@
         <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="2"/>
@@ -3299,7 +3299,7 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -3312,10 +3312,10 @@
         <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
@@ -3330,23 +3330,23 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63">
+        <f>ROW()</f>
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" t="s">
         <v>141</v>
       </c>
-      <c r="C63">
-        <f>ROW()</f>
-        <v>63</v>
-      </c>
-      <c r="D63" t="s">
-        <v>14</v>
-      </c>
-      <c r="E63" t="s">
-        <v>14</v>
-      </c>
-      <c r="F63" t="s">
-        <v>142</v>
-      </c>
       <c r="G63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="2"/>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="64" spans="1:11" ht="94.5">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3376,19 +3376,19 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G64" t="s">
+        <v>105</v>
+      </c>
+      <c r="H64" t="s">
         <v>144</v>
       </c>
-      <c r="G64" t="s">
-        <v>106</v>
-      </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>145</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>146</v>
-      </c>
-      <c r="J64" t="s">
-        <v>147</v>
       </c>
       <c r="K64" t="s">
         <v>18</v>
@@ -3396,10 +3396,10 @@
     </row>
     <row r="65" spans="1:12" ht="128.1">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3414,19 +3414,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F65" t="s">
+        <v>148</v>
+      </c>
+      <c r="G65" t="s">
+        <v>105</v>
+      </c>
+      <c r="H65" t="s">
         <v>149</v>
       </c>
-      <c r="G65" t="s">
-        <v>106</v>
-      </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>150</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>151</v>
-      </c>
-      <c r="J65" t="s">
-        <v>152</v>
       </c>
       <c r="K65" t="s">
         <v>18</v>
@@ -3434,10 +3434,10 @@
     </row>
     <row r="66" spans="1:12" ht="111.95">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3452,19 +3452,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" t="s">
+        <v>105</v>
+      </c>
+      <c r="H66" t="s">
         <v>154</v>
       </c>
-      <c r="G66" t="s">
-        <v>106</v>
-      </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>155</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>156</v>
-      </c>
-      <c r="J66" t="s">
-        <v>157</v>
       </c>
       <c r="K66" t="s">
         <v>18</v>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="67" spans="1:12" ht="159.94999999999999">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3490,19 +3490,19 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F67" t="s">
+        <v>158</v>
+      </c>
+      <c r="G67" t="s">
+        <v>105</v>
+      </c>
+      <c r="H67" t="s">
         <v>159</v>
       </c>
-      <c r="G67" t="s">
-        <v>106</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>160</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>161</v>
-      </c>
-      <c r="J67" t="s">
-        <v>162</v>
       </c>
       <c r="K67" t="s">
         <v>18</v>
@@ -3510,10 +3510,10 @@
     </row>
     <row r="68" spans="1:12" ht="159.94999999999999">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3528,19 +3528,19 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H68" t="s">
+        <v>163</v>
+      </c>
+      <c r="I68" t="s">
         <v>164</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>165</v>
-      </c>
-      <c r="J68" t="s">
-        <v>166</v>
       </c>
       <c r="K68" t="s">
         <v>18</v>
@@ -3551,7 +3551,7 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3565,16 +3565,16 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
+        <v>167</v>
+      </c>
+      <c r="G69" t="s">
         <v>168</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>169</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>170</v>
-      </c>
-      <c r="I69" t="s">
-        <v>171</v>
       </c>
       <c r="K69" t="s">
         <v>18</v>
@@ -3585,7 +3585,7 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3598,10 +3598,10 @@
         <v>14</v>
       </c>
       <c r="F70" t="s">
+        <v>167</v>
+      </c>
+      <c r="G70" t="s">
         <v>168</v>
-      </c>
-      <c r="G70" t="s">
-        <v>169</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ref="I70:I77" si="3">"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -3611,7 +3611,7 @@
         <v>18</v>
       </c>
       <c r="L70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="32.1">
@@ -3619,7 +3619,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3635,7 +3635,7 @@
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="3"/>
@@ -3650,26 +3650,26 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72">
+        <f>ROW()</f>
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" t="s">
+        <v>167</v>
+      </c>
+      <c r="G72" t="s">
+        <v>168</v>
+      </c>
+      <c r="I72" t="s">
         <v>175</v>
-      </c>
-      <c r="C72">
-        <f>ROW()</f>
-        <v>72</v>
-      </c>
-      <c r="D72" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" t="s">
-        <v>168</v>
-      </c>
-      <c r="G72" t="s">
-        <v>169</v>
-      </c>
-      <c r="I72" t="s">
-        <v>176</v>
       </c>
       <c r="K72" t="s">
         <v>18</v>
@@ -3680,7 +3680,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3693,10 +3693,10 @@
         <v>14</v>
       </c>
       <c r="F73" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
         <v>168</v>
-      </c>
-      <c r="G73" t="s">
-        <v>169</v>
       </c>
       <c r="I73" t="str">
         <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
@@ -3711,7 +3711,7 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3725,13 +3725,13 @@
         <v>14</v>
       </c>
       <c r="F74" t="s">
+        <v>178</v>
+      </c>
+      <c r="G74" t="s">
+        <v>168</v>
+      </c>
+      <c r="I74" t="s">
         <v>179</v>
-      </c>
-      <c r="G74" t="s">
-        <v>169</v>
-      </c>
-      <c r="I74" t="s">
-        <v>180</v>
       </c>
       <c r="K74" t="s">
         <v>18</v>
@@ -3742,32 +3742,32 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75">
+        <f>ROW()</f>
+        <v>75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" t="s">
+        <v>168</v>
+      </c>
+      <c r="I75" t="s">
         <v>181</v>
       </c>
-      <c r="C75">
-        <f>ROW()</f>
-        <v>75</v>
-      </c>
-      <c r="D75" t="s">
-        <v>14</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" t="s">
-        <v>169</v>
-      </c>
-      <c r="I75" t="s">
+      <c r="K75" t="s">
+        <v>18</v>
+      </c>
+      <c r="L75" t="s">
         <v>182</v>
-      </c>
-      <c r="K75" t="s">
-        <v>18</v>
-      </c>
-      <c r="L75" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="96">
@@ -3775,7 +3775,7 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3789,13 +3789,13 @@
         <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="3"/>
@@ -3810,7 +3810,7 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3824,13 +3824,13 @@
         <v>14</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="3"/>
@@ -3840,12 +3840,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="80.099999999999994">
+    <row r="78" spans="1:12" ht="94.5">
       <c r="A78" t="s">
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3859,10 +3859,10 @@
         <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="G78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I78" t="s">
         <v>189</v>
@@ -3892,7 +3892,7 @@
         <v>191</v>
       </c>
       <c r="G79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I79" t="s">
         <v>192</v>
@@ -3920,10 +3920,10 @@
         <v>14</v>
       </c>
       <c r="F80" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80" t="s">
         <v>168</v>
-      </c>
-      <c r="G80" t="s">
-        <v>169</v>
       </c>
       <c r="I80" t="s">
         <v>194</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="81" spans="1:12" ht="111.95">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
         <v>195</v>
@@ -3952,10 +3952,10 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G81" t="s">
         <v>168</v>
-      </c>
-      <c r="G81" t="s">
-        <v>169</v>
       </c>
       <c r="H81" t="s">
         <v>196</v>
@@ -3972,7 +3972,7 @@
     </row>
     <row r="82" spans="1:12" ht="111.95">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82" t="s">
         <v>199</v>
@@ -3993,7 +3993,7 @@
         <v>200</v>
       </c>
       <c r="G82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H82" t="s">
         <v>201</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="83" spans="1:12" ht="93" customHeight="1">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
         <v>204</v>
@@ -4031,7 +4031,7 @@
         <v>205</v>
       </c>
       <c r="G83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H83" t="s">
         <v>206</v>
@@ -4048,7 +4048,7 @@
     </row>
     <row r="84" spans="1:12" ht="240">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
         <v>209</v>
@@ -4066,10 +4066,10 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G84" t="s">
         <v>168</v>
-      </c>
-      <c r="G84" t="s">
-        <v>169</v>
       </c>
       <c r="H84" t="s">
         <v>210</v>
@@ -4183,7 +4183,7 @@
     <row r="1" spans="1:4" ht="15.95" customHeight="1">
       <c r="A1" s="4" t="str">
         <f>SUBSTITUTE(_xlfn.CONCAT(Sheet1!F2:F100),"][",",")</f>
-        <v>[$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$]</v>
+        <v>[$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$]</v>
       </c>
       <c r="B1" s="4" t="str">
         <f>TRIM(LEFT(A3,FIND(",",A3)-1))</f>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="C1" s="4" t="str">
         <f>RIGHT(A3,LEN(A3)-LEN(B1)-1)</f>
-        <v>$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>217</v>
@@ -4200,7 +4200,7 @@
     <row r="2" spans="1:4" ht="15.95" customHeight="1">
       <c r="A2" s="4" t="str">
         <f>MID(A1,2,LEN(A1)-2)</f>
-        <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>TRIM(IFERROR(LEFT(C1,FIND(",",C1)-1),C1))</f>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="C2" s="4" t="str">
         <f>TRIM(IFERROR(RIGHT(C1,LEN(C1)-LEN(B2)-1),""))</f>
-        <v>$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D2" s="4" t="str">
         <f t="array" ref="D2">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D1,B$1:B$100),0)),"")</f>
@@ -4218,7 +4218,7 @@
     <row r="3" spans="1:4" ht="15.95" customHeight="1">
       <c r="A3" s="4" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2,",,,",","),",,,",","),",,",",")</f>
-        <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>TRIM(IFERROR(LEFT(C2,FIND(",",C2)-1),C2))</f>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="C3" s="4" t="str">
         <f t="shared" ref="C3:C66" si="0">TRIM(IFERROR(RIGHT(C2,LEN(C2)-LEN(B3)-1),""))</f>
-        <v>1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="array" ref="D3">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D2,B$1:B$100),0)),"")</f>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="C4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="array" ref="D4">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D3,B$1:B$100),0)),"")</f>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="C5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="array" ref="D5">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D4,B$1:B$100),0)),"")</f>
@@ -4271,11 +4271,11 @@
       </c>
       <c r="C6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="array" ref="D6">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D5,B$1:B$100),0)),"")</f>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4286,11 +4286,11 @@
       </c>
       <c r="C7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="array" ref="D7">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D6,B$1:B$100),0)),"")</f>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>2D Graph</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4301,11 +4301,11 @@
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="array" ref="D8">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D7,B$1:B$100),0)),"")</f>
-        <v>2D Graph</v>
+        <v>Contour Maps</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4316,22 +4316,22 @@
       </c>
       <c r="C9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="array" ref="D9">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D8,B$1:B$100),0)),"")</f>
-        <v>Contour Maps</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\frac{d f}{d x}$</v>
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="array" ref="D10">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D9,B$1:B$100),0)),"")</f>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="array" ref="D11">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D10,B$1:B$100),0)),"")</f>
@@ -4357,11 +4357,11 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{d f}{d x}$</v>
+        <v>2D Graph</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="array" ref="D12">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D11,B$1:B$100),0)),"")</f>
@@ -4372,11 +4372,11 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>2D Graph</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D12,B$1:B$100),0)),"")</f>
@@ -4387,11 +4387,11 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2D Graph</v>
+        <v>Contour Maps</v>
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D13,B$1:B$100),0)),"")</f>
@@ -4402,11 +4402,11 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2D Graph</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D15" s="4" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D14,B$1:B$100),0)),"")</f>
@@ -4417,11 +4417,11 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Contour Maps</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D16" s="4" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D15,B$1:B$100),0)),"")</f>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D16,B$1:B$100),0)),"")</f>
@@ -4447,11 +4447,11 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="array" ref="D18">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D17,B$1:B$100),0)),"")</f>
@@ -4462,11 +4462,11 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="array" ref="D19">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D18,B$1:B$100),0)),"")</f>
@@ -4477,11 +4477,11 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>Contour Maps</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D20" s="4" t="str">
         <f t="array" ref="D20">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D19,B$1:B$100),0)),"")</f>
@@ -4492,11 +4492,11 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>2D Graph</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D21" s="4" t="str">
         <f t="array" ref="D21">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D20,B$1:B$100),0)),"")</f>
@@ -4507,11 +4507,11 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Contour Maps</v>
+        <v>$\frac{d f}{d x}$</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D22" s="4" t="str">
         <f t="array" ref="D22">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D21,B$1:B$100),0)),"")</f>
@@ -4522,11 +4522,11 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2D Graph</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D23" s="4" t="str">
         <f t="array" ref="D23">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D22,B$1:B$100),0)),"")</f>
@@ -4537,11 +4537,11 @@
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{d f}{d x}$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D24" s="4" t="str">
         <f t="array" ref="D24">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D23,B$1:B$100),0)),"")</f>
@@ -4552,11 +4552,11 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D25" s="4" t="str">
         <f t="array" ref="D25">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D24,B$1:B$100),0)),"")</f>
@@ -4567,11 +4567,11 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D26" s="4" t="str">
         <f t="array" ref="D26">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D25,B$1:B$100),0)),"")</f>
@@ -4582,11 +4582,11 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D27" s="4" t="str">
         <f t="array" ref="D27">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D26,B$1:B$100),0)),"")</f>
@@ -4597,11 +4597,11 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>Contour Maps</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D28" s="4" t="str">
         <f t="array" ref="D28">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D27,B$1:B$100),0)),"")</f>
@@ -4612,11 +4612,11 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="array" ref="D29">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D28,B$1:B$100),0)),"")</f>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="array" ref="D30">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D29,B$1:B$100),0)),"")</f>
@@ -4642,11 +4642,11 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>Inclinometer</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D31" s="4" t="str">
         <f t="array" ref="D31">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D30,B$1:B$100),0)),"")</f>
@@ -4657,11 +4657,11 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Contour Maps</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D32" s="4" t="str">
         <f t="array" ref="D32">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D31,B$1:B$100),0)),"")</f>
@@ -4672,11 +4672,11 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Inclinometer</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D33" s="4" t="str">
         <f t="array" ref="D33">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D32,B$1:B$100),0)),"")</f>
@@ -4687,11 +4687,11 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>Inclinometer</v>
       </c>
       <c r="C34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="array" ref="D34">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D33,B$1:B$100),0)),"")</f>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="C35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D35" s="4" t="str">
         <f t="array" ref="D35">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D34,B$1:B$100),0)),"")</f>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="C36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D36" s="4" t="str">
         <f t="array" ref="D36">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D35,B$1:B$100),0)),"")</f>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="C37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D37" s="4" t="str">
         <f t="array" ref="D37">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D36,B$1:B$100),0)),"")</f>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D38" s="4" t="str">
         <f t="array" ref="D38">IFERROR(INDEX(B$1:B$100,MATCH(0,COUNTIF($D$1:$D37,B$1:B$100),0)),"")</f>
@@ -4761,31 +4761,31 @@
     <row r="39" spans="1:4">
       <c r="B39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Inclinometer</v>
+        <v>$d \vec r$</v>
       </c>
       <c r="C40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$d \vec r$</v>
       </c>
       <c r="C41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -4795,17 +4795,17 @@
       </c>
       <c r="C42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$d \vec r$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4815,57 +4815,57 @@
       </c>
       <c r="C44" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$\vec \nabla \cdot \vec v$</v>
       </c>
       <c r="C45" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="B46" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$d \vec r$</v>
+        <v>$\vec \nabla \cdot \vec v$</v>
       </c>
       <c r="C46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \cdot \vec v$</v>
+        <v>$\vec \nabla \times \vec v$</v>
       </c>
       <c r="C47" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \cdot \vec v$</v>
+        <v>Contour Maps</v>
       </c>
       <c r="C48" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="B49" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \times \vec v$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C49" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -4875,37 +4875,37 @@
       </c>
       <c r="C50" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="B51" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$d \vec r$</v>
       </c>
       <c r="C51" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Contour Maps</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C52" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$d \vec r$</v>
+        <v>$\vec \nabla f$</v>
       </c>
       <c r="C53" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -4915,27 +4915,27 @@
       </c>
       <c r="C54" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$\vec \nabla \cdot \vec v$</v>
       </c>
       <c r="C55" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla f$</v>
+        <v>$\vec \nabla \cdot \vec v$</v>
       </c>
       <c r="C56" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="57" spans="2:3">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="C57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="58" spans="2:3">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="C58" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="59" spans="2:3">
@@ -4965,27 +4965,27 @@
       </c>
       <c r="C59" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \cdot \vec v$</v>
+        <v>$\vec \nabla \times \vec v$</v>
       </c>
       <c r="C60" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \cdot \vec v$</v>
+        <v>$\vec \nabla \times \vec v$</v>
       </c>
       <c r="C61" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="62" spans="2:3">
@@ -4995,7 +4995,7 @@
       </c>
       <c r="C62" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="63" spans="2:3">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="C63" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="64" spans="2:3">
@@ -5015,17 +5015,17 @@
       </c>
       <c r="C64" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>$\vec \nabla \times \vec v$</v>
+        <v>$\vec \nabla \cdot \vec v$</v>
       </c>
       <c r="C65" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="66" spans="2:3">
@@ -5035,67 +5035,67 @@
       </c>
       <c r="C66" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>$\vec \nabla \cdot \vec v$</v>
+        <v>$d \vec r$</v>
       </c>
       <c r="C67" s="4" t="str">
         <f t="shared" ref="C67:C109" si="3">TRIM(IFERROR(RIGHT(C66,LEN(C66)-LEN(B67)-1),""))</f>
-        <v>$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>$\vec \nabla \times \vec v$</v>
+        <v>3D plots</v>
       </c>
       <c r="C68" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>$d \vec r$</v>
+        <v>Kinesthetic</v>
       </c>
       <c r="C69" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" s="4" t="str">
         <f t="shared" ref="B70:B93" si="4">IFERROR(LEFT(C69,FIND(",",C69)-1),C69)</f>
-        <v>3D plots</v>
+        <v>Kinesthetic</v>
       </c>
       <c r="C70" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Kinesthetic</v>
+        <v>Vector Field Map</v>
       </c>
       <c r="C71" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="B72" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Kinesthetic</v>
+        <v>Contour Maps</v>
       </c>
       <c r="C72" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -5105,37 +5105,37 @@
       </c>
       <c r="C73" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Contour Maps</v>
+        <v>Vector Field Map</v>
       </c>
       <c r="C74" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Vector Field Map</v>
+        <v>$df$</v>
       </c>
       <c r="C75" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Vector Field Map</v>
+        <v>$df$</v>
       </c>
       <c r="C76" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -5145,7 +5145,7 @@
       </c>
       <c r="C77" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -5155,57 +5155,57 @@
       </c>
       <c r="C78" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$df$</v>
+        <v>$\Delta x$</v>
       </c>
       <c r="C79" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$df$</v>
+        <v>$dx$</v>
       </c>
       <c r="C80" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$\Delta x$</v>
+        <v>Experiment</v>
       </c>
       <c r="C81" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$dx$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C82" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Experiment</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C83" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="84" spans="2:3">
@@ -5215,47 +5215,47 @@
       </c>
       <c r="C84" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C85" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C86" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>Experiment</v>
       </c>
       <c r="C87" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Experiment</v>
+        <v>$df$</v>
       </c>
       <c r="C88" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="89" spans="2:3">
@@ -5265,83 +5265,83 @@
       </c>
       <c r="C89" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$df$</v>
+        <v>PDM</v>
       </c>
       <c r="C90" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>PDM</v>
+        <v>$df$</v>
       </c>
       <c r="C91" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="B92" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>$df$</v>
+        <v>PDM</v>
       </c>
       <c r="C92" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="B93" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>PDM</v>
+        <v>$\frac{\partial f}{\partial x}$</v>
       </c>
       <c r="C93" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="B94" s="4" t="str">
         <f>IFERROR(LEFT(C93,FIND(",",C93)-1),C93)</f>
-        <v>$\frac{\partial f}{\partial x}$</v>
+        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
       <c r="C94" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
+        <v>Table,$df$</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="B95" s="4" t="str">
         <f t="shared" ref="B95:B125" si="5">IFERROR(LEFT(C94,FIND(",",C94)-1),C94)</f>
-        <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
+        <v>Table</v>
       </c>
       <c r="C95" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>Table,$df$</v>
+        <v>$df$</v>
       </c>
     </row>
     <row r="96" spans="2:3">
       <c r="B96" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>Table</v>
+        <v>$df$</v>
       </c>
       <c r="C96" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>$df$</v>
+        <v/>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>$df$</v>
+        <v/>
       </c>
       <c r="C97" s="4" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
more love for orphans
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21217"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84CC10-268F-A148-A62C-477A4E0A9D68}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84CC10-268F-A148-A62C-477A4E0A9D68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,22 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="234">
   <si>
     <t>Act or Con</t>
   </si>
@@ -79,7 +84,7 @@
     <t>MTH 251</t>
   </si>
   <si>
-    <t>Understanding difference (how far apart two values are at one time) and change (how far apart the value of a single parameter is at two different times) is necessary for understanding derivatives.</t>
+    <t>Understanding both difference (how far apart two values are at one time) and change (how far apart the value of a single parameter is at two different times) is necessary for understanding derivatives.</t>
   </si>
   <si>
     <t>Active</t>
@@ -106,21 +111,30 @@
     <t>[1D Graph]</t>
   </si>
   <si>
-    <t>Do we need to define a secant line? That seems like too much.</t>
+    <t>The value of the derivative at a point on a curve can be approximated by the slope of a line secant with the curve near that point.</t>
   </si>
   <si>
     <t>The derivative at a point is the slope of a tangent line at that point</t>
   </si>
   <si>
-    <t>Do we need to define a tangent line? That seems like too much.</t>
+    <t>The value of the derivative at a point on a curve is equivalent to the slope of a line tangent to the curve at that point.</t>
   </si>
   <si>
     <t>The derivative is a limit</t>
   </si>
   <si>
+    <t>$\lim_{h \rightarrow 0} \frac{f(x+h)-f(x)}{h}$</t>
+  </si>
+  <si>
+    <t>What do we really want to say here?</t>
+  </si>
+  <si>
     <t>The derivative can be a function</t>
   </si>
   <si>
+    <t xml:space="preserve">For every value in the domain of a function, the function has exactly one value. </t>
+  </si>
+  <si>
     <t>The derivative of a constant is zero</t>
   </si>
   <si>
@@ -133,6 +147,9 @@
     <t>The derivative at a cusp is undefined</t>
   </si>
   <si>
+    <t> At a cusp (or kink) in a curve, the derivative (and it's value) are not defined.</t>
+  </si>
+  <si>
     <t>Variables can be held constant</t>
   </si>
   <si>
@@ -187,18 +204,30 @@
     <t>[2D Graph]</t>
   </si>
   <si>
+    <t>For a smooth, two dimensional function, a partial derivative can be found at any point and in any direction.</t>
+  </si>
+  <si>
     <t>There is a tangent line in every direction at every point</t>
   </si>
   <si>
+    <t>For a smooth, two dimensional function, a tangent line exists at any point and in any direction.</t>
+  </si>
+  <si>
     <t>The derivative is related to the density of contour lines</t>
   </si>
   <si>
     <t>[Contour Maps]</t>
   </si>
   <si>
+    <t>The magnitude of the derivative of a function is directly related to how closely together lie contour lines of the function: the closer together the contour lines, the greater the magnitude of the derivative.</t>
+  </si>
+  <si>
     <t>The value of a partial derivative depends on the value(s) of what is held constant</t>
   </si>
   <si>
+    <t>Is this really a statement about paths? I don't think we have path-related concepts.</t>
+  </si>
+  <si>
     <t>A partial derivative can be expressed in terms of other partial derivatives</t>
   </si>
   <si>
@@ -211,15 +240,21 @@
     <t>[$\vec \nabla f$]</t>
   </si>
   <si>
-    <t xml:space="preserve">For an $n-dimensional$ function $f$, the gradient of $f$ at a point is an $n$ dimensional vector </t>
+    <t>For an $n-$dimensional function $f$, the gradient of $f$ at a point is an $n-$dimensional vector </t>
   </si>
   <si>
     <t>The magnitude of the gradient is the value of the slope in the steepest direction</t>
   </si>
   <si>
+    <t>What more needs to be said?</t>
+  </si>
+  <si>
     <t>The gradient is perpendicular to contour lines</t>
   </si>
   <si>
+    <t>As the gradient lies along the direction of greatest change for a function, and contour lines lie along the direction of no change, these two objects (the gradient and contour lines) are perpendicular.</t>
+  </si>
+  <si>
     <t>All partial derivatives can be found as a slope of a tangent plane</t>
   </si>
   <si>
@@ -340,6 +375,9 @@
     <t>MTH 255</t>
   </si>
   <si>
+    <t>This concept doesn't make any sense.</t>
+  </si>
+  <si>
     <t>The magnitude of $d\vec r$ is the length of a small step along a path</t>
   </si>
   <si>
@@ -349,6 +387,9 @@
     <t>The direction of $d\vec r$ is tangent to a path</t>
   </si>
   <si>
+    <t>Tangent to what path? How is this useful?</t>
+  </si>
+  <si>
     <t>The gradient can tell you a small change in a function in any direction (differentials edition)</t>
   </si>
   <si>
@@ -367,13 +408,25 @@
     <t>The divergence at a point is a scalar. Taking the divergence of a function yields a scalar at every value in the domain of that function: a scalar field</t>
   </si>
   <si>
+    <t>$\vec\nabla\cdot\vec v = \frac{\partial v_x}{\partial x} + \frac{\partial v_y}{\partial y}+\frac{\partial v_z}{\partial z}$</t>
+  </si>
+  <si>
     <t>Put into words</t>
   </si>
   <si>
+    <t>$\vec\nabla\times\vec v = \cdots$</t>
+  </si>
+  <si>
     <t>[$\vec \nabla \times \vec v$]</t>
   </si>
   <si>
     <t>concept</t>
+  </si>
+  <si>
+    <t>$\oint\vec F\cdot d\vec A = \int\vec\nabla\cdot\vec F dV$</t>
+  </si>
+  <si>
+    <t>$\oint \vec F\cdot d\vec r = \int \vec\nabla\times\vec F\cdot d\vec A$</t>
   </si>
   <si>
     <t>The Hill</t>
@@ -846,14 +899,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>34750</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>130000</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1631204</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1726454</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>482600</xdr:rowOff>
     </xdr:to>
@@ -878,7 +931,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1042283" y="19405600"/>
+          <a:off x="3358975" y="24466550"/>
           <a:ext cx="1596454" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -890,16 +943,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>34750</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>581025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>9380</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1688354</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>333230</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -922,8 +975,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1042283" y="19227800"/>
-          <a:ext cx="1596454" cy="407314"/>
+          <a:off x="3320875" y="25022175"/>
+          <a:ext cx="1596454" cy="399905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -934,16 +987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>9379</xdr:rowOff>
+      <xdr:rowOff>18904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1631204</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>569310</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1735979</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>7335</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -966,8 +1019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1007533" y="18432846"/>
-          <a:ext cx="1631204" cy="566354"/>
+          <a:off x="3333750" y="25498279"/>
+          <a:ext cx="1631204" cy="559931"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -978,16 +1031,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1969379</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2302754</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1010,8 +1063,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1007533" y="18999200"/>
-          <a:ext cx="1969379" cy="584200"/>
+          <a:off x="3562350" y="26079450"/>
+          <a:ext cx="1969379" cy="581026"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1323,8 +1376,8 @@
   <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1380,7 +1433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48">
+    <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="32.1">
+    <row r="5" spans="1:12" ht="31.5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1493,18 +1546,14 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" ref="I5:I13" si="0">"A long description for "&amp;B5 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The derivative can be approximated by the slope of a secant line is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I5" t="s">
+        <v>26</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="32.1">
+    </row>
+    <row r="6" spans="1:12" ht="31.5">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1527,18 +1576,14 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>A long description for The derivative at a point is the slope of a tangent line at that point is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I6" t="s">
+        <v>28</v>
       </c>
       <c r="K6" t="s">
         <v>18</v>
       </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="32.1">
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1561,20 +1606,22 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>A long description for The derivative is a limit is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I7" t="s">
+        <v>30</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="32.1">
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <f>ROW()</f>
@@ -1592,27 +1639,30 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>A long description for The derivative can be a function is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I8" t="s">
+        <v>33</v>
       </c>
       <c r="K8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="32.1">
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="43.5" customHeight="1">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <f>ROW()</f>
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
+      <c r="D9" t="str">
+        <f>"["&amp;B2&amp;"]"</f>
+        <v>[Difference / Change]</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -1624,8 +1674,8 @@
         <v>16</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>A long description for The derivative of a constant is zero is not yet available--feel free to give us your suggestions on the poster!</v>
+        <f>"The derivative of a constant is always zero. This can be understood by thinking of '"&amp;B4 &amp;",' as the amount by which a constant changes is zero."</f>
+        <v>The derivative of a constant is always zero. This can be understood by thinking of 'The derivative is a ratio of small changes,' as the amount by which a constant changes is zero.</v>
       </c>
       <c r="K9" t="s">
         <v>18</v>
@@ -1636,7 +1686,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <f>ROW()</f>
@@ -1655,7 +1705,7 @@
         <v>16</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
+        <f>"A long description for "&amp;B10 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The derivative is a linear function is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K10" t="s">
@@ -1667,7 +1717,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <f>ROW()</f>
@@ -1686,19 +1736,19 @@
         <v>16</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I5:I13" si="0">"A long description for "&amp;B11 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for Power law is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="32.1">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <f>ROW()</f>
@@ -1716,9 +1766,8 @@
       <c r="G12" t="s">
         <v>16</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>A long description for The derivative at a cusp is undefined is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I12" t="s">
+        <v>38</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
@@ -1729,7 +1778,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <f>ROW()</f>
@@ -1755,7 +1804,7 @@
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1763,7 +1812,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <f>ROW()</f>
@@ -1776,24 +1825,24 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15">
         <f>ROW()</f>
@@ -1806,19 +1855,19 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K15" t="s">
         <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="47.25">
@@ -1826,7 +1875,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <f>ROW()</f>
@@ -1839,25 +1888,25 @@
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="63.95">
+    <row r="17" spans="1:12" ht="63.95">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <f>ROW()</f>
@@ -1870,24 +1919,24 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="48">
+    <row r="18" spans="1:12" ht="48">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <f>ROW()</f>
@@ -1901,24 +1950,24 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="32.1">
+    <row r="19" spans="1:12" ht="31.5">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C19">
         <f>ROW()</f>
@@ -1931,118 +1980,118 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="31.5">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <f>ROW()</f>
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="47.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <f>ROW()</f>
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="63">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22">
+        <f>ROW()</f>
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
         <v>52</v>
       </c>
-      <c r="G19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" ref="I19:I27" si="1">"A long description for "&amp;B19 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for There is a partial derivative in every direction at any point is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="32.1">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="G22" t="s">
         <v>53</v>
       </c>
-      <c r="C20">
-        <f>ROW()</f>
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for There is a tangent line in every direction at every point is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="32.1">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21">
-        <f>ROW()</f>
-        <v>21</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The derivative is related to the density of contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="48">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22">
-        <f>ROW()</f>
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" t="s">
-        <v>49</v>
-      </c>
       <c r="I22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I19:I27" si="1">"A long description for "&amp;B22 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The value of a partial derivative depends on the value(s) of what is held constant is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="78.75">
+      <c r="L22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="78.75">
       <c r="A23" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <f>ROW()</f>
@@ -2056,10 +2105,10 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
@@ -2069,12 +2118,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="32.1">
+    <row r="24" spans="1:12" ht="31.5">
       <c r="A24" t="s">
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <f>ROW()</f>
@@ -2087,21 +2136,21 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="48">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="47.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <f>ROW()</f>
@@ -2115,25 +2164,28 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="1"/>
+        <f>"A long description for "&amp;B25 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
         <v>A long description for The magnitude of the gradient is the value of the slope in the steepest direction is not yet available--feel free to give us your suggestions on the poster!</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="32.1">
+      <c r="L25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C26">
         <f>ROW()</f>
@@ -2146,25 +2198,24 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The gradient is perpendicular to contour lines is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>53</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="48">
+    <row r="27" spans="1:12" ht="31.5">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <f>ROW()</f>
@@ -2178,10 +2229,10 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
@@ -2190,13 +2241,16 @@
       <c r="K27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="32.1">
+      <c r="L27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" t="s">
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <f>ROW()</f>
@@ -2209,10 +2263,10 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I28" t="str">
         <f>"This is the long description for " &amp;B28 &amp;". It is quite a long description!"</f>
@@ -2221,73 +2275,76 @@
       <c r="K28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="78.75">
+      <c r="L28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="78.75">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29">
+        <f>ROW()</f>
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
         <v>66</v>
       </c>
-      <c r="C29">
-        <f>ROW()</f>
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" t="s">
-        <v>58</v>
-      </c>
       <c r="G29" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
         <v>68</v>
       </c>
-      <c r="C30">
-        <f>ROW()</f>
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" t="s">
-        <v>60</v>
-      </c>
       <c r="G30" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="63.95">
+    <row r="31" spans="1:12" ht="78.75">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C31">
         <v>28</v>
@@ -2299,24 +2356,27 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I31" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="96">
+      <c r="L31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="96">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2331,19 +2391,19 @@
         <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="I32" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
@@ -2351,10 +2411,10 @@
     </row>
     <row r="33" spans="1:12" ht="96">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2369,19 +2429,19 @@
         <v>[There is a partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I33" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="J33" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
@@ -2389,10 +2449,10 @@
     </row>
     <row r="34" spans="1:12" ht="71.25" customHeight="1">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2407,19 +2467,19 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="I34" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J34" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
@@ -2427,10 +2487,10 @@
     </row>
     <row r="35" spans="1:12" ht="96">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2444,16 +2504,16 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I35" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J35" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
@@ -2461,10 +2521,10 @@
     </row>
     <row r="36" spans="1:12" ht="111.95">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2479,19 +2539,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H36" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="I36" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
@@ -2499,10 +2559,10 @@
     </row>
     <row r="37" spans="1:12" ht="96">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2517,30 +2577,30 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F37" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I37" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="J37" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="48">
+    <row r="38" spans="1:12" ht="47.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <f>ROW()</f>
@@ -2554,10 +2614,10 @@
         <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G38" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I38" t="str">
         <f>"A long description for "&amp;B38 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2566,13 +2626,16 @@
       <c r="K38" t="s">
         <v>18</v>
       </c>
+      <c r="L38" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="33.950000000000003" customHeight="1">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2586,10 +2649,10 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I39" t="str">
         <f>"A long description for "&amp;B39 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2598,13 +2661,16 @@
       <c r="K39" t="s">
         <v>18</v>
       </c>
+      <c r="L39" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="33.950000000000003" customHeight="1">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
@@ -2617,10 +2683,10 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I40" t="str">
         <f>"A long description for "&amp;B40 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2629,13 +2695,16 @@
       <c r="K40" t="s">
         <v>18</v>
       </c>
+      <c r="L40" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="48">
       <c r="A41" t="s">
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C41">
         <f>ROW()</f>
@@ -2649,13 +2718,13 @@
         <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="G41" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I41" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="K41" t="s">
         <v>18</v>
@@ -2666,7 +2735,7 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
@@ -2679,10 +2748,10 @@
         <v>14</v>
       </c>
       <c r="F42" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="I42" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
@@ -2692,7 +2761,9 @@
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="C43" s="1">
         <f>ROW()</f>
         <v>43</v>
@@ -2704,10 +2775,10 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2716,14 +2787,16 @@
         <v>18</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30.95" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C44" s="1">
         <f>ROW()</f>
         <v>44</v>
@@ -2735,10 +2808,10 @@
         <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2747,14 +2820,16 @@
         <v>18</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="45" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="C45" s="1">
         <f>ROW()</f>
         <v>45</v>
@@ -2769,7 +2844,7 @@
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2778,14 +2853,16 @@
         <v>18</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="45.95" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="C46" s="1">
         <f>ROW()</f>
         <v>46</v>
@@ -2800,7 +2877,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2809,15 +2886,15 @@
         <v>18</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="111.95">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C47">
         <f>ROW()</f>
@@ -2832,19 +2909,19 @@
         <v>[The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F47" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="G47" t="s">
+        <v>113</v>
+      </c>
+      <c r="H47" t="s">
         <v>103</v>
       </c>
-      <c r="H47" t="s">
-        <v>93</v>
-      </c>
       <c r="I47" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="J47" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="K47" t="s">
         <v>18</v>
@@ -2852,10 +2929,10 @@
     </row>
     <row r="48" spans="1:12" ht="96">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="C48">
         <f>ROW()</f>
@@ -2870,33 +2947,33 @@
         <v>[The gradient can tell you a small change in a function in any direction (differentials edition)]</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G48" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H48" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="I48" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="J48" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="K48" t="s">
         <v>18</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="32.1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="32.1">
       <c r="A49" t="s">
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -2910,10 +2987,10 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G49" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" ref="I49:I63" si="2">"A long description for "&amp;B49 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -2923,12 +3000,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="48">
+    <row r="50" spans="1:12" ht="48">
       <c r="A50" t="s">
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -2941,10 +3018,10 @@
         <v>14</v>
       </c>
       <c r="F50" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G50" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
@@ -2954,12 +3031,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.75">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" t="s">
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -2972,10 +3049,10 @@
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G51" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="2"/>
@@ -2985,12 +3062,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="32.1">
+    <row r="52" spans="1:12" ht="32.1">
       <c r="A52" t="s">
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -3003,10 +3080,10 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G52" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="2"/>
@@ -3016,12 +3093,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="32.1">
+    <row r="53" spans="1:12" ht="32.1">
       <c r="A53" t="s">
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -3034,10 +3111,10 @@
         <v>14</v>
       </c>
       <c r="F53" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G53" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="2"/>
@@ -3047,12 +3124,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="32.1">
+    <row r="54" spans="1:12" ht="32.1">
       <c r="A54" t="s">
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -3065,24 +3142,24 @@
         <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G54" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I54" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="K54" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="31.5">
+    <row r="55" spans="1:12" ht="31.5">
       <c r="A55" t="s">
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C55">
         <f>ROW()</f>
@@ -3095,10 +3172,10 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G55" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="2"/>
@@ -3108,12 +3185,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="32.1">
+    <row r="56" spans="1:12" ht="32.1">
       <c r="A56" t="s">
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -3126,10 +3203,10 @@
         <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G56" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="2"/>
@@ -3139,12 +3216,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="32.1">
+    <row r="57" spans="1:12" ht="32.1">
       <c r="A57" t="s">
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -3157,10 +3234,10 @@
         <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G57" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="2"/>
@@ -3170,12 +3247,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="48">
+    <row r="58" spans="1:12" ht="48">
       <c r="A58" t="s">
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C58">
         <f>ROW()</f>
@@ -3188,10 +3265,10 @@
         <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G58" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="2"/>
@@ -3201,12 +3278,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="32.1">
+    <row r="59" spans="1:12" ht="31.5">
       <c r="A59" t="s">
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -3219,10 +3296,10 @@
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G59" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="2"/>
@@ -3231,13 +3308,16 @@
       <c r="K59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="31.5">
+      <c r="L59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="31.5">
       <c r="A60" t="s">
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C60">
         <f>ROW()</f>
@@ -3250,10 +3330,10 @@
         <v>14</v>
       </c>
       <c r="F60" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G60" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="2"/>
@@ -3262,13 +3342,16 @@
       <c r="K60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="32.1">
+      <c r="L60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="31.5">
       <c r="A61" t="s">
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -3281,10 +3364,10 @@
         <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G61" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="2"/>
@@ -3293,13 +3376,16 @@
       <c r="K61" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="32.1">
+      <c r="L61" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="31.5">
       <c r="A62" t="s">
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -3312,10 +3398,10 @@
         <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="G62" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
@@ -3324,13 +3410,16 @@
       <c r="K62" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="63.95">
+      <c r="L62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="63">
       <c r="A63" t="s">
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -3343,10 +3432,10 @@
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="G63" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="2"/>
@@ -3355,13 +3444,16 @@
       <c r="K63" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="94.5">
+      <c r="L63" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="94.5">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3376,19 +3468,19 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="G64" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H64" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="I64" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="J64" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="K64" t="s">
         <v>18</v>
@@ -3396,10 +3488,10 @@
     </row>
     <row r="65" spans="1:12" ht="128.1">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C65">
         <f>ROW()</f>
@@ -3414,19 +3506,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F65" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="G65" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="I65" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="J65" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="K65" t="s">
         <v>18</v>
@@ -3434,10 +3526,10 @@
     </row>
     <row r="66" spans="1:12" ht="111.95">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3452,19 +3544,19 @@
         <v>[The gradient's dimension is the same as real space. The gradient lives in the domain, The gradient is a local quantity]</v>
       </c>
       <c r="F66" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="G66" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H66" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="I66" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="J66" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="K66" t="s">
         <v>18</v>
@@ -3472,10 +3564,10 @@
     </row>
     <row r="67" spans="1:12" ht="159.94999999999999">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3490,19 +3582,19 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F67" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="G67" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H67" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="I67" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="J67" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="K67" t="s">
         <v>18</v>
@@ -3510,10 +3602,10 @@
     </row>
     <row r="68" spans="1:12" ht="159.94999999999999">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3528,19 +3620,19 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F68" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="G68" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="H68" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="I68" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="J68" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="K68" t="s">
         <v>18</v>
@@ -3551,7 +3643,7 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3565,16 +3657,16 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G69" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H69" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="I69" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="K69" t="s">
         <v>18</v>
@@ -3585,7 +3677,7 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3598,10 +3690,10 @@
         <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G70" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ref="I70:I77" si="3">"A long description for "&amp;B70 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
@@ -3611,7 +3703,7 @@
         <v>18</v>
       </c>
       <c r="L70" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="32.1">
@@ -3619,7 +3711,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3635,7 +3727,7 @@
         <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="3"/>
@@ -3650,7 +3742,7 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C72">
         <f>ROW()</f>
@@ -3663,13 +3755,13 @@
         <v>14</v>
       </c>
       <c r="F72" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G72" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I72" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="K72" t="s">
         <v>18</v>
@@ -3680,7 +3772,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C73">
         <f>ROW()</f>
@@ -3693,10 +3785,10 @@
         <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G73" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I73" t="str">
         <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
@@ -3711,7 +3803,7 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="C74">
         <f>ROW()</f>
@@ -3725,13 +3817,13 @@
         <v>14</v>
       </c>
       <c r="F74" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="G74" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I74" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="K74" t="s">
         <v>18</v>
@@ -3742,7 +3834,7 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3758,16 +3850,16 @@
         <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I75" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="K75" t="s">
         <v>18</v>
       </c>
       <c r="L75" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="96">
@@ -3775,7 +3867,7 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -3789,13 +3881,13 @@
         <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G76" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H76" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="3"/>
@@ -3810,7 +3902,7 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C77">
         <f>ROW()</f>
@@ -3824,13 +3916,13 @@
         <v>14</v>
       </c>
       <c r="F77" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G77" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H77" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="3"/>
@@ -3845,7 +3937,7 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -3859,13 +3951,13 @@
         <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="G78" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I78" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="K78" t="s">
         <v>18</v>
@@ -3876,7 +3968,7 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -3889,13 +3981,13 @@
         <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="G79" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I79" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="K79" t="s">
         <v>18</v>
@@ -3906,7 +3998,7 @@
         <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -3920,13 +4012,13 @@
         <v>14</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G80" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="I80" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="K80" t="s">
         <v>18</v>
@@ -3934,10 +4026,10 @@
     </row>
     <row r="81" spans="1:12" ht="111.95">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="C81">
         <f>ROW()</f>
@@ -3952,19 +4044,19 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G81" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H81" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="I81" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="J81" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="K81" t="s">
         <v>18</v>
@@ -3972,10 +4064,10 @@
     </row>
     <row r="82" spans="1:12" ht="111.95">
       <c r="A82" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -3990,19 +4082,19 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F82" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="G82" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H82" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="I82" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="J82" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="K82" t="s">
         <v>18</v>
@@ -4010,10 +4102,10 @@
     </row>
     <row r="83" spans="1:12" ht="93" customHeight="1">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -4028,19 +4120,19 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F83" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="G83" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H83" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="I83" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="J83" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="K83" t="s">
         <v>18</v>
@@ -4048,10 +4140,10 @@
     </row>
     <row r="84" spans="1:12" ht="240">
       <c r="A84" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -4066,50 +4158,50 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="G84" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="H84" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="I84" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="J84" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="K84" t="s">
         <v>18</v>
       </c>
       <c r="L84" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:12">
       <c r="L85" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:12">
       <c r="L86" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:12">
       <c r="L87" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:12">
       <c r="L88" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="L89" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4194,7 +4286,7 @@
         <v>$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,Kinesthetic,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.95" customHeight="1">

</xml_diff>

<commit_message>
make activities display nicer when multiple teach same concept
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0AA3D5-1D87-7248-9894-9D6521F420BA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39456E60-60F0-9741-9BCE-C0BB5CCC00B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1482,8 +1482,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2479,6 +2479,10 @@
       <c r="D32" t="str">
         <f>"["&amp;B4&amp;", "&amp;B13&amp;", "&amp;B17&amp;"]"</f>
         <v>[The derivative is a ratio of small changes, Variables can be held constant, "With respect to what" matters]</v>
+      </c>
+      <c r="E32" t="str">
+        <f>"["&amp;B18&amp;"]"</f>
+        <v>[Derivatives can be found while holding one or more variables constant]</v>
       </c>
       <c r="F32" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
link to nicer concept map and fix problem in spreadsheet (concept requireing itself)
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21320"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D6492-8911-5F45-A4C6-121AA204A23E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D6492-8911-5F45-A4C6-121AA204A23E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="3880" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="258">
   <si>
     <t>Act or Con</t>
   </si>
@@ -1472,8 +1472,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1652,7 +1652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51">
+    <row r="6" spans="1:12" ht="47.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1663,9 +1663,8 @@
         <f>ROW()</f>
         <v>6</v>
       </c>
-      <c r="D6" t="str">
-        <f>"["&amp;B6&amp;"]"</f>
-        <v>[The derivative at a point is the slope of a tangent line at that point]</v>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -4389,7 +4388,7 @@
       <formula>LEN(TRIM(L2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D47 D49:D1048576">
+  <conditionalFormatting sqref="D49:D1048576 D1:D47">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>$D1="[]"</formula>
     </cfRule>

</xml_diff>

<commit_message>
latest edit from Mike on the spreadsheet
</commit_message>
<xml_diff>
--- a/progression.xlsx
+++ b/progression.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21331"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikeArien/Library/Application Support/Box/Box Edit/Documents/283979119114/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D6C026-8A89-694A-8271-B26577787060}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A728C5-DE81-6D4A-9E92-7CB0BFDE2333}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Representations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="266">
   <si>
     <t>Act or Con</t>
   </si>
@@ -289,9 +284,6 @@
   </si>
   <si>
     <t>[$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$]</t>
-  </si>
-  <si>
-    <t>This is the long description for The components of the gradient are partial derivatives. It is quite a long description!</t>
   </si>
   <si>
     <t>What do we really want to say in the long description?</t>
@@ -791,9 +783,6 @@
     <t>pdm.jpg</t>
   </si>
   <si>
-    <t>NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
-  </si>
-  <si>
     <t>incycchainrule</t>
   </si>
   <si>
@@ -810,13 +799,40 @@
   </si>
   <si>
     <t>Representations Used (Columns A-C make this list)</t>
+  </si>
+  <si>
+    <t>FIXME: do we mean to say that the derivative is a linar operator?</t>
+  </si>
+  <si>
+    <t>FIXME: Is this really a statement about paths? I don't think we have path-related concepts.</t>
+  </si>
+  <si>
+    <t>FIXME: What more do we want the long description to say than the short dscription?</t>
+  </si>
+  <si>
+    <t>FIXME: This concept does not make any sense.</t>
+  </si>
+  <si>
+    <t>FIXME: What's the point of this concept?</t>
+  </si>
+  <si>
+    <t>FIXME: Tangent to what path? How is this useful?</t>
+  </si>
+  <si>
+    <t>FIXME: Does the difference between zapping with d and taking the total differential need to be articulated?</t>
+  </si>
+  <si>
+    <t>FIXME: What?</t>
+  </si>
+  <si>
+    <t>FIXME: NOT CORRECT DESCRIPTION: In this activity, students experimentally determine various derivatives using the partial derivate machine, a mechanical analogue for thermodynamic systems. Students explore the ratio, limit, and function aspects of multi-variable derivatives, with an emphasis on holding different variables constant. This activity is also an excellent exercise in representational fluency, as students must coordinate experiments and tables of data with (new) symbolic notations.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -827,13 +843,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -873,7 +882,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -891,9 +900,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1474,27 +1480,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="E70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
-    <col min="3" max="3" width="9.625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.625" customWidth="1"/>
-    <col min="5" max="5" width="39.625" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="72.625" customWidth="1"/>
-    <col min="10" max="10" width="11.875" customWidth="1"/>
-    <col min="12" max="12" width="33.125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="72.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="12" max="12" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.100000000000001">
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="51">
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="33.950000000000003">
+    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="33.950000000000003">
+    <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="33.950000000000003">
+    <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51">
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="51">
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="51">
+    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="43.5" customHeight="1">
+    <row r="9" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="33.950000000000003">
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1798,9 +1804,8 @@
       <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="I10" t="str">
-        <f>"A long description for "&amp;B10 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: do we mean to say that the derivative is a linar operator?"</f>
-        <v>A long description for The derivative is a linear function is not yet available--feel free to give us your suggestions on the poster! FIXME: do we mean to say that the derivative is a linar operator?</v>
+      <c r="I10" t="s">
+        <v>257</v>
       </c>
       <c r="K10" t="s">
         <v>18</v>
@@ -1809,7 +1814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.100000000000001">
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.100000000000001">
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1869,7 +1874,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="31.5">
+    <row r="13" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1899,7 +1904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="68.099999999999994">
+    <row r="14" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1929,7 +1934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.100000000000001">
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="51">
+    <row r="16" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1990,7 +1995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="68.099999999999994">
+    <row r="17" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2020,7 +2025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="51">
+    <row r="18" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2051,7 +2056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="33.950000000000003">
+    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2081,7 +2086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="33.950000000000003">
+    <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2111,7 +2116,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="63">
+    <row r="21" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2142,7 +2147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="51">
+    <row r="22" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2165,9 +2170,8 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-      <c r="I22" t="str">
-        <f>"A long description for "&amp;B22 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: Is this really a statement about paths? I don't think we have path-related concepts."</f>
-        <v>A long description for The value of a partial derivative depends on the value(s) of what is held constant is not yet available--feel free to give us your suggestions on the poster! FIXME: Is this really a statement about paths? I don't think we have path-related concepts.</v>
+      <c r="I22" t="s">
+        <v>258</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -2176,7 +2180,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="84.95">
+    <row r="23" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2200,9 +2204,8 @@
       <c r="G23" t="s">
         <v>54</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" ref="I22:I23" si="0">"A long description for "&amp;B23 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for A partial derivative can be expressed in terms of other partial derivatives is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I23" t="s">
+        <v>136</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
@@ -2211,7 +2214,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="33.950000000000003">
+    <row r="24" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="51">
+    <row r="25" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2262,9 +2265,8 @@
       <c r="G25" t="s">
         <v>54</v>
       </c>
-      <c r="I25" t="str">
-        <f>"A long description for "&amp;B25 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The magnitude of the gradient is the value of the slope in the steepest direction is not yet available--feel free to give us your suggestions on the poster!</v>
+      <c r="I25" t="s">
+        <v>259</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
@@ -2273,7 +2275,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="51">
+    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2303,7 +2305,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="51">
+    <row r="27" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2334,7 +2336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="84.95">
+    <row r="28" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="84.95">
+    <row r="29" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="17.100000000000001">
+    <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="68.099999999999994">
+    <row r="31" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2449,21 +2451,21 @@
         <v>54</v>
       </c>
       <c r="I31" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
         <v>86</v>
       </c>
-      <c r="K31" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" t="s">
+    </row>
+    <row r="32" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="102">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>88</v>
-      </c>
-      <c r="B32" t="s">
-        <v>89</v>
       </c>
       <c r="C32">
         <f>ROW()</f>
@@ -2484,24 +2486,24 @@
         <v>54</v>
       </c>
       <c r="H32" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" t="s">
         <v>90</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>91</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
         <v>92</v>
-      </c>
-      <c r="K32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="102">
-      <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
       </c>
       <c r="C33">
         <f>ROW()</f>
@@ -2516,30 +2518,30 @@
         <v>[There is a partial derivative in every direction at any point, There is a tangent line in every direction at every point, The derivative is related to the density of contour lines, The value of a partial derivative depends on the value(s) of what is held constant]</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G33" t="s">
         <v>54</v>
       </c>
       <c r="H33" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" t="s">
         <v>95</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>96</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
         <v>97</v>
-      </c>
-      <c r="K33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
       </c>
       <c r="C34">
         <f>ROW()</f>
@@ -2554,30 +2556,30 @@
         <v>[A partial derivative can be expressed in terms of other partial derivatives]</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
         <v>54</v>
       </c>
       <c r="H34" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34" t="s">
         <v>100</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>101</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
         <v>102</v>
-      </c>
-      <c r="K34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="102">
-      <c r="A35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" t="s">
-        <v>103</v>
       </c>
       <c r="C35">
         <f>ROW()</f>
@@ -2591,27 +2593,27 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G35" t="s">
         <v>54</v>
       </c>
       <c r="I35" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" t="s">
         <v>105</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
         <v>106</v>
-      </c>
-      <c r="K35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="119.1">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>107</v>
       </c>
       <c r="C36">
         <f>ROW()</f>
@@ -2626,30 +2628,30 @@
         <v>[The gradient points in the direction of greatest increase of the function, The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G36" t="s">
         <v>54</v>
       </c>
       <c r="H36" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" t="s">
         <v>109</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>110</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
         <v>111</v>
-      </c>
-      <c r="K36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="102">
-      <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" t="s">
-        <v>112</v>
       </c>
       <c r="C37">
         <f>ROW()</f>
@@ -2664,57 +2666,57 @@
         <v>[All partial derivatives can be found as a slope of a tangent plane, The components of the gradient are partial derivatives]</v>
       </c>
       <c r="F37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G37" t="s">
         <v>54</v>
       </c>
       <c r="H37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" t="s">
         <v>114</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>115</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="K37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="6" customFormat="1" ht="135.94999999999999">
-      <c r="A38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="D38" s="6" t="str">
         <f>"["&amp;B6&amp;", "&amp;B$24&amp;"]"</f>
         <v>[The derivative at a point is the slope of a tangent line at that point, The gradient is a vector]</v>
       </c>
       <c r="F38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="K38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L38" s="6" t="s">
+    </row>
+    <row r="39" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="51">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
-        <v>122</v>
       </c>
       <c r="C39">
         <f>ROW()</f>
@@ -2728,28 +2730,27 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" t="s">
+        <v>260</v>
+      </c>
+      <c r="K39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39" t="s">
         <v>123</v>
       </c>
-      <c r="G39" t="s">
-        <v>119</v>
-      </c>
-      <c r="I39" t="str">
-        <f>"A long description for "&amp;B39 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: This concept does not make any sense."</f>
-        <v>A long description for Each component of $d \vec r$ is an arbitrary small change between two arbitrary position vectors.  is not yet available--feel free to give us your suggestions on the poster! FIXME: This concept does not make any sense.</v>
-      </c>
-      <c r="K39" t="s">
-        <v>18</v>
-      </c>
-      <c r="L39" t="s">
+    </row>
+    <row r="40" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="33.950000000000003" customHeight="1">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" t="s">
-        <v>125</v>
       </c>
       <c r="C40">
         <f>ROW()</f>
@@ -2763,62 +2764,60 @@
         <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G40" t="s">
+        <v>125</v>
+      </c>
+      <c r="I40" t="s">
+        <v>261</v>
+      </c>
+      <c r="K40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" t="s">
         <v>126</v>
       </c>
-      <c r="I40" t="str">
-        <f>"A long description for "&amp;B40 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: What's the point of this concept?"</f>
-        <v>A long description for The magnitude of $d\vec r$ is the length of a small step along a path is not yet available--feel free to give us your suggestions on the poster! FIXME: What's the point of this concept?</v>
-      </c>
-      <c r="K40" t="s">
-        <v>18</v>
-      </c>
-      <c r="L40" t="s">
+    </row>
+    <row r="41" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="33.950000000000003" customHeight="1">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C41">
+        <f>ROW()</f>
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I41" t="s">
+        <v>262</v>
+      </c>
+      <c r="K41" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41" t="s">
         <v>128</v>
       </c>
-      <c r="C41">
-        <f>ROW()</f>
-        <v>41</v>
-      </c>
-      <c r="D41" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" t="s">
-        <v>123</v>
-      </c>
-      <c r="G41" t="s">
-        <v>126</v>
-      </c>
-      <c r="I41" t="str">
-        <f>"A long description for "&amp;B41 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: Tangent to what path? How is this useful?"</f>
-        <v>A long description for The direction of $d\vec r$ is tangent to a path is not yet available--feel free to give us your suggestions on the poster! FIXME: Tangent to what path? How is this useful?</v>
-      </c>
-      <c r="K41" t="s">
-        <v>18</v>
-      </c>
-      <c r="L41" t="s">
+    </row>
+    <row r="42" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="51">
-      <c r="A42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" t="s">
-        <v>130</v>
       </c>
       <c r="C42">
         <f>ROW()</f>
@@ -2832,122 +2831,122 @@
         <v>14</v>
       </c>
       <c r="F42" t="s">
+        <v>130</v>
+      </c>
+      <c r="G42" t="s">
+        <v>118</v>
+      </c>
+      <c r="I42" t="s">
         <v>131</v>
       </c>
-      <c r="G42" t="s">
-        <v>119</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
         <v>132</v>
       </c>
-      <c r="K42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="33.950000000000003">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C43">
+        <f>ROW()</f>
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" t="s">
         <v>133</v>
       </c>
-      <c r="C43">
-        <f>ROW()</f>
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="I43" t="s">
         <v>134</v>
       </c>
-      <c r="I43" t="s">
+      <c r="K43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="51" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1">
+        <f>ROW()</f>
+        <v>44</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" t="s">
         <v>136</v>
-      </c>
-      <c r="C44" s="1">
-        <f>ROW()</f>
-        <v>44</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" t="s">
-        <v>134</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L44" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="30.95" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1">
+        <f>ROW()</f>
+        <v>45</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="1">
-        <f>ROW()</f>
-        <v>45</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" t="s">
-        <v>140</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="1" t="s">
-        <v>137</v>
+      <c r="I45" t="s">
+        <v>136</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="45" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C46" s="1">
         <f>ROW()</f>
         <v>46</v>
@@ -2962,26 +2961,26 @@
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="1" t="s">
-        <v>137</v>
+      <c r="I46" t="s">
+        <v>136</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="45.95" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" s="1">
         <f>ROW()</f>
@@ -2997,26 +2996,26 @@
         <v>14</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="1" t="s">
-        <v>137</v>
+      <c r="I47" t="s">
+        <v>136</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="6" customFormat="1" ht="45.95" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="6" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>14</v>
@@ -3029,28 +3028,28 @@
         <v>[The gradient is a vector, The gradient points in the direction of greatest increase of the function, The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" t="s">
+        <v>136</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" t="s">
         <v>145</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="119.1">
-      <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" t="s">
-        <v>146</v>
       </c>
       <c r="C49">
         <f>ROW()</f>
@@ -3065,30 +3064,30 @@
         <v>[The gradient points in the direction of greatest increase of the function, The magnitude of the gradient is the value of the slope in the steepest direction, The gradient is perpendicular to contour lines]</v>
       </c>
       <c r="F49" t="s">
+        <v>146</v>
+      </c>
+      <c r="G49" t="s">
+        <v>118</v>
+      </c>
+      <c r="H49" t="s">
+        <v>108</v>
+      </c>
+      <c r="I49" t="s">
         <v>147</v>
       </c>
-      <c r="G49" t="s">
-        <v>119</v>
-      </c>
-      <c r="H49" t="s">
-        <v>109</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>148</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
         <v>149</v>
-      </c>
-      <c r="K49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="102">
-      <c r="A50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" t="s">
-        <v>150</v>
       </c>
       <c r="C50">
         <f>ROW()</f>
@@ -3106,30 +3105,30 @@
         <v>62</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H50" t="s">
+        <v>150</v>
+      </c>
+      <c r="I50" t="s">
         <v>151</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>152</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K50" t="s">
-        <v>18</v>
-      </c>
-      <c r="L50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="33.950000000000003">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
-        <v>155</v>
       </c>
       <c r="C51">
         <f>ROW()</f>
@@ -3143,28 +3142,27 @@
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" t="s">
-        <v>126</v>
-      </c>
-      <c r="I51" t="str">
-        <f>"A long description for "&amp;B51 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for Differential form of $\vec r$ in spherical and cylindrical coordinates is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I51" t="s">
+        <v>136</v>
       </c>
       <c r="K51" t="s">
         <v>18</v>
       </c>
       <c r="L51" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="51">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" t="s">
-        <v>157</v>
       </c>
       <c r="C52">
         <f>ROW()</f>
@@ -3180,22 +3178,22 @@
         <v>70</v>
       </c>
       <c r="G52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I52" t="s">
+        <v>157</v>
+      </c>
+      <c r="K52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
         <v>158</v>
-      </c>
-      <c r="K52" t="s">
-        <v>18</v>
-      </c>
-      <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="1:12" ht="68.099999999999994">
-      <c r="A53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" t="s">
-        <v>159</v>
       </c>
       <c r="C53">
         <f>ROW()</f>
@@ -3212,21 +3210,21 @@
         <v>70</v>
       </c>
       <c r="G53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I53" t="s">
+        <v>159</v>
+      </c>
+      <c r="K53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
         <v>160</v>
-      </c>
-      <c r="K53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="51">
-      <c r="A54" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" t="s">
-        <v>161</v>
       </c>
       <c r="C54">
         <f>ROW()</f>
@@ -3242,54 +3240,54 @@
         <v>70</v>
       </c>
       <c r="G54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I54" t="s">
+        <v>161</v>
+      </c>
+      <c r="K54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
         <v>162</v>
       </c>
-      <c r="K54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="33.950000000000003">
-      <c r="A55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C55">
+        <f>ROW()</f>
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" t="s">
+        <v>125</v>
+      </c>
+      <c r="I55" t="s">
         <v>163</v>
       </c>
-      <c r="C55">
-        <f>ROW()</f>
-        <v>55</v>
-      </c>
-      <c r="D55" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" t="s">
-        <v>134</v>
-      </c>
-      <c r="G55" t="s">
-        <v>126</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="K55" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K55" t="s">
-        <v>18</v>
-      </c>
-      <c r="L55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="33.950000000000003">
-      <c r="A56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" t="s">
-        <v>166</v>
       </c>
       <c r="C56">
         <f>ROW()</f>
@@ -3303,27 +3301,27 @@
         <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I56" t="s">
+        <v>166</v>
+      </c>
+      <c r="K56" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K56" t="s">
-        <v>18</v>
-      </c>
-      <c r="L56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="33.950000000000003">
-      <c r="A57" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57" t="s">
-        <v>169</v>
       </c>
       <c r="C57">
         <f>ROW()</f>
@@ -3337,62 +3335,60 @@
         <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G57" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" t="str">
-        <f>"A long description for "&amp;B57 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The divergence is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I57" t="s">
+        <v>136</v>
       </c>
       <c r="K57" t="s">
         <v>18</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="33.950000000000003">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>12</v>
       </c>
       <c r="B58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58">
+        <f>ROW()</f>
+        <v>58</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" t="s">
+        <v>133</v>
+      </c>
+      <c r="G58" t="s">
+        <v>125</v>
+      </c>
+      <c r="I58" t="s">
+        <v>136</v>
+      </c>
+      <c r="K58" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C58">
-        <f>ROW()</f>
-        <v>58</v>
-      </c>
-      <c r="D58" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" t="s">
-        <v>134</v>
-      </c>
-      <c r="G58" t="s">
-        <v>126</v>
-      </c>
-      <c r="I58" t="str">
-        <f>"A long description for "&amp;B58 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME not a complete concept"</f>
-        <v>A long description for The divergence of the electric field is equal to is not yet available--feel free to give us your suggestions on the poster! FIXME not a complete concept</v>
-      </c>
-      <c r="K58" t="s">
-        <v>18</v>
-      </c>
-      <c r="L58" s="1" t="s">
+    </row>
+    <row r="59" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="33.950000000000003">
-      <c r="A59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" t="s">
-        <v>172</v>
       </c>
       <c r="C59">
         <f>ROW()</f>
@@ -3406,62 +3402,60 @@
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G59" t="s">
-        <v>126</v>
-      </c>
-      <c r="I59" t="str">
-        <f t="shared" ref="I57:I65" si="1">"A long description for "&amp;B59 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for The divergence of the magnetic field is zero is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I59" t="s">
+        <v>136</v>
       </c>
       <c r="K59" t="s">
         <v>18</v>
       </c>
       <c r="L59" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="51">
-      <c r="A60" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C60">
+        <f>ROW()</f>
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" t="s">
+        <v>139</v>
+      </c>
+      <c r="G60" t="s">
+        <v>125</v>
+      </c>
+      <c r="I60" t="s">
+        <v>136</v>
+      </c>
+      <c r="K60" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C60">
-        <f>ROW()</f>
-        <v>60</v>
-      </c>
-      <c r="D60" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" t="s">
-        <v>140</v>
-      </c>
-      <c r="G60" t="s">
-        <v>126</v>
-      </c>
-      <c r="I60" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The curl is related to the line integral around a closed loop. ("circulation") is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K60" t="s">
-        <v>18</v>
-      </c>
-      <c r="L60" s="1" t="s">
+    </row>
+    <row r="61" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="33.950000000000003">
-      <c r="A61" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" t="s">
-        <v>176</v>
       </c>
       <c r="C61">
         <f>ROW()</f>
@@ -3475,28 +3469,27 @@
         <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G61" t="s">
-        <v>126</v>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for the curl is a (vector) function is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I61" t="s">
+        <v>136</v>
       </c>
       <c r="K61" t="s">
         <v>18</v>
       </c>
       <c r="L61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="33.950000000000003">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62">
         <f>ROW()</f>
@@ -3510,28 +3503,27 @@
         <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G62" t="s">
-        <v>126</v>
-      </c>
-      <c r="I62" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The curl is a local quantity is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I62" t="s">
+        <v>136</v>
       </c>
       <c r="K62" t="s">
         <v>18</v>
       </c>
       <c r="L62" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="33.950000000000003">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C63">
         <f>ROW()</f>
@@ -3545,28 +3537,27 @@
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G63" t="s">
-        <v>126</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The magnetic field is equal to the curl of the magnetic vector potential is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I63" t="s">
+        <v>136</v>
       </c>
       <c r="K63" t="s">
         <v>18</v>
       </c>
       <c r="L63" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="33.950000000000003">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C64">
         <f>ROW()</f>
@@ -3580,14 +3571,13 @@
         <v>14</v>
       </c>
       <c r="F64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G64" t="s">
-        <v>126</v>
-      </c>
-      <c r="I64" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The curl of the electric field is zero in electrostatics is not yet available--feel free to give us your suggestions on the poster!</v>
+        <v>125</v>
+      </c>
+      <c r="I64" t="s">
+        <v>136</v>
       </c>
       <c r="K64" t="s">
         <v>18</v>
@@ -3596,46 +3586,45 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="68.099999999999994">
+    <row r="65" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>12</v>
       </c>
       <c r="B65" t="s">
+        <v>179</v>
+      </c>
+      <c r="C65">
+        <f>ROW()</f>
+        <v>65</v>
+      </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" t="s">
         <v>180</v>
       </c>
-      <c r="C65">
-        <f>ROW()</f>
-        <v>65</v>
-      </c>
-      <c r="D65" t="s">
-        <v>14</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
+        <v>125</v>
+      </c>
+      <c r="I65" t="s">
+        <v>136</v>
+      </c>
+      <c r="K65" t="s">
+        <v>18</v>
+      </c>
+      <c r="L65" t="s">
         <v>181</v>
       </c>
-      <c r="G65" t="s">
-        <v>126</v>
-      </c>
-      <c r="I65" t="str">
-        <f t="shared" si="1"/>
-        <v>A long description for The divergence of the curl is equal to mu times the current in magneto-statics is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K65" t="s">
-        <v>18</v>
-      </c>
-      <c r="L65" t="s">
+    </row>
+    <row r="66" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="102">
-      <c r="A66" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" t="s">
-        <v>183</v>
       </c>
       <c r="C66">
         <f>ROW()</f>
@@ -3650,30 +3639,30 @@
         <v>[Differential form of $\vec r$ in spherical and cylindrical coordinates, The magnitude of $d\vec r$ is the length of a small step along a path, The direction of $d\vec r$ is tangent to a path]</v>
       </c>
       <c r="F66" t="s">
+        <v>183</v>
+      </c>
+      <c r="G66" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" t="s">
         <v>184</v>
       </c>
-      <c r="G66" t="s">
-        <v>126</v>
-      </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>185</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>186</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" t="s">
         <v>187</v>
-      </c>
-      <c r="K66" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="135.94999999999999">
-      <c r="A67" t="s">
-        <v>88</v>
-      </c>
-      <c r="B67" t="s">
-        <v>188</v>
       </c>
       <c r="C67">
         <f>ROW()</f>
@@ -3688,30 +3677,30 @@
         <v>[The gradient lives in the domain and has the same number of spatial dimensions as the original function, The gradient is a local quantity]</v>
       </c>
       <c r="F67" t="s">
+        <v>188</v>
+      </c>
+      <c r="G67" t="s">
+        <v>125</v>
+      </c>
+      <c r="H67" t="s">
         <v>189</v>
       </c>
-      <c r="G67" t="s">
-        <v>126</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>190</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>191</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
         <v>192</v>
-      </c>
-      <c r="K67" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="119.1">
-      <c r="A68" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68" t="s">
-        <v>193</v>
       </c>
       <c r="C68">
         <f>ROW()</f>
@@ -3726,30 +3715,30 @@
         <v>[The gradient lives in the domain and has the same number of spatial dimensions as the original function, The gradient is a local quantity]</v>
       </c>
       <c r="F68" t="s">
+        <v>193</v>
+      </c>
+      <c r="G68" t="s">
+        <v>125</v>
+      </c>
+      <c r="H68" t="s">
         <v>194</v>
       </c>
-      <c r="G68" t="s">
-        <v>126</v>
-      </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>195</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>196</v>
       </c>
-      <c r="J68" t="s">
+      <c r="K68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" t="s">
         <v>197</v>
-      </c>
-      <c r="K68" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="170.1">
-      <c r="A69" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" t="s">
-        <v>198</v>
       </c>
       <c r="C69">
         <f>ROW()</f>
@@ -3764,30 +3753,30 @@
         <v>[The divergence is related to the total flux through a closed surface, The divergence is a function, The divergence is a local quantity]</v>
       </c>
       <c r="F69" t="s">
+        <v>198</v>
+      </c>
+      <c r="G69" t="s">
+        <v>125</v>
+      </c>
+      <c r="H69" t="s">
         <v>199</v>
       </c>
-      <c r="G69" t="s">
-        <v>126</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>200</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
         <v>201</v>
       </c>
-      <c r="J69" t="s">
+      <c r="K69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" t="s">
         <v>202</v>
-      </c>
-      <c r="K69" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="170.1">
-      <c r="A70" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" t="s">
-        <v>203</v>
       </c>
       <c r="C70">
         <f>ROW()</f>
@@ -3802,30 +3791,30 @@
         <v>[The curl is related to the line integral around a closed loop. ("circulation"), the curl is a (vector) function, The curl is a local quantity]</v>
       </c>
       <c r="F70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H70" t="s">
+        <v>203</v>
+      </c>
+      <c r="I70" t="s">
         <v>204</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>205</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" t="s">
         <v>206</v>
-      </c>
-      <c r="K70" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="135.94999999999999">
-      <c r="A71" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" t="s">
-        <v>207</v>
       </c>
       <c r="C71">
         <f>ROW()</f>
@@ -3839,122 +3828,120 @@
         <v>14</v>
       </c>
       <c r="F71" t="s">
+        <v>207</v>
+      </c>
+      <c r="G71" t="s">
         <v>208</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>209</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>210</v>
       </c>
-      <c r="I71" t="s">
+      <c r="K71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
         <v>211</v>
       </c>
-      <c r="K71" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="31.5">
-      <c r="A72" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C72">
+        <f>ROW()</f>
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" t="s">
+        <v>207</v>
+      </c>
+      <c r="G72" t="s">
+        <v>208</v>
+      </c>
+      <c r="I72" t="s">
+        <v>263</v>
+      </c>
+      <c r="K72" t="s">
+        <v>18</v>
+      </c>
+      <c r="L72" t="s">
         <v>212</v>
       </c>
-      <c r="C72">
-        <f>ROW()</f>
-        <v>72</v>
-      </c>
-      <c r="D72" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" t="s">
+    </row>
+    <row r="73" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" t="s">
+        <v>213</v>
+      </c>
+      <c r="C73">
+        <f>ROW()</f>
+        <v>73</v>
+      </c>
+      <c r="D73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" t="s">
         <v>208</v>
       </c>
-      <c r="G72" t="s">
-        <v>209</v>
-      </c>
-      <c r="I72" t="str">
-        <f>"A long description for "&amp;B72 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME: Does the difference between zapping with d and taking the total differential need to be articulated?"</f>
-        <v>A long description for Equations can be 'zapped with d' to relate differentials is not yet available--feel free to give us your suggestions on the poster! FIXME: Does the difference between zapping with d and taking the total differential need to be articulated?</v>
-      </c>
-      <c r="K72" t="s">
-        <v>18</v>
-      </c>
-      <c r="L72" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="31.5">
-      <c r="A73" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="I73" t="s">
+        <v>264</v>
+      </c>
+      <c r="K73" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" t="s">
         <v>214</v>
       </c>
-      <c r="C73">
-        <f>ROW()</f>
-        <v>73</v>
-      </c>
-      <c r="D73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" t="s">
-        <v>14</v>
-      </c>
-      <c r="G73" t="s">
-        <v>209</v>
-      </c>
-      <c r="I73" t="str">
-        <f>"A long description for "&amp;B73 &amp;" is not yet available--feel free to give us your suggestions on the poster! FIXME what?"</f>
-        <v>A long description for Individual differentials can be manipulated algebraically is not yet available--feel free to give us your suggestions on the poster! FIXME what?</v>
-      </c>
-      <c r="K73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="48.95" customHeight="1">
-      <c r="A74" t="s">
-        <v>12</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C74">
+        <f>ROW()</f>
+        <v>74</v>
+      </c>
+      <c r="D74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" t="s">
+        <v>207</v>
+      </c>
+      <c r="G74" t="s">
+        <v>208</v>
+      </c>
+      <c r="I74" t="s">
         <v>215</v>
       </c>
-      <c r="C74">
-        <f>ROW()</f>
-        <v>74</v>
-      </c>
-      <c r="D74" t="s">
-        <v>14</v>
-      </c>
-      <c r="E74" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" t="s">
-        <v>208</v>
-      </c>
-      <c r="G74" t="s">
-        <v>209</v>
-      </c>
-      <c r="I74" t="s">
+      <c r="K74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
         <v>216</v>
-      </c>
-      <c r="K74" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="33.950000000000003">
-      <c r="A75" t="s">
-        <v>12</v>
-      </c>
-      <c r="B75" t="s">
-        <v>217</v>
       </c>
       <c r="C75">
         <f>ROW()</f>
@@ -3968,10 +3955,10 @@
         <v>14</v>
       </c>
       <c r="F75" t="s">
+        <v>207</v>
+      </c>
+      <c r="G75" t="s">
         <v>208</v>
-      </c>
-      <c r="G75" t="s">
-        <v>209</v>
       </c>
       <c r="I75" t="str">
         <f>"$df$ can be viewed as a small chunk of $f$. When combined with '" &amp;B4 &amp;"', it's easy to relate differentials to derivatives."</f>
@@ -3981,12 +3968,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="84.95">
+    <row r="76" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C76">
         <f>ROW()</f>
@@ -4000,57 +3987,57 @@
         <v>14</v>
       </c>
       <c r="F76" t="s">
+        <v>218</v>
+      </c>
+      <c r="G76" t="s">
+        <v>208</v>
+      </c>
+      <c r="I76" t="s">
         <v>219</v>
       </c>
-      <c r="G76" t="s">
-        <v>209</v>
-      </c>
-      <c r="I76" t="s">
+      <c r="K76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
         <v>220</v>
       </c>
-      <c r="K76" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="47.25">
-      <c r="A77" t="s">
-        <v>12</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C77">
+        <f>ROW()</f>
+        <v>77</v>
+      </c>
+      <c r="D77" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" t="s">
+        <v>208</v>
+      </c>
+      <c r="I77" t="s">
         <v>221</v>
       </c>
-      <c r="C77">
-        <f>ROW()</f>
-        <v>77</v>
-      </c>
-      <c r="D77" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" t="s">
-        <v>209</v>
-      </c>
-      <c r="I77" t="s">
+      <c r="K77" t="s">
+        <v>18</v>
+      </c>
+      <c r="L77" t="s">
         <v>222</v>
       </c>
-      <c r="K77" t="s">
-        <v>18</v>
-      </c>
-      <c r="L77" t="s">
+    </row>
+    <row r="78" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="102">
-      <c r="A78" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" t="s">
-        <v>224</v>
       </c>
       <c r="C78">
         <f>ROW()</f>
@@ -4067,25 +4054,24 @@
         <v>53</v>
       </c>
       <c r="G78" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H78" t="s">
+        <v>224</v>
+      </c>
+      <c r="I78" t="s">
+        <v>136</v>
+      </c>
+      <c r="K78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" t="s">
         <v>225</v>
-      </c>
-      <c r="I78" t="str">
-        <f t="shared" ref="I72:I79" si="2">"A long description for "&amp;B78 &amp;" is not yet available--feel free to give us your suggestions on the poster!"</f>
-        <v>A long description for Partial derivatives that do not have the same variable(s) held constant are not the same derivative is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K78" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="50.25" customHeight="1">
-      <c r="A79" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" t="s">
-        <v>226</v>
       </c>
       <c r="C79">
         <f>ROW()</f>
@@ -4102,25 +4088,24 @@
         <v>67</v>
       </c>
       <c r="G79" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H79" t="s">
+        <v>226</v>
+      </c>
+      <c r="I79" t="s">
+        <v>136</v>
+      </c>
+      <c r="K79" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" t="s">
         <v>227</v>
-      </c>
-      <c r="I79" t="str">
-        <f t="shared" si="2"/>
-        <v>A long description for Partial derivatives are coefficients in a differentials equation is not yet available--feel free to give us your suggestions on the poster!</v>
-      </c>
-      <c r="K79" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="84.95">
-      <c r="A80" t="s">
-        <v>12</v>
-      </c>
-      <c r="B80" t="s">
-        <v>228</v>
       </c>
       <c r="C80">
         <f>ROW()</f>
@@ -4134,54 +4119,54 @@
         <v>14</v>
       </c>
       <c r="F80" t="s">
+        <v>228</v>
+      </c>
+      <c r="G80" t="s">
+        <v>208</v>
+      </c>
+      <c r="I80" t="s">
         <v>229</v>
       </c>
-      <c r="G80" t="s">
-        <v>209</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="K80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" t="s">
         <v>230</v>
       </c>
-      <c r="K80" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="68.099999999999994">
-      <c r="A81" t="s">
-        <v>12</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C81">
+        <f>ROW()</f>
+        <v>81</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" t="s">
         <v>231</v>
       </c>
-      <c r="C81">
-        <f>ROW()</f>
-        <v>81</v>
-      </c>
-      <c r="D81" t="s">
-        <v>14</v>
-      </c>
-      <c r="E81" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
+        <v>208</v>
+      </c>
+      <c r="I81" t="s">
         <v>232</v>
       </c>
-      <c r="G81" t="s">
-        <v>209</v>
-      </c>
-      <c r="I81" t="s">
+      <c r="K81" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" t="s">
         <v>233</v>
-      </c>
-      <c r="K81" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="51">
-      <c r="A82" t="s">
-        <v>12</v>
-      </c>
-      <c r="B82" t="s">
-        <v>234</v>
       </c>
       <c r="C82">
         <f>ROW()</f>
@@ -4195,24 +4180,24 @@
         <v>14</v>
       </c>
       <c r="F82" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G82" t="s">
         <v>208</v>
       </c>
-      <c r="G82" t="s">
-        <v>209</v>
-      </c>
       <c r="I82" t="s">
+        <v>234</v>
+      </c>
+      <c r="K82" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="s">
         <v>235</v>
-      </c>
-      <c r="K82" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="119.1">
-      <c r="A83" t="s">
-        <v>88</v>
-      </c>
-      <c r="B83" t="s">
-        <v>236</v>
       </c>
       <c r="C83">
         <f>ROW()</f>
@@ -4227,30 +4212,30 @@
         <v>[Differentials are small changes or differences, Equations can be 'zapped with d' to relate differentials, Individual differentials can be manipulated algebraically, Total differentials are linear]</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" t="s">
         <v>208</v>
       </c>
-      <c r="G83" t="s">
-        <v>209</v>
-      </c>
       <c r="H83" t="s">
+        <v>236</v>
+      </c>
+      <c r="I83" t="s">
         <v>237</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>238</v>
       </c>
-      <c r="J83" t="s">
+      <c r="K83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="119" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
         <v>239</v>
-      </c>
-      <c r="K83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="119.1">
-      <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" t="s">
-        <v>240</v>
       </c>
       <c r="C84">
         <f>ROW()</f>
@@ -4265,30 +4250,30 @@
         <v>[Differentials are small chunks]</v>
       </c>
       <c r="F84" t="s">
+        <v>240</v>
+      </c>
+      <c r="G84" t="s">
+        <v>208</v>
+      </c>
+      <c r="H84" t="s">
         <v>241</v>
       </c>
-      <c r="G84" t="s">
-        <v>209</v>
-      </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>242</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>243</v>
       </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
         <v>244</v>
-      </c>
-      <c r="K84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="93" customHeight="1">
-      <c r="A85" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" t="s">
-        <v>245</v>
       </c>
       <c r="C85">
         <f>ROW()</f>
@@ -4303,30 +4288,30 @@
         <v>[There are experimental limits to how $small$ of a change can be measured, The derivative can be interpreted physically, Partial derivatives that do not have the same variable(s) held constant are not the same derivative, Partial derivatives are coefficients in a differentials equation]</v>
       </c>
       <c r="F85" t="s">
+        <v>245</v>
+      </c>
+      <c r="G85" t="s">
+        <v>208</v>
+      </c>
+      <c r="H85" t="s">
         <v>246</v>
       </c>
-      <c r="G85" t="s">
-        <v>209</v>
-      </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>247</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
         <v>248</v>
       </c>
-      <c r="J85" t="s">
+      <c r="K85" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
         <v>249</v>
-      </c>
-      <c r="K85" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="255">
-      <c r="A86" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" t="s">
-        <v>250</v>
       </c>
       <c r="C86">
         <f>ROW()</f>
@@ -4341,54 +4326,54 @@
         <v>[You can flip a partial derivative if the same variable(s) are constant, There might be experimental limits on which quantities you can measure, Differentials allow the finding of partial derivatives when a variable cannot be solved for]</v>
       </c>
       <c r="F86" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" t="s">
         <v>208</v>
       </c>
-      <c r="G86" t="s">
-        <v>209</v>
-      </c>
       <c r="H86" t="s">
+        <v>250</v>
+      </c>
+      <c r="I86" t="s">
+        <v>265</v>
+      </c>
+      <c r="J86" t="s">
         <v>251</v>
       </c>
-      <c r="I86" t="s">
+      <c r="K86" t="s">
+        <v>18</v>
+      </c>
+      <c r="L86" t="s">
         <v>252</v>
       </c>
-      <c r="J86" t="s">
+    </row>
+    <row r="87" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L87" t="s">
         <v>253</v>
       </c>
-      <c r="K86" t="s">
-        <v>18</v>
-      </c>
-      <c r="L86" t="s">
+    </row>
+    <row r="88" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L88" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L89" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L90" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="17.100000000000001">
-      <c r="L87" t="s">
+    <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L91" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="17.100000000000001">
-      <c r="L88" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="17.100000000000001">
-      <c r="L89" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="17.100000000000001">
-      <c r="L90" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="17.100000000000001">
-      <c r="L91" t="s">
-        <v>257</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I49:I1048576 I1:I47">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="A long description">
       <formula>NOT(ISERROR(SEARCH("A long description",I1)))</formula>
     </cfRule>
@@ -4443,19 +4428,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EFD8F-45BF-44EB-A2B4-FA9451BFAEEC}">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0" xr3:uid="{54CBAB97-8F37-53EE-95A6-74C785BB320D}">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="63.5" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="25.875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="92.875" customWidth="1"/>
-    <col min="5" max="5" width="28.375" customWidth="1"/>
+    <col min="2" max="3" width="25.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="92.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.95" customHeight="1">
+    <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="str">
         <f>SUBSTITUTE(_xlfn.CONCAT(Sheet1!F2:F102),"][",",")</f>
         <v>[$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,2D Graph, Contour Map,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$,surface, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$]</v>
@@ -4469,10 +4454,10 @@
         <v>$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,2D Graph, Contour Map,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$,surface, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.95" customHeight="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>MID(A1,2,LEN(A1)-2)</f>
         <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,,,,,,1D Graph,2D Graph, Contour Map,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$,surface, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,,,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,,$df$,$df$,$\Delta x$,$dx$,Experiment,,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
@@ -4490,7 +4475,7 @@
         <v>$\Delta x$</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1">
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2,",,,",","),",,,",","),",,",",")</f>
         <v>$\Delta x$,$\Delta x$,$\frac{\Delta f}{\Delta x}$,1D Graph,1D Graph,1D Graph,2D Graph, Contour Map,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\frac{d f}{d x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,2D Graph,2D Graph,Contour Maps,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,Contour Maps,2D Graph,$\frac{d f}{d x}$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\vec \nabla f$,$\vec \nabla f$,$\left(\frac{\partial f}{\partial x}\right)_y$,Contour Maps,$\frac{\partial f}{\partial x}$, Contour Maps, Inclinometer,$\frac{\partial f}{\partial x}$,$\frac{\partial f}{\partial x}$, Inclinometer,$\frac{\partial f}{\partial x}$,surface, Inclinometer,$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
@@ -4508,7 +4493,7 @@
         <v>$\frac{\Delta f}{\Delta x}$</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95" customHeight="1">
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:B65" si="1">IFERROR(LEFT(C3,FIND(",",C3)-1),C3)</f>
@@ -4523,7 +4508,7 @@
         <v>1D Graph</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" customHeight="1">
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4538,7 +4523,7 @@
         <v>2D Graph</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4553,7 +4538,7 @@
         <v>Contour Map</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4568,7 +4553,7 @@
         <v>$\frac{d f}{d x}$</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4583,7 +4568,7 @@
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4598,7 +4583,7 @@
         <v>Contour Maps</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4613,7 +4598,7 @@
         <v>$\frac{\partial f}{\partial x}$</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4628,7 +4613,7 @@
         <v>$\vec \nabla f$</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4643,7 +4628,7 @@
         <v>Inclinometer</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4658,7 +4643,7 @@
         <v>surface</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4673,7 +4658,7 @@
         <v>$d \vec r$</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4688,7 +4673,7 @@
         <v>$\vec \nabla \cdot \vec v$</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4703,7 +4688,7 @@
         <v>$\vec \nabla \times \vec v$</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4718,7 +4703,7 @@
         <v>$df$</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4733,7 +4718,7 @@
         <v>3D plots</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4748,7 +4733,7 @@
         <v>Kinesthetic</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4763,7 +4748,7 @@
         <v>Vector Field Map</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4778,7 +4763,7 @@
         <v>$dx$</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4793,7 +4778,7 @@
         <v>Experiment</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4808,7 +4793,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4823,7 +4808,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4838,7 +4823,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4853,7 +4838,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4868,7 +4853,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4883,7 +4868,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4898,7 +4883,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4913,7 +4898,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4928,7 +4913,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4943,7 +4928,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4958,7 +4943,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4973,7 +4958,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4988,7 +4973,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5003,7 +4988,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5018,7 +5003,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5033,7 +5018,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Inclinometer</v>
@@ -5043,7 +5028,7 @@
         <v>$\frac{\partial f}{\partial x}$, Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\frac{\partial f}{\partial x}$</v>
@@ -5053,7 +5038,7 @@
         <v>Inclinometer,$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Inclinometer</v>
@@ -5063,7 +5048,7 @@
         <v>$\vec \nabla f$,$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5073,7 +5058,7 @@
         <v>$\vec \nabla f$, surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5083,7 +5068,7 @@
         <v>surface, Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="str">
         <f t="shared" si="1"/>
         <v>surface</v>
@@ -5093,7 +5078,7 @@
         <v>Contour Maps,$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Contour Maps</v>
@@ -5103,7 +5088,7 @@
         <v>$d \vec r$,$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5113,7 +5098,7 @@
         <v>$d \vec r$,$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5123,7 +5108,7 @@
         <v>$d \vec r$,$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5133,7 +5118,7 @@
         <v>$\vec \nabla f$,$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5143,7 +5128,7 @@
         <v>$d \vec r$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5153,7 +5138,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5163,7 +5148,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5173,7 +5158,7 @@
         <v>$\vec \nabla \times \vec v$,$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="53" spans="2:3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5183,7 +5168,7 @@
         <v>$df$,$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$df$</v>
@@ -5193,7 +5178,7 @@
         <v>$\vec \nabla f$,$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="55" spans="2:3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5203,7 +5188,7 @@
         <v>$d \vec r$,Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="56" spans="2:3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5213,7 +5198,7 @@
         <v>Contour Maps, $\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="57" spans="2:3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Contour Maps</v>
@@ -5223,7 +5208,7 @@
         <v>$\vec \nabla f$,Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="58" spans="2:3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5233,7 +5218,7 @@
         <v>Contour Maps,$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="59" spans="2:3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Contour Maps</v>
@@ -5243,7 +5228,7 @@
         <v>$d \vec r$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="60" spans="2:3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$d \vec r$</v>
@@ -5253,7 +5238,7 @@
         <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="61" spans="2:3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5263,7 +5248,7 @@
         <v>$\vec \nabla f$,$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="62" spans="2:3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5273,7 +5258,7 @@
         <v>$\vec \nabla f$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="63" spans="2:3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla f$</v>
@@ -5283,7 +5268,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="64" spans="2:3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5293,7 +5278,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="65" spans="2:3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="str">
         <f t="shared" si="1"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5303,7 +5288,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="66" spans="2:3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="str">
         <f t="shared" ref="B66:B69" si="2">IFERROR(LEFT(C65,FIND(",",C65)-1),C65)</f>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5313,7 +5298,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="str">
         <f t="shared" si="2"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5323,7 +5308,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="str">
         <f t="shared" si="2"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5333,7 +5318,7 @@
         <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="str">
         <f t="shared" si="2"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5343,7 +5328,7 @@
         <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="str">
         <f t="shared" ref="B70:B93" si="4">IFERROR(LEFT(C69,FIND(",",C69)-1),C69)</f>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5353,7 +5338,7 @@
         <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="71" spans="2:3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5363,7 +5348,7 @@
         <v>$\vec \nabla \times \vec v$,$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5373,7 +5358,7 @@
         <v>$\vec \nabla \times \vec v$,$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5383,7 +5368,7 @@
         <v>$\vec \nabla \cdot \vec v$,$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla \cdot \vec v$</v>
@@ -5393,7 +5378,7 @@
         <v>$\vec \nabla \times \vec v$,$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="75" spans="2:3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla \times \vec v$</v>
@@ -5403,7 +5388,7 @@
         <v>$d \vec r$, 3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="76" spans="2:3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$d \vec r$</v>
@@ -5413,7 +5398,7 @@
         <v>3D plots,$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="77" spans="2:3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="str">
         <f t="shared" si="4"/>
         <v>3D plots</v>
@@ -5423,7 +5408,7 @@
         <v>$\vec \nabla f$, Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="78" spans="2:3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\vec \nabla f$</v>
@@ -5433,7 +5418,7 @@
         <v>Kinesthetic, Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="79" spans="2:3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Kinesthetic</v>
@@ -5443,7 +5428,7 @@
         <v>Contour Maps,Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Contour Maps</v>
@@ -5453,7 +5438,7 @@
         <v>Kinesthetic, Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B81" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Kinesthetic</v>
@@ -5463,7 +5448,7 @@
         <v>Vector Field Map, Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="82" spans="2:3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Vector Field Map</v>
@@ -5473,7 +5458,7 @@
         <v>Contour Maps,Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="83" spans="2:3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B83" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Contour Maps</v>
@@ -5483,7 +5468,7 @@
         <v>Vector Field Map,Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="84" spans="2:3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Vector Field Map</v>
@@ -5493,7 +5478,7 @@
         <v>Vector Field Map,$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="85" spans="2:3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Vector Field Map</v>
@@ -5503,7 +5488,7 @@
         <v>$df$,$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="86" spans="2:3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$df$</v>
@@ -5513,7 +5498,7 @@
         <v>$df$,$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$df$</v>
@@ -5523,7 +5508,7 @@
         <v>$df$,$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$df$</v>
@@ -5533,7 +5518,7 @@
         <v>$df$,$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="89" spans="2:3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$df$</v>
@@ -5543,7 +5528,7 @@
         <v>$\Delta x$,$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="90" spans="2:3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\Delta x$</v>
@@ -5553,7 +5538,7 @@
         <v>$dx$,Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="91" spans="2:3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$dx$</v>
@@ -5563,7 +5548,7 @@
         <v>Experiment,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Experiment</v>
@@ -5573,7 +5558,7 @@
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="str">
         <f t="shared" si="4"/>
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
@@ -5583,7 +5568,7 @@
         <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B94" s="4" t="str">
         <f>IFERROR(LEFT(C93,FIND(",",C93)-1),C93)</f>
         <v>$\frac{\partial f}{\partial x}$</v>
@@ -5593,7 +5578,7 @@
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="95" spans="2:3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="str">
         <f t="shared" ref="B95:B125" si="5">IFERROR(LEFT(C94,FIND(",",C94)-1),C94)</f>
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
@@ -5603,7 +5588,7 @@
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$,$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
@@ -5613,7 +5598,7 @@
         <v>$\frac{\partial f}{\partial x}$,Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$\frac{\partial f}{\partial x}$</v>
@@ -5623,7 +5608,7 @@
         <v>Experiment,$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Experiment</v>
@@ -5633,7 +5618,7 @@
         <v>$df$,$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="99" spans="2:3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$df$</v>
@@ -5643,7 +5628,7 @@
         <v>$df$,PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$df$</v>
@@ -5653,7 +5638,7 @@
         <v>PDM, $df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="101" spans="2:3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="str">
         <f t="shared" si="5"/>
         <v>PDM</v>
@@ -5663,7 +5648,7 @@
         <v>$df$,PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="102" spans="2:3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$df$</v>
@@ -5673,7 +5658,7 @@
         <v>PDM, $\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="str">
         <f t="shared" si="5"/>
         <v>PDM</v>
@@ -5683,7 +5668,7 @@
         <v>$\frac{\partial f}{\partial x}$,$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="104" spans="2:3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$\frac{\partial f}{\partial x}$</v>
@@ -5693,7 +5678,7 @@
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$,Table,$df$</v>
       </c>
     </row>
-    <row r="105" spans="2:3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$\left(\frac{\partial f}{\partial x}\right)_y$</v>
@@ -5703,7 +5688,7 @@
         <v>Table,$df$</v>
       </c>
     </row>
-    <row r="106" spans="2:3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Table</v>
@@ -5713,7 +5698,7 @@
         <v>$df$</v>
       </c>
     </row>
-    <row r="107" spans="2:3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B107" s="4" t="str">
         <f t="shared" si="5"/>
         <v>$df$</v>
@@ -5723,7 +5708,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="2:3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B108" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5733,7 +5718,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="2:3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5743,7 +5728,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="2:3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B110" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5753,7 +5738,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="2:3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B111" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5763,7 +5748,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="2:3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5773,7 +5758,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5783,7 +5768,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5793,7 +5778,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B115" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5803,7 +5788,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B116" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5813,7 +5798,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5823,7 +5808,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B118" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5833,7 +5818,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B119" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5843,7 +5828,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B120" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5853,7 +5838,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B121" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5863,7 +5848,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5873,7 +5858,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B123" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5883,7 +5868,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="2:3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B124" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5893,7 +5878,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="2:3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B125" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>

</xml_diff>